<commit_message>
add new sites to check
</commit_message>
<xml_diff>
--- a/pull-requests/filters.xlsx
+++ b/pull-requests/filters.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5214" uniqueCount="2306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5219" uniqueCount="2311">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -4913,6 +4913,9 @@
     <t xml:space="preserve">!!! easylist</t>
   </si>
   <si>
+    <t xml:space="preserve">DONE</t>
+  </si>
+  <si>
     <t xml:space="preserve">481</t>
   </si>
   <si>
@@ -5279,6 +5282,15 @@
     <t xml:space="preserve">http://www.racingforum.pl/</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.24gliwice.pl/wiadomosci/nie-umial-pogodzic-sie-z-odrzuceniem-uporczywie-nekal-wybranke-sms-ami-i-telefonami/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">todo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://radioq.fm</t>
+  </si>
+  <si>
     <t xml:space="preserve">1-2</t>
   </si>
   <si>
@@ -5517,6 +5529,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.polonia-peterborough.uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://2conv.com/pl53/terms/</t>
   </si>
   <si>
     <t xml:space="preserve">Domain</t>
@@ -6970,7 +6985,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -7062,11 +7077,27 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <strike val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Lato Medium"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lato Medium"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -7209,7 +7240,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7334,19 +7365,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7358,7 +7397,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7370,7 +7409,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7390,51 +7429,9 @@
     <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="3">
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF006600"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FFCC0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="0"/>
-        <i val="0"/>
-        <color rgb="FF996600"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+    <dxf/>
+    <dxf/>
+    <dxf/>
   </dxfs>
   <colors>
     <indexedColors>
@@ -7446,10 +7443,10 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF00599D"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -7477,7 +7474,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -7525,12 +7522,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M986"/>
+  <dimension ref="A1:M987"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A950" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B950" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A950" activeCellId="0" sqref="A950"/>
-      <selection pane="topRight" activeCell="B875" activeCellId="0" sqref="B875"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A893" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B893" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A893" activeCellId="0" sqref="A893"/>
+      <selection pane="topRight" activeCell="C906" activeCellId="0" sqref="C906"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27592,44 +27589,44 @@
         <v>212</v>
       </c>
     </row>
-    <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="816" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A816" s="1" t="s">
         <v>1619</v>
       </c>
       <c r="B816" s="30" t="s">
         <v>1620</v>
       </c>
-      <c r="C816" s="25" t="s">
+      <c r="C816" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="D816" s="31" t="s">
+      <c r="D816" s="32" t="s">
         <v>1621</v>
       </c>
-      <c r="E816" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="F816" s="32" t="s">
+      <c r="E816" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="F816" s="33" t="s">
         <v>1622</v>
       </c>
-      <c r="G816" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="H816" s="3" t="s">
-        <v>284</v>
+      <c r="G816" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="H816" s="34" t="s">
+        <v>1623</v>
       </c>
     </row>
     <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A817" s="11" t="s">
-        <v>1623</v>
+        <v>1624</v>
       </c>
       <c r="B817" s="12" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="C817" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D817" s="3" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="E817" s="12" t="s">
         <v>212</v>
@@ -27641,16 +27638,16 @@
     </row>
     <row r="818" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A818" s="1" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="B818" s="23" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="C818" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D818" s="8" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="E818" s="12" t="s">
         <v>212</v>
@@ -27662,16 +27659,16 @@
     </row>
     <row r="819" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A819" s="11" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
       <c r="B819" s="29" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="C819" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D819" s="12" t="s">
-        <v>1631</v>
+        <v>1632</v>
       </c>
       <c r="E819" s="12" t="s">
         <v>212</v>
@@ -27683,16 +27680,16 @@
     </row>
     <row r="820" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A820" s="1" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="B820" s="29" t="s">
-        <v>1633</v>
+        <v>1634</v>
       </c>
       <c r="C820" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D820" s="8" t="s">
-        <v>1634</v>
+        <v>1635</v>
       </c>
       <c r="E820" s="12" t="s">
         <v>212</v>
@@ -27705,7 +27702,7 @@
     <row r="821" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A821" s="11"/>
       <c r="B821" s="29" t="s">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="C821" s="12" t="s">
         <v>32</v>
@@ -27721,7 +27718,7 @@
     </row>
     <row r="822" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B822" s="29" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="C822" s="12" t="s">
         <v>14</v>
@@ -27737,16 +27734,16 @@
     </row>
     <row r="823" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A823" s="11" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
       <c r="B823" s="29" t="s">
-        <v>1638</v>
+        <v>1639</v>
       </c>
       <c r="C823" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D823" s="12" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
       <c r="E823" s="12" t="s">
         <v>212</v>
@@ -27758,7 +27755,7 @@
     </row>
     <row r="824" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B824" s="29" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="C824" s="12" t="s">
         <v>32</v>
@@ -27775,7 +27772,7 @@
     <row r="825" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A825" s="11"/>
       <c r="B825" s="12" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="C825" s="12" t="s">
         <v>32</v>
@@ -27791,10 +27788,10 @@
     </row>
     <row r="826" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A826" s="1" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="B826" s="23" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="C826" s="12" t="s">
         <v>14</v>
@@ -27812,16 +27809,16 @@
     </row>
     <row r="827" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A827" s="11" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="B827" s="12" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="C827" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D827" s="12" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="E827" s="12" t="s">
         <v>212</v>
@@ -27833,16 +27830,16 @@
     </row>
     <row r="828" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A828" s="1" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="B828" s="23" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="C828" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D828" s="8" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="E828" s="12" t="s">
         <v>212</v>
@@ -27855,7 +27852,7 @@
     <row r="829" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A829" s="11"/>
       <c r="B829" s="12" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="C829" s="12" t="s">
         <v>32</v>
@@ -27871,16 +27868,16 @@
     </row>
     <row r="830" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A830" s="1" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="B830" s="23" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="C830" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D830" s="29" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="E830" s="12" t="s">
         <v>212</v>
@@ -27892,16 +27889,16 @@
     </row>
     <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A831" s="11" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="B831" s="12" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="C831" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D831" s="3" t="s">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="E831" s="12" t="s">
         <v>212</v>
@@ -27913,7 +27910,7 @@
     </row>
     <row r="832" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B832" s="23" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="C832" s="12" t="s">
         <v>32</v>
@@ -27930,7 +27927,7 @@
     <row r="833" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A833" s="11"/>
       <c r="B833" s="12" t="s">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="C833" s="12" t="s">
         <v>14</v>
@@ -27946,16 +27943,16 @@
     </row>
     <row r="834" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A834" s="1" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="B834" s="23" t="s">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="C834" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D834" s="29" t="s">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="E834" s="12" t="s">
         <v>212</v>
@@ -27968,7 +27965,7 @@
     <row r="835" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A835" s="11"/>
       <c r="B835" s="12" t="s">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="C835" s="12" t="s">
         <v>14</v>
@@ -27984,16 +27981,16 @@
     </row>
     <row r="836" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A836" s="1" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="B836" s="29" t="s">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="C836" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D836" s="29" t="s">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="E836" s="12" t="s">
         <v>212</v>
@@ -28005,16 +28002,16 @@
     </row>
     <row r="837" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A837" s="11" t="s">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="B837" s="29" t="s">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="C837" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D837" s="29" t="s">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="E837" s="12" t="s">
         <v>212</v>
@@ -28026,16 +28023,16 @@
     </row>
     <row r="838" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A838" s="1" t="s">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="B838" s="23" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="C838" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D838" s="3" t="s">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="E838" s="12" t="s">
         <v>212</v>
@@ -28048,7 +28045,7 @@
     <row r="839" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A839" s="11"/>
       <c r="B839" s="12" t="s">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="C839" s="12" t="s">
         <v>14</v>
@@ -28064,7 +28061,7 @@
     </row>
     <row r="840" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B840" s="23" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="C840" s="12" t="s">
         <v>14</v>
@@ -28080,16 +28077,16 @@
     </row>
     <row r="841" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A841" s="11" t="s">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="B841" s="12" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="C841" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D841" s="29" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="E841" s="12" t="s">
         <v>212</v>
@@ -28101,7 +28098,7 @@
     </row>
     <row r="842" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B842" s="23" t="s">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="C842" s="12" t="s">
         <v>32</v>
@@ -28118,7 +28115,7 @@
     <row r="843" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A843" s="11"/>
       <c r="B843" s="12" t="s">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="C843" s="12" t="s">
         <v>14</v>
@@ -28134,16 +28131,16 @@
     </row>
     <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A844" s="1" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="B844" s="23" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="C844" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D844" s="3" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="E844" s="12" t="s">
         <v>212</v>
@@ -28156,7 +28153,7 @@
     <row r="845" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A845" s="11"/>
       <c r="B845" s="12" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="C845" s="12" t="s">
         <v>14</v>
@@ -28172,16 +28169,16 @@
     </row>
     <row r="846" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A846" s="1" t="s">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="B846" s="23" t="s">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="C846" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D846" s="29" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="E846" s="12" t="s">
         <v>212</v>
@@ -28193,16 +28190,16 @@
     </row>
     <row r="847" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A847" s="11" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="B847" s="29" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="C847" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D847" s="29" t="s">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="E847" s="12" t="s">
         <v>212</v>
@@ -28214,16 +28211,16 @@
     </row>
     <row r="848" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A848" s="1" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="B848" s="29" t="s">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="C848" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D848" s="3" t="s">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="E848" s="12" t="s">
         <v>212</v>
@@ -28235,16 +28232,16 @@
     </row>
     <row r="849" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A849" s="11" t="s">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="B849" s="12" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="C849" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D849" s="3" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="E849" s="12" t="s">
         <v>212</v>
@@ -28256,7 +28253,7 @@
     </row>
     <row r="850" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B850" s="23" t="s">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="C850" s="12" t="s">
         <v>14</v>
@@ -28272,16 +28269,16 @@
     </row>
     <row r="851" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A851" s="11" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="B851" s="12" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="C851" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D851" s="29" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="E851" s="12" t="s">
         <v>212</v>
@@ -28293,7 +28290,7 @@
     </row>
     <row r="852" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B852" s="23" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="C852" s="12" t="s">
         <v>14</v>
@@ -28309,16 +28306,16 @@
     </row>
     <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A853" s="11" t="s">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="B853" s="29" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="C853" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D853" s="8" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="E853" s="12" t="s">
         <v>212</v>
@@ -28330,16 +28327,16 @@
     </row>
     <row r="854" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A854" s="1" t="s">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="B854" s="29" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="C854" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D854" s="29" t="s">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="E854" s="12" t="s">
         <v>212</v>
@@ -28351,16 +28348,16 @@
     </row>
     <row r="855" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A855" s="11" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
       <c r="B855" s="12" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="C855" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D855" s="29" t="s">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="E855" s="12" t="s">
         <v>212</v>
@@ -28372,16 +28369,16 @@
     </row>
     <row r="856" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A856" s="1" t="s">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="B856" s="29" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="C856" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D856" s="3" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="E856" s="12" t="s">
         <v>212</v>
@@ -28393,16 +28390,16 @@
     </row>
     <row r="857" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A857" s="11" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="B857" s="12" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="C857" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D857" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="E857" s="12" t="s">
         <v>212</v>
@@ -28414,16 +28411,16 @@
     </row>
     <row r="858" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A858" s="1" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="B858" s="23" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="C858" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D858" s="29" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="E858" s="12" t="s">
         <v>212</v>
@@ -28435,16 +28432,16 @@
     </row>
     <row r="859" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A859" s="11" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="B859" s="29" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="C859" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D859" s="29" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="E859" s="12" t="s">
         <v>212</v>
@@ -28456,16 +28453,16 @@
     </row>
     <row r="860" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A860" s="1" t="s">
-        <v>1721</v>
+        <v>1722</v>
       </c>
       <c r="B860" s="29" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="C860" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D860" s="29" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="E860" s="12" t="s">
         <v>212</v>
@@ -28477,16 +28474,16 @@
     </row>
     <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A861" s="11" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="B861" s="29" t="s">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="C861" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D861" s="8" t="s">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="E861" s="12" t="s">
         <v>212</v>
@@ -28498,16 +28495,16 @@
     </row>
     <row r="862" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A862" s="1" t="s">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="B862" s="23" t="s">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="C862" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D862" s="29" t="s">
-        <v>1729</v>
+        <v>1730</v>
       </c>
       <c r="E862" s="12" t="s">
         <v>212</v>
@@ -28520,7 +28517,7 @@
     <row r="863" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A863" s="11"/>
       <c r="B863" s="12" t="s">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="C863" s="12" t="s">
         <v>14</v>
@@ -28536,16 +28533,16 @@
     </row>
     <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A864" s="1" t="s">
-        <v>1731</v>
+        <v>1732</v>
       </c>
       <c r="B864" s="23" t="s">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="C864" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D864" s="12" t="s">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="E864" s="12" t="s">
         <v>212</v>
@@ -28558,7 +28555,7 @@
     <row r="865" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A865" s="11"/>
       <c r="B865" s="12" t="s">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="C865" s="12" t="s">
         <v>32</v>
@@ -28574,7 +28571,7 @@
     </row>
     <row r="866" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B866" s="23" t="s">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="C866" s="12" t="s">
         <v>14</v>
@@ -28588,41 +28585,45 @@
         <v>212</v>
       </c>
     </row>
-    <row r="867" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="867" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A867" s="11" t="s">
-        <v>1736</v>
-      </c>
-      <c r="B867" s="29" t="s">
         <v>1737</v>
       </c>
-      <c r="C867" s="12" t="s">
+      <c r="B867" s="30" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C867" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="D867" s="8" t="s">
-        <v>1738</v>
-      </c>
-      <c r="E867" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="F867" s="33" t="s">
+      <c r="D867" s="32" t="s">
+        <v>1739</v>
+      </c>
+      <c r="E867" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="F867" s="35" t="s">
         <v>1622</v>
       </c>
-      <c r="G867" s="12" t="s">
-        <v>212</v>
-      </c>
+      <c r="G867" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="H867" s="34" t="s">
+        <v>1623</v>
+      </c>
+      <c r="I867" s="34"/>
     </row>
     <row r="868" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A868" s="1" t="s">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="B868" s="29" t="s">
-        <v>1740</v>
+        <v>1741</v>
       </c>
       <c r="C868" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D868" s="29" t="s">
-        <v>1741</v>
+        <v>1742</v>
       </c>
       <c r="E868" s="12" t="s">
         <v>212</v>
@@ -28634,16 +28635,16 @@
     </row>
     <row r="869" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A869" s="11" t="s">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="B869" s="29" t="s">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="C869" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D869" s="29" t="s">
-        <v>1744</v>
+        <v>1745</v>
       </c>
       <c r="E869" s="12" t="s">
         <v>212</v>
@@ -29107,15 +29108,28 @@
         <v>1</v>
       </c>
       <c r="F901" s="3" t="s">
-        <v>1744</v>
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="902" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F902" s="3" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="906" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D906" s="3" t="s">
+        <v>1747</v>
+      </c>
+      <c r="F906" s="3" t="s">
+        <v>1748</v>
       </c>
     </row>
     <row r="907" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D907" s="3" t="s">
-        <v>1745</v>
+        <v>1749</v>
       </c>
       <c r="F907" s="3" t="s">
-        <v>1746</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="908" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29123,15 +29137,15 @@
         <v>1</v>
       </c>
       <c r="F908" s="3" t="s">
-        <v>1747</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="909" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D909" s="3" t="s">
-        <v>1748</v>
+        <v>1752</v>
       </c>
       <c r="F909" s="3" t="s">
-        <v>1749</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="911" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29139,10 +29153,10 @@
     </row>
     <row r="912" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D912" s="3" t="s">
-        <v>1750</v>
+        <v>1754</v>
       </c>
       <c r="F912" s="3" t="s">
-        <v>1751</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="913" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29150,7 +29164,7 @@
         <v>1</v>
       </c>
       <c r="F913" s="3" t="s">
-        <v>1752</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="914" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29175,13 +29189,13 @@
     </row>
     <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D918" s="12" t="s">
-        <v>1753</v>
+        <v>1757</v>
       </c>
       <c r="E918" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F918" s="12" t="s">
-        <v>1754</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29192,7 +29206,7 @@
         <v>212</v>
       </c>
       <c r="F919" s="8" t="s">
-        <v>1755</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29203,7 +29217,7 @@
         <v>212</v>
       </c>
       <c r="F920" s="12" t="s">
-        <v>1756</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29212,7 +29226,7 @@
         <v>212</v>
       </c>
       <c r="F921" s="12" t="s">
-        <v>1757</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29221,7 +29235,7 @@
         <v>212</v>
       </c>
       <c r="F922" s="8" t="s">
-        <v>1758</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="923" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29237,7 +29251,7 @@
         <v>212</v>
       </c>
       <c r="F924" s="8" t="s">
-        <v>1759</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29248,40 +29262,40 @@
         <v>212</v>
       </c>
       <c r="F925" s="12" t="s">
-        <v>1760</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D926" s="8" t="s">
-        <v>1761</v>
+        <v>1765</v>
       </c>
       <c r="E926" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F926" s="8" t="s">
-        <v>1762</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D927" s="12" t="s">
-        <v>1761</v>
+        <v>1765</v>
       </c>
       <c r="E927" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F927" s="12" t="s">
-        <v>1763</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D928" s="8" t="s">
-        <v>1764</v>
+        <v>1768</v>
       </c>
       <c r="E928" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F928" s="8" t="s">
-        <v>1765</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="929" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29304,29 +29318,29 @@
         <v>212</v>
       </c>
       <c r="F931" s="12" t="s">
-        <v>1766</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D932" s="8" t="s">
-        <v>1767</v>
+        <v>1771</v>
       </c>
       <c r="E932" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F932" s="8" t="s">
-        <v>1768</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D933" s="12" t="s">
-        <v>1769</v>
+        <v>1773</v>
       </c>
       <c r="E933" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F933" s="29" t="s">
-        <v>1770</v>
+        <v>1774</v>
       </c>
     </row>
     <row r="934" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29342,7 +29356,7 @@
         <v>212</v>
       </c>
       <c r="F935" s="12" t="s">
-        <v>1771</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29353,7 +29367,7 @@
         <v>212</v>
       </c>
       <c r="F936" s="8" t="s">
-        <v>1772</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29365,24 +29379,24 @@
     </row>
     <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D938" s="8" t="s">
-        <v>1773</v>
+        <v>1777</v>
       </c>
       <c r="E938" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F938" s="8" t="s">
-        <v>1774</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D939" s="12" t="s">
-        <v>1775</v>
+        <v>1779</v>
       </c>
       <c r="E939" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F939" s="12" t="s">
-        <v>1776</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29400,7 +29414,7 @@
         <v>212</v>
       </c>
       <c r="F941" s="12" t="s">
-        <v>1777</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29411,7 +29425,7 @@
         <v>212</v>
       </c>
       <c r="F942" s="8" t="s">
-        <v>1778</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29422,7 +29436,7 @@
         <v>212</v>
       </c>
       <c r="F943" s="12" t="s">
-        <v>1779</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29440,7 +29454,7 @@
         <v>212</v>
       </c>
       <c r="F945" s="12" t="s">
-        <v>1780</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="946" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29450,13 +29464,13 @@
     </row>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D947" s="12" t="s">
-        <v>1781</v>
+        <v>1785</v>
       </c>
       <c r="E947" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F947" s="12" t="s">
-        <v>1741</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29474,7 +29488,7 @@
         <v>212</v>
       </c>
       <c r="F949" s="12" t="s">
-        <v>1782</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29485,7 +29499,7 @@
         <v>212</v>
       </c>
       <c r="F950" s="8" t="s">
-        <v>1783</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29496,7 +29510,7 @@
         <v>212</v>
       </c>
       <c r="F951" s="12" t="s">
-        <v>1784</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29514,34 +29528,34 @@
         <v>212</v>
       </c>
       <c r="F953" s="12" t="s">
-        <v>1785</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D954" s="8" t="s">
-        <v>1786</v>
+        <v>1790</v>
       </c>
       <c r="E954" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F954" s="29" t="s">
-        <v>1787</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="955" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D955" s="3" t="s">
-        <v>1788</v>
+        <v>1792</v>
       </c>
       <c r="F955" s="3" t="s">
-        <v>1789</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="956" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D956" s="3" t="s">
-        <v>1790</v>
+        <v>1794</v>
       </c>
       <c r="F956" s="3" t="s">
-        <v>1791</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="957" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29549,7 +29563,7 @@
         <v>2</v>
       </c>
       <c r="F957" s="3" t="s">
-        <v>1792</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="958" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29557,23 +29571,23 @@
         <v>1</v>
       </c>
       <c r="F958" s="3" t="s">
-        <v>1793</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="960" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D960" s="3" t="s">
-        <v>1794</v>
+        <v>1798</v>
       </c>
       <c r="F960" s="3" t="s">
-        <v>1795</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="961" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D961" s="3" t="s">
-        <v>1796</v>
+        <v>1800</v>
       </c>
       <c r="F961" s="3" t="s">
-        <v>1797</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="962" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29581,7 +29595,7 @@
         <v>1</v>
       </c>
       <c r="F962" s="3" t="s">
-        <v>1798</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="964" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29589,12 +29603,12 @@
         <v>1</v>
       </c>
       <c r="F964" s="3" t="s">
-        <v>1799</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="965" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F965" s="29" t="s">
-        <v>1800</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="966" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29602,7 +29616,7 @@
         <v>1</v>
       </c>
       <c r="F966" s="3" t="s">
-        <v>1801</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="967" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29610,52 +29624,52 @@
         <v>2</v>
       </c>
       <c r="F967" s="3" t="s">
-        <v>1802</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="968" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F968" s="29" t="s">
-        <v>1803</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="969" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D969" s="3" t="s">
-        <v>1804</v>
+        <v>1808</v>
       </c>
       <c r="F969" s="3" t="s">
-        <v>1805</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="970" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D970" s="3" t="s">
-        <v>1806</v>
+        <v>1810</v>
       </c>
       <c r="F970" s="3" t="s">
-        <v>1807</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="971" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D971" s="3" t="s">
-        <v>1806</v>
+        <v>1810</v>
       </c>
       <c r="F971" s="3" t="s">
-        <v>1808</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="972" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D972" s="3" t="s">
-        <v>1806</v>
+        <v>1810</v>
       </c>
       <c r="F972" s="3" t="s">
-        <v>1809</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="974" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D974" s="3" t="s">
-        <v>1745</v>
+        <v>1749</v>
       </c>
       <c r="F974" s="3" t="s">
-        <v>1810</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="975" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29666,55 +29680,55 @@
         <v>1</v>
       </c>
       <c r="F976" s="3" t="s">
-        <v>1811</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="977" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D977" s="3" t="s">
-        <v>1812</v>
+        <v>1816</v>
       </c>
       <c r="F977" s="3" t="s">
-        <v>1813</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="978" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D978" s="3" t="s">
-        <v>1814</v>
+        <v>1818</v>
       </c>
       <c r="F978" s="3" t="s">
-        <v>1815</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="979" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D979" s="3" t="s">
-        <v>1804</v>
+        <v>1808</v>
       </c>
       <c r="F979" s="3" t="s">
-        <v>1816</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="981" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D981" s="3" t="s">
-        <v>1817</v>
+        <v>1821</v>
       </c>
       <c r="F981" s="3" t="s">
-        <v>1818</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="982" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D982" s="3" t="s">
-        <v>1819</v>
+        <v>1823</v>
       </c>
       <c r="F982" s="3" t="s">
-        <v>1820</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="983" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D983" s="3" t="s">
-        <v>1804</v>
+        <v>1808</v>
       </c>
       <c r="F983" s="3" t="s">
-        <v>1821</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="984" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29722,23 +29736,28 @@
         <v>1</v>
       </c>
       <c r="F984" s="3" t="s">
-        <v>1822</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="985" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D985" s="3" t="s">
-        <v>1745</v>
+        <v>1749</v>
       </c>
       <c r="F985" s="3" t="s">
-        <v>1823</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="986" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D986" s="3" t="s">
-        <v>1804</v>
+        <v>1808</v>
       </c>
       <c r="F986" s="3" t="s">
-        <v>1824</v>
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="987" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F987" s="3" t="s">
+        <v>1829</v>
       </c>
     </row>
   </sheetData>
@@ -30716,1362 +30735,1362 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>1825</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>1826</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>1827</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>1828</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>1829</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>1830</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>1831</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>1832</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>1833</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>1834</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>1835</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>1836</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>1837</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>1838</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>1839</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>1840</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>1829</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>1841</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>1842</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>1843</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="s">
-        <v>1844</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>1845</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="s">
-        <v>1846</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="s">
-        <v>1847</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="s">
-        <v>1848</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="s">
-        <v>1849</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="22" t="s">
-        <v>1850</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="22" t="s">
-        <v>1851</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="22" t="s">
-        <v>1852</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>1853</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="22" t="s">
-        <v>1854</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="22" t="s">
-        <v>1855</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>1856</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="22" t="s">
-        <v>1857</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="22" t="s">
-        <v>1858</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="22" t="s">
-        <v>1859</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="22" t="s">
-        <v>1860</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="22" t="s">
-        <v>1861</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="22" t="s">
-        <v>1862</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>1863</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>1864</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="22" t="s">
-        <v>1865</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="22" t="s">
-        <v>1866</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>1867</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="22" t="s">
-        <v>1868</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="22" t="s">
-        <v>1869</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>1870</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>1871</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="22" t="s">
-        <v>1872</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>1873</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="22" t="s">
-        <v>1874</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="22" t="s">
-        <v>1875</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="22" t="s">
-        <v>1876</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="22" t="s">
-        <v>1877</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>1878</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="22" t="s">
-        <v>1879</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="22" t="s">
-        <v>1880</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22" t="s">
-        <v>1881</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="22" t="s">
-        <v>1882</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="22" t="s">
-        <v>1883</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="22" t="s">
-        <v>1884</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="22" t="s">
-        <v>1885</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="22" t="s">
-        <v>1886</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="22" t="s">
-        <v>1887</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="22" t="s">
-        <v>1888</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="22" t="s">
-        <v>1889</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="22" t="s">
-        <v>1890</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="22" t="s">
-        <v>1891</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="22" t="s">
-        <v>1892</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="22" t="s">
-        <v>1893</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="22" t="s">
-        <v>1894</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="22" t="s">
-        <v>1895</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="22" t="s">
-        <v>1896</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="22" t="s">
-        <v>1897</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="22" t="s">
-        <v>1898</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="22" t="s">
-        <v>1899</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="22" t="s">
-        <v>1900</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="22" t="s">
-        <v>1901</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="22" t="s">
-        <v>1902</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="22" t="s">
-        <v>1903</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="22" t="s">
-        <v>1904</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="22" t="s">
-        <v>1905</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="22" t="s">
-        <v>1906</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="22" t="s">
-        <v>1907</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="22" t="s">
-        <v>1908</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="22" t="s">
-        <v>1909</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="22" t="s">
-        <v>1910</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="22" t="s">
-        <v>1911</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="22" t="s">
-        <v>1912</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="22" t="s">
-        <v>1831</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="22" t="s">
-        <v>1913</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="22" t="s">
-        <v>1914</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="22" t="s">
-        <v>1915</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="22" t="s">
-        <v>1838</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="22" t="s">
-        <v>1916</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="22" t="s">
-        <v>1917</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="22" t="s">
-        <v>1918</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="22" t="s">
-        <v>1919</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="22" t="s">
-        <v>1920</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="22" t="s">
-        <v>1921</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="22" t="s">
-        <v>1922</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="22" t="s">
-        <v>1923</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="22" t="s">
-        <v>1924</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="22" t="s">
-        <v>1925</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="22" t="s">
-        <v>1926</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="22" t="s">
-        <v>1927</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="22" t="s">
-        <v>1928</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="22" t="s">
-        <v>1929</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="22" t="s">
-        <v>1930</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="22" t="s">
-        <v>1931</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="22" t="s">
-        <v>1932</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="22" t="s">
-        <v>1933</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="22" t="s">
-        <v>1934</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="22" t="s">
-        <v>1935</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="22" t="s">
-        <v>1936</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="22" t="s">
-        <v>1937</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="22" t="s">
-        <v>1938</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="22" t="s">
-        <v>1939</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="22" t="s">
-        <v>1940</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="22" t="s">
-        <v>1941</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="22" t="s">
-        <v>1942</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="22" t="s">
-        <v>1943</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="22" t="s">
-        <v>1944</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="22" t="s">
-        <v>1945</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="22" t="s">
-        <v>1946</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="22" t="s">
-        <v>1947</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="22" t="s">
-        <v>1948</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="22" t="s">
-        <v>1949</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="22" t="s">
-        <v>1950</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="22" t="s">
-        <v>1951</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="22" t="s">
-        <v>1952</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="22" t="s">
-        <v>1953</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="22" t="s">
-        <v>1954</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="22" t="s">
-        <v>1955</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="22" t="s">
-        <v>1956</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="22" t="s">
-        <v>1957</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="22" t="s">
-        <v>1958</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="22" t="s">
-        <v>1959</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="22" t="s">
-        <v>1960</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="22" t="s">
-        <v>1961</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="22" t="s">
-        <v>1962</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="22" t="s">
-        <v>1963</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="22" t="s">
-        <v>1964</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="22" t="s">
-        <v>1965</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="22" t="s">
-        <v>1966</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="22" t="s">
-        <v>1967</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="22" t="s">
-        <v>1968</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="22" t="s">
-        <v>1969</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="22" t="s">
-        <v>1970</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="22" t="s">
-        <v>1971</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="22" t="s">
-        <v>1972</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="22" t="s">
-        <v>1973</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="22" t="s">
-        <v>1974</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="22" t="s">
-        <v>1975</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="22" t="s">
-        <v>1976</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="22" t="s">
-        <v>1977</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="22" t="s">
-        <v>1978</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="22" t="s">
-        <v>1979</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="22" t="s">
-        <v>1980</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="22" t="s">
-        <v>1981</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="22" t="s">
-        <v>1982</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="22" t="s">
-        <v>1983</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="22" t="s">
-        <v>1984</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="22" t="s">
-        <v>1985</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="22" t="s">
-        <v>1986</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="22" t="s">
-        <v>1987</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="22" t="s">
-        <v>1988</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="22" t="s">
-        <v>1989</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="22" t="s">
-        <v>1990</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="22" t="s">
-        <v>1991</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="22" t="s">
-        <v>1992</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="22" t="s">
-        <v>1993</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="22" t="s">
-        <v>1994</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="22" t="s">
-        <v>1995</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="22" t="s">
-        <v>1996</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="22" t="s">
-        <v>1997</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="22" t="s">
-        <v>1998</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="22" t="s">
-        <v>1999</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="22" t="s">
-        <v>2000</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="22" t="s">
-        <v>2001</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="22" t="s">
-        <v>2002</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="22" t="s">
-        <v>2003</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="22" t="s">
-        <v>2004</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="22" t="s">
-        <v>2005</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="22" t="s">
-        <v>2006</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="22" t="s">
-        <v>2007</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="22" t="s">
-        <v>2008</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="22" t="s">
-        <v>2009</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="22" t="s">
-        <v>2010</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="22" t="s">
-        <v>2011</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="22" t="s">
-        <v>2012</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="22" t="s">
-        <v>2013</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="22" t="s">
-        <v>2014</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="22" t="s">
-        <v>2015</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="22" t="s">
-        <v>2016</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="22" t="s">
-        <v>2017</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="22" t="s">
-        <v>2018</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="22" t="s">
-        <v>1826</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="22" t="s">
-        <v>2019</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="22" t="s">
-        <v>2020</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="22" t="s">
-        <v>2021</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="22" t="s">
-        <v>2022</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="22" t="s">
-        <v>2023</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="22" t="s">
-        <v>2024</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="22" t="s">
-        <v>2025</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="22" t="s">
-        <v>2026</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="22" t="s">
-        <v>2027</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="22" t="s">
-        <v>2028</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="22" t="s">
-        <v>2029</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="22" t="s">
-        <v>2030</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="22" t="s">
-        <v>2031</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="22" t="s">
-        <v>2032</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="22" t="s">
-        <v>2033</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="22" t="s">
-        <v>2034</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="22" t="s">
-        <v>2035</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="22" t="s">
-        <v>2036</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="22" t="s">
-        <v>2037</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="22" t="s">
-        <v>2038</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="22" t="s">
-        <v>2039</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="22" t="s">
-        <v>2040</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="22" t="s">
-        <v>2041</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="22" t="s">
-        <v>2042</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="22" t="s">
-        <v>2043</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="22" t="s">
-        <v>2044</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="22" t="s">
-        <v>2045</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="22" t="s">
-        <v>2046</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="22" t="s">
-        <v>2047</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="22" t="s">
-        <v>2048</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="22" t="s">
-        <v>2049</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="22" t="s">
-        <v>2050</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="22" t="s">
-        <v>2051</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="22" t="s">
-        <v>2052</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="22" t="s">
-        <v>2053</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="22" t="s">
-        <v>2054</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="22" t="s">
-        <v>2055</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="22" t="s">
-        <v>2056</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="22" t="s">
-        <v>2057</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="22" t="s">
-        <v>2058</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="22" t="s">
-        <v>2059</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="22" t="s">
-        <v>2060</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="22" t="s">
-        <v>2061</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="22" t="s">
-        <v>2062</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="22" t="s">
-        <v>2063</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="22" t="s">
-        <v>1836</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="22" t="s">
-        <v>2064</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="22" t="s">
-        <v>2065</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="22" t="s">
-        <v>2066</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="22" t="s">
-        <v>2067</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="22" t="s">
-        <v>2068</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="22" t="s">
-        <v>2069</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="22" t="s">
-        <v>2070</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="22" t="s">
-        <v>2071</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="22" t="s">
-        <v>2072</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="22" t="s">
-        <v>2073</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="22" t="s">
-        <v>2074</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="22" t="s">
-        <v>2075</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="22" t="s">
-        <v>2076</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="22" t="s">
-        <v>2077</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="22" t="s">
-        <v>2078</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="22" t="s">
-        <v>2079</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="22" t="s">
-        <v>2080</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="22" t="s">
-        <v>2081</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="22" t="s">
-        <v>2082</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="22" t="s">
-        <v>2083</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="22" t="s">
-        <v>2084</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="22" t="s">
-        <v>2085</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="22" t="s">
-        <v>2086</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="22" t="s">
-        <v>2087</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="22" t="s">
-        <v>1843</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="22" t="s">
-        <v>2088</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="22" t="s">
-        <v>2089</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="22" t="s">
-        <v>2090</v>
+        <v>2095</v>
       </c>
     </row>
   </sheetData>
@@ -32105,160 +32124,160 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="34" t="s">
-        <v>2091</v>
+      <c r="B1" s="36" t="s">
+        <v>2096</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="35" t="s">
-        <v>2092</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>2093</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>2094</v>
-      </c>
-      <c r="I2" s="38"/>
+      <c r="B2" s="37" t="s">
+        <v>2097</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>2098</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>2099</v>
+      </c>
+      <c r="I2" s="40"/>
       <c r="K2" s="22" t="s">
-        <v>2095</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="35" t="s">
-        <v>2096</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>2093</v>
-      </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="37" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>2098</v>
+      </c>
+      <c r="H3" s="38"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="12" t="s">
-        <v>2097</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="22" t="s">
-        <v>2098</v>
-      </c>
-      <c r="C4" s="40"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="36"/>
+        <v>2103</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="12" t="s">
-        <v>2099</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="40"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="36"/>
+      <c r="C5" s="42"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="38"/>
       <c r="K5" s="8" t="s">
-        <v>2100</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="40"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="36"/>
+      <c r="C6" s="42"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="38"/>
       <c r="K6" s="12" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="29"/>
-      <c r="C7" s="40"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="36"/>
+      <c r="C7" s="42"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="38"/>
       <c r="K7" s="29" t="s">
-        <v>2101</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="12" t="s">
-        <v>2102</v>
-      </c>
-      <c r="C8" s="40"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="36"/>
+        <v>2107</v>
+      </c>
+      <c r="C8" s="42"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="38"/>
       <c r="K8" s="22" t="s">
-        <v>2103</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="29" t="s">
-        <v>2104</v>
-      </c>
-      <c r="C9" s="40"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="36"/>
+        <v>2109</v>
+      </c>
+      <c r="C9" s="42"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="38"/>
       <c r="K9" s="8" t="s">
-        <v>2105</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="8" t="s">
-        <v>2106</v>
-      </c>
-      <c r="C10" s="40"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="36"/>
+        <v>2111</v>
+      </c>
+      <c r="C10" s="42"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="38"/>
       <c r="K10" s="12" t="s">
-        <v>2107</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="12" t="s">
-        <v>2108</v>
-      </c>
-      <c r="C11" s="40"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="36"/>
+        <v>2113</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="38"/>
       <c r="K11" s="8" t="s">
-        <v>2109</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="8" t="s">
-        <v>2110</v>
+        <v>2115</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>2111</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0"/>
       <c r="K13" s="8" t="s">
-        <v>2112</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>2113</v>
+        <v>2118</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>2114</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>2115</v>
+        <v>2120</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>2116</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K16" s="12" t="s">
-        <v>2117</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32266,10 +32285,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="22" t="s">
-        <v>2118</v>
+        <v>2123</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>2119</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32277,109 +32296,109 @@
         <v>119</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>2120</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>2121</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>2122</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="22" t="s">
-        <v>2123</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>2124</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>2125</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>2126</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>2127</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>2128</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>2129</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>2130</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="22" t="s">
-        <v>2131</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>2132</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="22" t="s">
-        <v>2133</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>2134</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>2135</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="22" t="s">
-        <v>2136</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="22" t="s">
-        <v>2137</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>2138</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>2139</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="22" t="s">
-        <v>2140</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32389,47 +32408,47 @@
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="22" t="s">
-        <v>2141</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="22" t="s">
-        <v>2142</v>
+        <v>2147</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>2143</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>2144</v>
+        <v>2149</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>2145</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>2146</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>2147</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="22" t="s">
-        <v>2148</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="22" t="s">
-        <v>2149</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32437,17 +32456,17 @@
         <v>193</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>1761</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="22" t="s">
-        <v>2150</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="22" t="s">
-        <v>2151</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32457,32 +32476,32 @@
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="22" t="s">
-        <v>2152</v>
+        <v>2157</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="22" t="s">
-        <v>2153</v>
+        <v>2158</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="22" t="s">
-        <v>2154</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="22" t="s">
-        <v>2155</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="22" t="s">
-        <v>2156</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="8" t="s">
-        <v>2157</v>
+        <v>2162</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>212</v>
@@ -32493,7 +32512,7 @@
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="8" t="s">
-        <v>2158</v>
+        <v>2163</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>212</v>
@@ -32504,13 +32523,13 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="8" t="s">
-        <v>2159</v>
+        <v>2164</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>212</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>2160</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32529,12 +32548,12 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>2161</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="3" t="s">
-        <v>2162</v>
+        <v>2167</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="n">
@@ -32543,7 +32562,7 @@
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="8" t="s">
-        <v>2163</v>
+        <v>2168</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>212</v>
@@ -32554,7 +32573,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="3" t="s">
-        <v>2164</v>
+        <v>2169</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="n">
@@ -32563,7 +32582,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="3" t="s">
-        <v>2165</v>
+        <v>2170</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
@@ -32577,7 +32596,7 @@
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="8" t="s">
-        <v>2166</v>
+        <v>2171</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>212</v>
@@ -32586,7 +32605,7 @@
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="12" t="s">
-        <v>2167</v>
+        <v>2172</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>212</v>
@@ -32597,7 +32616,7 @@
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>2168</v>
+        <v>2173</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>212</v>
@@ -32615,7 +32634,7 @@
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="8" t="s">
-        <v>2169</v>
+        <v>2174</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>212</v>
@@ -32626,7 +32645,7 @@
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>2170</v>
+        <v>2175</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>212</v>
@@ -32637,7 +32656,7 @@
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="12" t="s">
-        <v>2171</v>
+        <v>2176</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>212</v>
@@ -32648,18 +32667,18 @@
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="12" t="s">
-        <v>2172</v>
+        <v>2177</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>212</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>2173</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
-        <v>2174</v>
+        <v>2179</v>
       </c>
       <c r="C91" s="12" t="s">
         <v>212</v>
@@ -32670,7 +32689,7 @@
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="8" t="s">
-        <v>2175</v>
+        <v>2180</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>212</v>
@@ -32681,18 +32700,18 @@
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="12" t="s">
-        <v>2176</v>
+        <v>2181</v>
       </c>
       <c r="C93" s="12" t="s">
         <v>212</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>2177</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="8" t="s">
-        <v>2178</v>
+        <v>2183</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>212</v>
@@ -32703,7 +32722,7 @@
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="12" t="s">
-        <v>2179</v>
+        <v>2184</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>212</v>
@@ -32714,7 +32733,7 @@
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="12" t="s">
-        <v>2180</v>
+        <v>2185</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>212</v>
@@ -32725,7 +32744,7 @@
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="8" t="s">
-        <v>2181</v>
+        <v>2186</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>212</v>
@@ -32736,7 +32755,7 @@
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="12" t="s">
-        <v>2100</v>
+        <v>2105</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>212</v>
@@ -32747,7 +32766,7 @@
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="8" t="s">
-        <v>2182</v>
+        <v>2187</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>212</v>
@@ -32758,7 +32777,7 @@
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="12" t="s">
-        <v>2183</v>
+        <v>2188</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>212</v>
@@ -32769,7 +32788,7 @@
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>2184</v>
+        <v>2189</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>212</v>
@@ -32780,7 +32799,7 @@
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>2185</v>
+        <v>2190</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>212</v>
@@ -32791,16 +32810,16 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="3" t="s">
-        <v>2186</v>
+        <v>2191</v>
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3" t="s">
-        <v>2187</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
-        <v>2188</v>
+        <v>2193</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>212</v>
@@ -32811,18 +32830,18 @@
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="12" t="s">
-        <v>2189</v>
+        <v>2194</v>
       </c>
       <c r="C105" s="12" t="s">
         <v>212</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>2190</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="8" t="s">
-        <v>2191</v>
+        <v>2196</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>212</v>
@@ -32833,7 +32852,7 @@
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="12" t="s">
-        <v>2192</v>
+        <v>2197</v>
       </c>
       <c r="C107" s="12" t="s">
         <v>212</v>
@@ -32844,7 +32863,7 @@
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="8" t="s">
-        <v>2193</v>
+        <v>2198</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>212</v>
@@ -32855,7 +32874,7 @@
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="12" t="s">
-        <v>2194</v>
+        <v>2199</v>
       </c>
       <c r="C109" s="12" t="s">
         <v>212</v>
@@ -32876,7 +32895,7 @@
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="8" t="s">
-        <v>2195</v>
+        <v>2200</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>212</v>
@@ -32887,7 +32906,7 @@
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="12" t="s">
-        <v>2196</v>
+        <v>2201</v>
       </c>
       <c r="C113" s="12" t="s">
         <v>212</v>
@@ -32903,7 +32922,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
-        <v>2197</v>
+        <v>2202</v>
       </c>
       <c r="C115" s="0"/>
       <c r="D115" s="0" t="s">
@@ -32912,16 +32931,16 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="0" t="s">
-        <v>2198</v>
+        <v>2203</v>
       </c>
       <c r="C116" s="0"/>
       <c r="D116" s="0" t="s">
-        <v>2199</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="0" t="s">
-        <v>2200</v>
+        <v>2205</v>
       </c>
       <c r="C117" s="0"/>
       <c r="D117" s="0" t="s">
@@ -32935,7 +32954,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="0" t="s">
-        <v>2201</v>
+        <v>2206</v>
       </c>
       <c r="C119" s="0"/>
       <c r="D119" s="0" t="n">
@@ -32958,7 +32977,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
-        <v>2202</v>
+        <v>2207</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="3" t="s">
@@ -32967,27 +32986,27 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>2203</v>
+        <v>2208</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
-        <v>2199</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="8" t="s">
-        <v>2204</v>
+        <v>2209</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>212</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>2205</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="12" t="s">
-        <v>2206</v>
+        <v>2211</v>
       </c>
       <c r="C125" s="12" t="s">
         <v>212</v>
@@ -32998,7 +33017,7 @@
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="12" t="s">
-        <v>2207</v>
+        <v>2212</v>
       </c>
       <c r="C126" s="12" t="s">
         <v>212</v>
@@ -33009,7 +33028,7 @@
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="8" t="s">
-        <v>2208</v>
+        <v>2213</v>
       </c>
       <c r="C127" s="8" t="s">
         <v>212</v>
@@ -33020,7 +33039,7 @@
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="12" t="s">
-        <v>2209</v>
+        <v>2214</v>
       </c>
       <c r="C128" s="12" t="s">
         <v>212</v>
@@ -33031,7 +33050,7 @@
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="12" t="s">
-        <v>2210</v>
+        <v>2215</v>
       </c>
       <c r="C129" s="12" t="s">
         <v>212</v>
@@ -33049,7 +33068,7 @@
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="12" t="s">
-        <v>2211</v>
+        <v>2216</v>
       </c>
       <c r="C131" s="12" t="s">
         <v>212</v>
@@ -33391,472 +33410,472 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="22" t="s">
-        <v>2212</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="22" t="s">
-        <v>2213</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="22" t="s">
-        <v>2214</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="22" t="s">
-        <v>2215</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>2216</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>2217</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>2218</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="22" t="s">
-        <v>2219</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="22" t="s">
-        <v>2220</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="22" t="s">
-        <v>2221</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="22" t="s">
-        <v>2222</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="22" t="s">
-        <v>2223</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="22" t="s">
-        <v>2224</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="22" t="s">
-        <v>2225</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="22" t="s">
-        <v>2226</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="22" t="s">
-        <v>2227</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="22" t="s">
-        <v>2228</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="22" t="s">
-        <v>2229</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="22" t="s">
-        <v>2230</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="22" t="s">
-        <v>2231</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="22" t="s">
-        <v>2232</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="22" t="s">
-        <v>2233</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="22" t="s">
-        <v>2234</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="22" t="s">
-        <v>2235</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="22" t="s">
-        <v>2236</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="22" t="s">
-        <v>2237</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="22" t="s">
-        <v>2238</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="22" t="s">
-        <v>2239</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="22" t="s">
-        <v>2240</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="22" t="s">
-        <v>2241</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="22" t="s">
-        <v>2242</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="22" t="s">
-        <v>2243</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="22" t="s">
-        <v>2244</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="22" t="s">
-        <v>2245</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="22" t="s">
-        <v>2246</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="22" t="s">
-        <v>2247</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="22" t="s">
-        <v>2248</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="22" t="s">
-        <v>2249</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="22" t="s">
-        <v>2250</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="22" t="s">
-        <v>2251</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="22" t="s">
-        <v>2252</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="22" t="s">
-        <v>2253</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="22" t="s">
-        <v>2254</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="22" t="s">
-        <v>2255</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="22" t="s">
-        <v>2256</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="22" t="s">
-        <v>2257</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="22" t="s">
-        <v>2258</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="22" t="s">
-        <v>2259</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="22" t="s">
-        <v>2260</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="22" t="s">
-        <v>2261</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="22" t="s">
-        <v>2262</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="22" t="s">
-        <v>2263</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="22" t="s">
-        <v>2264</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="22" t="s">
-        <v>2265</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="22" t="s">
-        <v>2266</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="22" t="s">
-        <v>2267</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="22" t="s">
-        <v>2268</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="22" t="s">
-        <v>2269</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="22" t="s">
-        <v>2270</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="22" t="s">
-        <v>2271</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="22" t="s">
-        <v>2272</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="22" t="s">
-        <v>2273</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="22" t="s">
-        <v>2274</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="22" t="s">
-        <v>2275</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="22" t="s">
-        <v>2276</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="22" t="s">
-        <v>2277</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="22" t="s">
-        <v>2278</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="22" t="s">
-        <v>2279</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="22" t="s">
-        <v>2280</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="22" t="s">
-        <v>2281</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="22" t="s">
-        <v>2282</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="22" t="s">
-        <v>2283</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="22" t="s">
-        <v>2284</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="22" t="s">
-        <v>2285</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="22" t="s">
-        <v>2286</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="22" t="s">
-        <v>2287</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="22" t="s">
-        <v>2288</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="22" t="s">
-        <v>2289</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="22" t="s">
-        <v>2290</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="22" t="s">
-        <v>2291</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="22" t="s">
-        <v>2292</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="22" t="s">
-        <v>2293</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="22" t="s">
-        <v>2294</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="22" t="s">
-        <v>2295</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="22" t="s">
-        <v>2296</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="22" t="s">
-        <v>2297</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="22" t="s">
-        <v>2298</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="22" t="s">
-        <v>2299</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="22" t="s">
-        <v>2300</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="22" t="s">
-        <v>2301</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="22" t="s">
-        <v>2302</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="22" t="s">
-        <v>2303</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="22" t="s">
-        <v>2304</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="22" t="s">
-        <v>2305</v>
+        <v>2310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new websites to check
</commit_message>
<xml_diff>
--- a/pull-requests/filters.xlsx
+++ b/pull-requests/filters.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5219" uniqueCount="2311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5224" uniqueCount="2316">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -5532,6 +5532,21 @@
   </si>
   <si>
     <t xml:space="preserve">https://2conv.com/pl53/terms/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.warzywapolowe.pl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gloto-single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://petronews.pl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">banners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://kierowcyhgv.uk</t>
   </si>
   <si>
     <t xml:space="preserve">Domain</t>
@@ -7522,12 +7537,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M987"/>
+  <dimension ref="A1:M990"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A893" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B893" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A893" activeCellId="0" sqref="A893"/>
-      <selection pane="topRight" activeCell="C906" activeCellId="0" sqref="C906"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A962" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B962" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A962" activeCellId="0" sqref="A962"/>
+      <selection pane="topRight" activeCell="D991" activeCellId="0" sqref="D991"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29758,6 +29773,27 @@
     <row r="987" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F987" s="3" t="s">
         <v>1829</v>
+      </c>
+    </row>
+    <row r="988" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F988" s="3" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="989" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D989" s="3" t="s">
+        <v>1831</v>
+      </c>
+      <c r="F989" s="3" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="990" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D990" s="3" t="s">
+        <v>1833</v>
+      </c>
+      <c r="F990" s="3" t="s">
+        <v>1834</v>
       </c>
     </row>
   </sheetData>
@@ -30735,1362 +30771,1362 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>1830</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>1831</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>1832</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>1833</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>1834</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>1835</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>1836</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>1837</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>1838</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>1839</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>1840</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>1841</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>1842</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>1843</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>1844</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>1845</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>1834</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>1846</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>1847</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>1848</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="s">
-        <v>1849</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>1850</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="s">
-        <v>1851</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="s">
-        <v>1852</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="s">
-        <v>1853</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="s">
-        <v>1854</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="22" t="s">
-        <v>1855</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="22" t="s">
-        <v>1856</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="22" t="s">
-        <v>1857</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>1858</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="22" t="s">
-        <v>1859</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="22" t="s">
-        <v>1860</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>1861</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="22" t="s">
-        <v>1862</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="22" t="s">
-        <v>1863</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="22" t="s">
-        <v>1864</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="22" t="s">
-        <v>1865</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="22" t="s">
-        <v>1866</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="22" t="s">
-        <v>1867</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>1868</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>1869</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="22" t="s">
-        <v>1870</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="22" t="s">
-        <v>1871</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>1872</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="22" t="s">
-        <v>1873</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="22" t="s">
-        <v>1874</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>1875</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>1876</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="22" t="s">
-        <v>1877</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>1878</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="22" t="s">
-        <v>1879</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="22" t="s">
-        <v>1880</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="22" t="s">
-        <v>1881</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="22" t="s">
-        <v>1882</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>1883</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="22" t="s">
-        <v>1884</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="22" t="s">
-        <v>1885</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22" t="s">
-        <v>1886</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="22" t="s">
-        <v>1887</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="22" t="s">
-        <v>1888</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="22" t="s">
-        <v>1889</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="22" t="s">
-        <v>1890</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="22" t="s">
-        <v>1891</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="22" t="s">
-        <v>1892</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="22" t="s">
-        <v>1893</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="22" t="s">
-        <v>1894</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="22" t="s">
-        <v>1895</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="22" t="s">
-        <v>1896</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="22" t="s">
-        <v>1897</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="22" t="s">
-        <v>1898</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="22" t="s">
-        <v>1899</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="22" t="s">
-        <v>1900</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="22" t="s">
-        <v>1901</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="22" t="s">
-        <v>1902</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="22" t="s">
-        <v>1903</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="22" t="s">
-        <v>1904</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="22" t="s">
-        <v>1905</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="22" t="s">
-        <v>1906</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="22" t="s">
-        <v>1907</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="22" t="s">
-        <v>1908</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="22" t="s">
-        <v>1909</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="22" t="s">
-        <v>1910</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="22" t="s">
-        <v>1911</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="22" t="s">
-        <v>1912</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="22" t="s">
-        <v>1913</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="22" t="s">
-        <v>1914</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="22" t="s">
-        <v>1915</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="22" t="s">
-        <v>1916</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="22" t="s">
-        <v>1917</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="22" t="s">
-        <v>1836</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="22" t="s">
-        <v>1918</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="22" t="s">
-        <v>1919</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="22" t="s">
-        <v>1920</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="22" t="s">
-        <v>1843</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="22" t="s">
-        <v>1921</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="22" t="s">
-        <v>1922</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="22" t="s">
-        <v>1923</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="22" t="s">
-        <v>1924</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="22" t="s">
-        <v>1925</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="22" t="s">
-        <v>1926</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="22" t="s">
-        <v>1927</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="22" t="s">
-        <v>1928</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="22" t="s">
-        <v>1929</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="22" t="s">
-        <v>1930</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="22" t="s">
-        <v>1931</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="22" t="s">
-        <v>1932</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="22" t="s">
-        <v>1933</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="22" t="s">
-        <v>1934</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="22" t="s">
-        <v>1935</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="22" t="s">
-        <v>1936</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="22" t="s">
-        <v>1937</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="22" t="s">
-        <v>1938</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="22" t="s">
-        <v>1939</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="22" t="s">
-        <v>1940</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="22" t="s">
-        <v>1941</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="22" t="s">
-        <v>1942</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="22" t="s">
-        <v>1943</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="22" t="s">
-        <v>1944</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="22" t="s">
-        <v>1945</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="22" t="s">
-        <v>1946</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="22" t="s">
-        <v>1947</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="22" t="s">
-        <v>1948</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="22" t="s">
-        <v>1949</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="22" t="s">
-        <v>1950</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="22" t="s">
-        <v>1951</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="22" t="s">
-        <v>1952</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="22" t="s">
-        <v>1953</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="22" t="s">
-        <v>1954</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="22" t="s">
-        <v>1955</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="22" t="s">
-        <v>1956</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="22" t="s">
-        <v>1957</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="22" t="s">
-        <v>1958</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="22" t="s">
-        <v>1959</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="22" t="s">
-        <v>1960</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="22" t="s">
-        <v>1961</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="22" t="s">
-        <v>1962</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="22" t="s">
-        <v>1963</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="22" t="s">
-        <v>1964</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="22" t="s">
-        <v>1965</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="22" t="s">
-        <v>1966</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="22" t="s">
-        <v>1967</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="22" t="s">
-        <v>1968</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="22" t="s">
-        <v>1969</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="22" t="s">
-        <v>1970</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="22" t="s">
-        <v>1971</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="22" t="s">
-        <v>1972</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="22" t="s">
-        <v>1973</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="22" t="s">
-        <v>1974</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="22" t="s">
-        <v>1975</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="22" t="s">
-        <v>1976</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="22" t="s">
-        <v>1977</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="22" t="s">
-        <v>1978</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="22" t="s">
-        <v>1979</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="22" t="s">
-        <v>1980</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="22" t="s">
-        <v>1981</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="22" t="s">
-        <v>1982</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="22" t="s">
-        <v>1983</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="22" t="s">
-        <v>1984</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="22" t="s">
-        <v>1985</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="22" t="s">
-        <v>1986</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="22" t="s">
-        <v>1987</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="22" t="s">
-        <v>1988</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="22" t="s">
-        <v>1989</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="22" t="s">
-        <v>1990</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="22" t="s">
-        <v>1991</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="22" t="s">
-        <v>1992</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="22" t="s">
-        <v>1993</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="22" t="s">
-        <v>1994</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="22" t="s">
-        <v>1995</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="22" t="s">
-        <v>1996</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="22" t="s">
-        <v>1997</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="22" t="s">
-        <v>1998</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="22" t="s">
-        <v>1999</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="22" t="s">
-        <v>2000</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="22" t="s">
-        <v>2001</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="22" t="s">
-        <v>2002</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="22" t="s">
-        <v>2003</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="22" t="s">
-        <v>2004</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="22" t="s">
-        <v>2005</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="22" t="s">
-        <v>2006</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="22" t="s">
-        <v>2007</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="22" t="s">
-        <v>2008</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="22" t="s">
-        <v>2009</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="22" t="s">
-        <v>2010</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="22" t="s">
-        <v>2011</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="22" t="s">
-        <v>2012</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="22" t="s">
-        <v>2013</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="22" t="s">
-        <v>2014</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="22" t="s">
-        <v>2015</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="22" t="s">
-        <v>2016</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="22" t="s">
-        <v>2017</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="22" t="s">
-        <v>2018</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="22" t="s">
-        <v>2019</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="22" t="s">
-        <v>2020</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="22" t="s">
-        <v>2021</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="22" t="s">
-        <v>2022</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="22" t="s">
-        <v>2023</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="22" t="s">
-        <v>1831</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="22" t="s">
-        <v>2024</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="22" t="s">
-        <v>2025</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="22" t="s">
-        <v>2026</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="22" t="s">
-        <v>2027</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="22" t="s">
-        <v>2028</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="22" t="s">
-        <v>2029</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="22" t="s">
-        <v>2030</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="22" t="s">
-        <v>2031</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="22" t="s">
-        <v>2032</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="22" t="s">
-        <v>2033</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="22" t="s">
-        <v>2034</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="22" t="s">
-        <v>2035</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="22" t="s">
-        <v>2036</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="22" t="s">
-        <v>2037</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="22" t="s">
-        <v>2038</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="22" t="s">
-        <v>2039</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="22" t="s">
-        <v>2040</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="22" t="s">
-        <v>2041</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="22" t="s">
-        <v>2042</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="22" t="s">
-        <v>2043</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="22" t="s">
-        <v>2044</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="22" t="s">
-        <v>2045</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="22" t="s">
-        <v>2046</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="22" t="s">
-        <v>2047</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="22" t="s">
-        <v>2048</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="22" t="s">
-        <v>2049</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="22" t="s">
-        <v>2050</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="22" t="s">
-        <v>2051</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="22" t="s">
-        <v>2052</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="22" t="s">
-        <v>2053</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="22" t="s">
-        <v>2054</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="22" t="s">
-        <v>2055</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="22" t="s">
-        <v>2056</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="22" t="s">
-        <v>2057</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="22" t="s">
-        <v>2058</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="22" t="s">
-        <v>2059</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="22" t="s">
-        <v>2060</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="22" t="s">
-        <v>2061</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="22" t="s">
-        <v>2062</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="22" t="s">
-        <v>2063</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="22" t="s">
-        <v>2064</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="22" t="s">
-        <v>2065</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="22" t="s">
-        <v>2066</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="22" t="s">
-        <v>2067</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="22" t="s">
-        <v>2068</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="22" t="s">
-        <v>1841</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="22" t="s">
-        <v>2069</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="22" t="s">
-        <v>2070</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="22" t="s">
-        <v>2071</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="22" t="s">
-        <v>2072</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="22" t="s">
-        <v>2073</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="22" t="s">
-        <v>2074</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="22" t="s">
-        <v>2075</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="22" t="s">
-        <v>2076</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="22" t="s">
-        <v>2077</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="22" t="s">
-        <v>2078</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="22" t="s">
-        <v>2079</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="22" t="s">
-        <v>2080</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="22" t="s">
-        <v>2081</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="22" t="s">
-        <v>2082</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="22" t="s">
-        <v>2083</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="22" t="s">
-        <v>2084</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="22" t="s">
-        <v>2085</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="22" t="s">
-        <v>2086</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="22" t="s">
-        <v>2087</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="22" t="s">
-        <v>2088</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="22" t="s">
-        <v>2089</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="22" t="s">
-        <v>2090</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="22" t="s">
-        <v>2091</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="22" t="s">
-        <v>2092</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="22" t="s">
-        <v>1848</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="22" t="s">
-        <v>2093</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="22" t="s">
-        <v>2094</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="22" t="s">
-        <v>2095</v>
+        <v>2100</v>
       </c>
     </row>
   </sheetData>
@@ -32125,48 +32161,48 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="36" t="s">
-        <v>2096</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="37" t="s">
-        <v>2097</v>
+        <v>2102</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>2098</v>
+        <v>2103</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>2099</v>
+        <v>2104</v>
       </c>
       <c r="I2" s="40"/>
       <c r="K2" s="22" t="s">
-        <v>2100</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="37" t="s">
-        <v>2101</v>
+        <v>2106</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>2098</v>
+        <v>2103</v>
       </c>
       <c r="H3" s="38"/>
       <c r="I3" s="41"/>
       <c r="J3" s="38"/>
       <c r="K3" s="12" t="s">
-        <v>2102</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="22" t="s">
-        <v>2103</v>
+        <v>2108</v>
       </c>
       <c r="C4" s="42"/>
       <c r="H4" s="38"/>
       <c r="I4" s="41"/>
       <c r="J4" s="38"/>
       <c r="K4" s="12" t="s">
-        <v>2104</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32175,7 +32211,7 @@
       <c r="I5" s="41"/>
       <c r="J5" s="38"/>
       <c r="K5" s="8" t="s">
-        <v>2105</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32194,90 +32230,90 @@
       <c r="I7" s="41"/>
       <c r="J7" s="38"/>
       <c r="K7" s="29" t="s">
-        <v>2106</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="12" t="s">
-        <v>2107</v>
+        <v>2112</v>
       </c>
       <c r="C8" s="42"/>
       <c r="H8" s="38"/>
       <c r="I8" s="41"/>
       <c r="J8" s="38"/>
       <c r="K8" s="22" t="s">
-        <v>2108</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="29" t="s">
-        <v>2109</v>
+        <v>2114</v>
       </c>
       <c r="C9" s="42"/>
       <c r="H9" s="38"/>
       <c r="I9" s="41"/>
       <c r="J9" s="38"/>
       <c r="K9" s="8" t="s">
-        <v>2110</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="8" t="s">
-        <v>2111</v>
+        <v>2116</v>
       </c>
       <c r="C10" s="42"/>
       <c r="H10" s="38"/>
       <c r="I10" s="41"/>
       <c r="J10" s="38"/>
       <c r="K10" s="12" t="s">
-        <v>2112</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="12" t="s">
-        <v>2113</v>
+        <v>2118</v>
       </c>
       <c r="C11" s="42"/>
       <c r="H11" s="38"/>
       <c r="I11" s="41"/>
       <c r="J11" s="38"/>
       <c r="K11" s="8" t="s">
-        <v>2114</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="8" t="s">
-        <v>2115</v>
+        <v>2120</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>2116</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0"/>
       <c r="K13" s="8" t="s">
-        <v>2117</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>2118</v>
+        <v>2123</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>2119</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>2120</v>
+        <v>2125</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>2121</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K16" s="12" t="s">
-        <v>2122</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32285,10 +32321,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="22" t="s">
-        <v>2123</v>
+        <v>2128</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>2124</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32296,109 +32332,109 @@
         <v>119</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>2125</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>2126</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>2127</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="22" t="s">
-        <v>2128</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>2129</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>2130</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>2131</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>2132</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>2133</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>2134</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>2135</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="22" t="s">
-        <v>2136</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>2137</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="22" t="s">
-        <v>2138</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>2139</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>2140</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="22" t="s">
-        <v>2141</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="22" t="s">
-        <v>2142</v>
+        <v>2147</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>2143</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>2144</v>
+        <v>2149</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="22" t="s">
-        <v>2145</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32408,47 +32444,47 @@
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="22" t="s">
-        <v>2146</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="22" t="s">
-        <v>2147</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>2148</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>2149</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>2150</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>2151</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>2152</v>
+        <v>2157</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="22" t="s">
-        <v>2153</v>
+        <v>2158</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="22" t="s">
-        <v>2154</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32461,12 +32497,12 @@
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="22" t="s">
-        <v>2155</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="22" t="s">
-        <v>2156</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32476,32 +32512,32 @@
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="22" t="s">
-        <v>2157</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="22" t="s">
-        <v>2158</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="22" t="s">
-        <v>2159</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="22" t="s">
-        <v>2160</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="22" t="s">
-        <v>2161</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="8" t="s">
-        <v>2162</v>
+        <v>2167</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>212</v>
@@ -32512,7 +32548,7 @@
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="8" t="s">
-        <v>2163</v>
+        <v>2168</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>212</v>
@@ -32523,13 +32559,13 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="8" t="s">
-        <v>2164</v>
+        <v>2169</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>212</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>2165</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32548,12 +32584,12 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>2166</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="3" t="s">
-        <v>2167</v>
+        <v>2172</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="n">
@@ -32562,7 +32598,7 @@
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="8" t="s">
-        <v>2168</v>
+        <v>2173</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>212</v>
@@ -32573,7 +32609,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="3" t="s">
-        <v>2169</v>
+        <v>2174</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="n">
@@ -32582,7 +32618,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="3" t="s">
-        <v>2170</v>
+        <v>2175</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
@@ -32596,7 +32632,7 @@
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="8" t="s">
-        <v>2171</v>
+        <v>2176</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>212</v>
@@ -32605,7 +32641,7 @@
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="12" t="s">
-        <v>2172</v>
+        <v>2177</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>212</v>
@@ -32616,7 +32652,7 @@
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>2173</v>
+        <v>2178</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>212</v>
@@ -32634,7 +32670,7 @@
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="8" t="s">
-        <v>2174</v>
+        <v>2179</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>212</v>
@@ -32645,7 +32681,7 @@
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>2175</v>
+        <v>2180</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>212</v>
@@ -32656,7 +32692,7 @@
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="12" t="s">
-        <v>2176</v>
+        <v>2181</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>212</v>
@@ -32667,18 +32703,18 @@
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="12" t="s">
-        <v>2177</v>
+        <v>2182</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>212</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>2178</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
-        <v>2179</v>
+        <v>2184</v>
       </c>
       <c r="C91" s="12" t="s">
         <v>212</v>
@@ -32689,7 +32725,7 @@
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="8" t="s">
-        <v>2180</v>
+        <v>2185</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>212</v>
@@ -32700,18 +32736,18 @@
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="12" t="s">
-        <v>2181</v>
+        <v>2186</v>
       </c>
       <c r="C93" s="12" t="s">
         <v>212</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>2182</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="8" t="s">
-        <v>2183</v>
+        <v>2188</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>212</v>
@@ -32722,7 +32758,7 @@
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="12" t="s">
-        <v>2184</v>
+        <v>2189</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>212</v>
@@ -32733,7 +32769,7 @@
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="12" t="s">
-        <v>2185</v>
+        <v>2190</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>212</v>
@@ -32744,7 +32780,7 @@
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="8" t="s">
-        <v>2186</v>
+        <v>2191</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>212</v>
@@ -32755,7 +32791,7 @@
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="12" t="s">
-        <v>2105</v>
+        <v>2110</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>212</v>
@@ -32766,7 +32802,7 @@
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="8" t="s">
-        <v>2187</v>
+        <v>2192</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>212</v>
@@ -32777,7 +32813,7 @@
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="12" t="s">
-        <v>2188</v>
+        <v>2193</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>212</v>
@@ -32788,7 +32824,7 @@
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>2189</v>
+        <v>2194</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>212</v>
@@ -32799,7 +32835,7 @@
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>2190</v>
+        <v>2195</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>212</v>
@@ -32810,16 +32846,16 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="3" t="s">
-        <v>2191</v>
+        <v>2196</v>
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3" t="s">
-        <v>2192</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
-        <v>2193</v>
+        <v>2198</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>212</v>
@@ -32830,18 +32866,18 @@
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="12" t="s">
-        <v>2194</v>
+        <v>2199</v>
       </c>
       <c r="C105" s="12" t="s">
         <v>212</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>2195</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="8" t="s">
-        <v>2196</v>
+        <v>2201</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>212</v>
@@ -32852,7 +32888,7 @@
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="12" t="s">
-        <v>2197</v>
+        <v>2202</v>
       </c>
       <c r="C107" s="12" t="s">
         <v>212</v>
@@ -32863,7 +32899,7 @@
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="8" t="s">
-        <v>2198</v>
+        <v>2203</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>212</v>
@@ -32874,7 +32910,7 @@
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="12" t="s">
-        <v>2199</v>
+        <v>2204</v>
       </c>
       <c r="C109" s="12" t="s">
         <v>212</v>
@@ -32895,7 +32931,7 @@
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="8" t="s">
-        <v>2200</v>
+        <v>2205</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>212</v>
@@ -32906,7 +32942,7 @@
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="12" t="s">
-        <v>2201</v>
+        <v>2206</v>
       </c>
       <c r="C113" s="12" t="s">
         <v>212</v>
@@ -32922,7 +32958,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
-        <v>2202</v>
+        <v>2207</v>
       </c>
       <c r="C115" s="0"/>
       <c r="D115" s="0" t="s">
@@ -32931,16 +32967,16 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="0" t="s">
-        <v>2203</v>
+        <v>2208</v>
       </c>
       <c r="C116" s="0"/>
       <c r="D116" s="0" t="s">
-        <v>2204</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="0" t="s">
-        <v>2205</v>
+        <v>2210</v>
       </c>
       <c r="C117" s="0"/>
       <c r="D117" s="0" t="s">
@@ -32954,7 +32990,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="0" t="s">
-        <v>2206</v>
+        <v>2211</v>
       </c>
       <c r="C119" s="0"/>
       <c r="D119" s="0" t="n">
@@ -32977,7 +33013,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
-        <v>2207</v>
+        <v>2212</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="3" t="s">
@@ -32986,27 +33022,27 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>2208</v>
+        <v>2213</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
-        <v>2204</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="8" t="s">
-        <v>2209</v>
+        <v>2214</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>212</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>2210</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="12" t="s">
-        <v>2211</v>
+        <v>2216</v>
       </c>
       <c r="C125" s="12" t="s">
         <v>212</v>
@@ -33017,7 +33053,7 @@
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="12" t="s">
-        <v>2212</v>
+        <v>2217</v>
       </c>
       <c r="C126" s="12" t="s">
         <v>212</v>
@@ -33028,7 +33064,7 @@
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="8" t="s">
-        <v>2213</v>
+        <v>2218</v>
       </c>
       <c r="C127" s="8" t="s">
         <v>212</v>
@@ -33039,7 +33075,7 @@
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="12" t="s">
-        <v>2214</v>
+        <v>2219</v>
       </c>
       <c r="C128" s="12" t="s">
         <v>212</v>
@@ -33050,7 +33086,7 @@
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="12" t="s">
-        <v>2215</v>
+        <v>2220</v>
       </c>
       <c r="C129" s="12" t="s">
         <v>212</v>
@@ -33068,7 +33104,7 @@
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="12" t="s">
-        <v>2216</v>
+        <v>2221</v>
       </c>
       <c r="C131" s="12" t="s">
         <v>212</v>
@@ -33410,472 +33446,472 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="22" t="s">
-        <v>2217</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="22" t="s">
-        <v>2218</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="22" t="s">
-        <v>2219</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="22" t="s">
-        <v>2220</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>2221</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>2222</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>2223</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="22" t="s">
-        <v>2224</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="22" t="s">
-        <v>2225</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="22" t="s">
-        <v>2226</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="22" t="s">
-        <v>2227</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="22" t="s">
-        <v>2228</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="22" t="s">
-        <v>2229</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="22" t="s">
-        <v>2230</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="22" t="s">
-        <v>2231</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="22" t="s">
-        <v>2232</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="22" t="s">
-        <v>2233</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="22" t="s">
-        <v>2234</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="22" t="s">
-        <v>2235</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="22" t="s">
-        <v>2236</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="22" t="s">
-        <v>2237</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="22" t="s">
-        <v>2238</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="22" t="s">
-        <v>2239</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="22" t="s">
-        <v>2240</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="22" t="s">
-        <v>2241</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="22" t="s">
-        <v>2242</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="22" t="s">
-        <v>2243</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="22" t="s">
-        <v>2244</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="22" t="s">
-        <v>2245</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="22" t="s">
-        <v>2246</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="22" t="s">
-        <v>2247</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="22" t="s">
-        <v>2248</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="22" t="s">
-        <v>2249</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="22" t="s">
-        <v>2250</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="22" t="s">
-        <v>2251</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="22" t="s">
-        <v>2252</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="22" t="s">
-        <v>2253</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="22" t="s">
-        <v>2254</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="22" t="s">
-        <v>2255</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="22" t="s">
-        <v>2256</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="22" t="s">
-        <v>2257</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="22" t="s">
-        <v>2258</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="22" t="s">
-        <v>2259</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="22" t="s">
-        <v>2260</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="22" t="s">
-        <v>2261</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="22" t="s">
-        <v>2262</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="22" t="s">
-        <v>2263</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="22" t="s">
-        <v>2264</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="22" t="s">
-        <v>2265</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="22" t="s">
-        <v>2266</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="22" t="s">
-        <v>2267</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="22" t="s">
-        <v>2268</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="22" t="s">
-        <v>2269</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="22" t="s">
-        <v>2270</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="22" t="s">
-        <v>2271</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="22" t="s">
-        <v>2272</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="22" t="s">
-        <v>2273</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="22" t="s">
-        <v>2274</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="22" t="s">
-        <v>2275</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="22" t="s">
-        <v>2276</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="22" t="s">
-        <v>2277</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="22" t="s">
-        <v>2278</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="22" t="s">
-        <v>2279</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="22" t="s">
-        <v>2280</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="22" t="s">
-        <v>2281</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="22" t="s">
-        <v>2282</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="22" t="s">
-        <v>2283</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="22" t="s">
-        <v>2284</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="22" t="s">
-        <v>2285</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="22" t="s">
-        <v>2286</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="22" t="s">
-        <v>2287</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="22" t="s">
-        <v>2288</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="22" t="s">
-        <v>2289</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="22" t="s">
-        <v>2290</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="22" t="s">
-        <v>2291</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="22" t="s">
-        <v>2292</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="22" t="s">
-        <v>2293</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="22" t="s">
-        <v>2294</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="22" t="s">
-        <v>2295</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="22" t="s">
-        <v>2296</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="22" t="s">
-        <v>2297</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="22" t="s">
-        <v>2298</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="22" t="s">
-        <v>2299</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="22" t="s">
-        <v>2300</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="22" t="s">
-        <v>2301</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="22" t="s">
-        <v>2302</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="22" t="s">
-        <v>2303</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="22" t="s">
-        <v>2304</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="22" t="s">
-        <v>2305</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="22" t="s">
-        <v>2306</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="22" t="s">
-        <v>2307</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="22" t="s">
-        <v>2308</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="22" t="s">
-        <v>2309</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="22" t="s">
-        <v>2310</v>
+        <v>2315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new websites to check
</commit_message>
<xml_diff>
--- a/pull-requests/filters.xlsx
+++ b/pull-requests/filters.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5224" uniqueCount="2316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5226" uniqueCount="2317">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -5280,6 +5280,9 @@
   </si>
   <si>
     <t xml:space="preserve">http://www.racingforum.pl/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://cieszyninfo.pl</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.24gliwice.pl/wiadomosci/nie-umial-pogodzic-sie-z-odrzuceniem-uporczywie-nekal-wybranke-sms-ami-i-telefonami/</t>
@@ -7539,10 +7542,10 @@
   </sheetPr>
   <dimension ref="A1:M990"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A962" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B962" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A962" activeCellId="0" sqref="A962"/>
-      <selection pane="topRight" activeCell="D991" activeCellId="0" sqref="D991"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A845" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B845" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A845" activeCellId="0" sqref="A845"/>
+      <selection pane="topRight" activeCell="B874" activeCellId="0" sqref="B874"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -28669,12 +28672,16 @@
         <v>212</v>
       </c>
     </row>
-    <row r="870" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B870" s="23"/>
+    <row r="870" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B870" s="23" t="s">
+        <v>1145</v>
+      </c>
       <c r="C870" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D870" s="8"/>
+      <c r="D870" s="8" t="s">
+        <v>1746</v>
+      </c>
       <c r="E870" s="12" t="s">
         <v>212</v>
       </c>
@@ -29128,23 +29135,23 @@
     </row>
     <row r="902" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F902" s="3" t="s">
-        <v>1746</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="906" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D906" s="3" t="s">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="F906" s="3" t="s">
-        <v>1748</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="907" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D907" s="3" t="s">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="F907" s="3" t="s">
-        <v>1750</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="908" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29152,15 +29159,15 @@
         <v>1</v>
       </c>
       <c r="F908" s="3" t="s">
-        <v>1751</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="909" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D909" s="3" t="s">
-        <v>1752</v>
+        <v>1753</v>
       </c>
       <c r="F909" s="3" t="s">
-        <v>1753</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="911" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29168,10 +29175,10 @@
     </row>
     <row r="912" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D912" s="3" t="s">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="F912" s="3" t="s">
-        <v>1755</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="913" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29179,7 +29186,7 @@
         <v>1</v>
       </c>
       <c r="F913" s="3" t="s">
-        <v>1756</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="914" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29204,13 +29211,13 @@
     </row>
     <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D918" s="12" t="s">
-        <v>1757</v>
+        <v>1758</v>
       </c>
       <c r="E918" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F918" s="12" t="s">
-        <v>1758</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29221,7 +29228,7 @@
         <v>212</v>
       </c>
       <c r="F919" s="8" t="s">
-        <v>1759</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29232,7 +29239,7 @@
         <v>212</v>
       </c>
       <c r="F920" s="12" t="s">
-        <v>1760</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29241,7 +29248,7 @@
         <v>212</v>
       </c>
       <c r="F921" s="12" t="s">
-        <v>1761</v>
+        <v>1762</v>
       </c>
     </row>
     <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29250,7 +29257,7 @@
         <v>212</v>
       </c>
       <c r="F922" s="8" t="s">
-        <v>1762</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="923" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29266,7 +29273,7 @@
         <v>212</v>
       </c>
       <c r="F924" s="8" t="s">
-        <v>1763</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29277,40 +29284,40 @@
         <v>212</v>
       </c>
       <c r="F925" s="12" t="s">
-        <v>1764</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D926" s="8" t="s">
-        <v>1765</v>
+        <v>1766</v>
       </c>
       <c r="E926" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F926" s="8" t="s">
-        <v>1766</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D927" s="12" t="s">
-        <v>1765</v>
+        <v>1766</v>
       </c>
       <c r="E927" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F927" s="12" t="s">
-        <v>1767</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D928" s="8" t="s">
-        <v>1768</v>
+        <v>1769</v>
       </c>
       <c r="E928" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F928" s="8" t="s">
-        <v>1769</v>
+        <v>1770</v>
       </c>
     </row>
     <row r="929" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29333,29 +29340,29 @@
         <v>212</v>
       </c>
       <c r="F931" s="12" t="s">
-        <v>1770</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D932" s="8" t="s">
-        <v>1771</v>
+        <v>1772</v>
       </c>
       <c r="E932" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F932" s="8" t="s">
-        <v>1772</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D933" s="12" t="s">
-        <v>1773</v>
+        <v>1774</v>
       </c>
       <c r="E933" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F933" s="29" t="s">
-        <v>1774</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="934" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29371,7 +29378,7 @@
         <v>212</v>
       </c>
       <c r="F935" s="12" t="s">
-        <v>1775</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29382,7 +29389,7 @@
         <v>212</v>
       </c>
       <c r="F936" s="8" t="s">
-        <v>1776</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29394,24 +29401,24 @@
     </row>
     <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D938" s="8" t="s">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="E938" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F938" s="8" t="s">
-        <v>1778</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D939" s="12" t="s">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="E939" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F939" s="12" t="s">
-        <v>1780</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29429,7 +29436,7 @@
         <v>212</v>
       </c>
       <c r="F941" s="12" t="s">
-        <v>1781</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29440,7 +29447,7 @@
         <v>212</v>
       </c>
       <c r="F942" s="8" t="s">
-        <v>1782</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29451,7 +29458,7 @@
         <v>212</v>
       </c>
       <c r="F943" s="12" t="s">
-        <v>1783</v>
+        <v>1784</v>
       </c>
     </row>
     <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29469,7 +29476,7 @@
         <v>212</v>
       </c>
       <c r="F945" s="12" t="s">
-        <v>1784</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="946" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29479,7 +29486,7 @@
     </row>
     <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D947" s="12" t="s">
-        <v>1785</v>
+        <v>1786</v>
       </c>
       <c r="E947" s="12" t="s">
         <v>212</v>
@@ -29503,7 +29510,7 @@
         <v>212</v>
       </c>
       <c r="F949" s="12" t="s">
-        <v>1786</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29514,7 +29521,7 @@
         <v>212</v>
       </c>
       <c r="F950" s="8" t="s">
-        <v>1787</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29525,7 +29532,7 @@
         <v>212</v>
       </c>
       <c r="F951" s="12" t="s">
-        <v>1788</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29543,34 +29550,34 @@
         <v>212</v>
       </c>
       <c r="F953" s="12" t="s">
-        <v>1789</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D954" s="8" t="s">
-        <v>1790</v>
+        <v>1791</v>
       </c>
       <c r="E954" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F954" s="29" t="s">
-        <v>1791</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="955" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D955" s="3" t="s">
-        <v>1792</v>
+        <v>1793</v>
       </c>
       <c r="F955" s="3" t="s">
-        <v>1793</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="956" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D956" s="3" t="s">
-        <v>1794</v>
+        <v>1795</v>
       </c>
       <c r="F956" s="3" t="s">
-        <v>1795</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="957" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29578,7 +29585,7 @@
         <v>2</v>
       </c>
       <c r="F957" s="3" t="s">
-        <v>1796</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="958" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29586,23 +29593,23 @@
         <v>1</v>
       </c>
       <c r="F958" s="3" t="s">
-        <v>1797</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="960" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D960" s="3" t="s">
-        <v>1798</v>
+        <v>1799</v>
       </c>
       <c r="F960" s="3" t="s">
-        <v>1799</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="961" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D961" s="3" t="s">
-        <v>1800</v>
+        <v>1801</v>
       </c>
       <c r="F961" s="3" t="s">
-        <v>1801</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="962" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29610,7 +29617,7 @@
         <v>1</v>
       </c>
       <c r="F962" s="3" t="s">
-        <v>1802</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="964" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29618,12 +29625,12 @@
         <v>1</v>
       </c>
       <c r="F964" s="3" t="s">
-        <v>1803</v>
+        <v>1804</v>
       </c>
     </row>
     <row r="965" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F965" s="29" t="s">
-        <v>1804</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="966" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29631,7 +29638,7 @@
         <v>1</v>
       </c>
       <c r="F966" s="3" t="s">
-        <v>1805</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="967" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29639,52 +29646,52 @@
         <v>2</v>
       </c>
       <c r="F967" s="3" t="s">
-        <v>1806</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="968" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F968" s="29" t="s">
-        <v>1807</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="969" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D969" s="3" t="s">
-        <v>1808</v>
+        <v>1809</v>
       </c>
       <c r="F969" s="3" t="s">
-        <v>1809</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="970" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D970" s="3" t="s">
-        <v>1810</v>
+        <v>1811</v>
       </c>
       <c r="F970" s="3" t="s">
-        <v>1811</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="971" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D971" s="3" t="s">
-        <v>1810</v>
+        <v>1811</v>
       </c>
       <c r="F971" s="3" t="s">
-        <v>1812</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="972" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D972" s="3" t="s">
-        <v>1810</v>
+        <v>1811</v>
       </c>
       <c r="F972" s="3" t="s">
-        <v>1813</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="974" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D974" s="3" t="s">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="F974" s="3" t="s">
-        <v>1814</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="975" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29695,55 +29702,55 @@
         <v>1</v>
       </c>
       <c r="F976" s="3" t="s">
-        <v>1815</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="977" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D977" s="3" t="s">
-        <v>1816</v>
+        <v>1817</v>
       </c>
       <c r="F977" s="3" t="s">
-        <v>1817</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="978" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D978" s="3" t="s">
-        <v>1818</v>
+        <v>1819</v>
       </c>
       <c r="F978" s="3" t="s">
-        <v>1819</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="979" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D979" s="3" t="s">
-        <v>1808</v>
+        <v>1809</v>
       </c>
       <c r="F979" s="3" t="s">
-        <v>1820</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="981" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D981" s="3" t="s">
-        <v>1821</v>
+        <v>1822</v>
       </c>
       <c r="F981" s="3" t="s">
-        <v>1822</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="982" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D982" s="3" t="s">
-        <v>1823</v>
+        <v>1824</v>
       </c>
       <c r="F982" s="3" t="s">
-        <v>1824</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="983" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D983" s="3" t="s">
-        <v>1808</v>
+        <v>1809</v>
       </c>
       <c r="F983" s="3" t="s">
-        <v>1825</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="984" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29751,49 +29758,49 @@
         <v>1</v>
       </c>
       <c r="F984" s="3" t="s">
-        <v>1826</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="985" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D985" s="3" t="s">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="F985" s="3" t="s">
-        <v>1827</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="986" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D986" s="3" t="s">
-        <v>1808</v>
+        <v>1809</v>
       </c>
       <c r="F986" s="3" t="s">
-        <v>1828</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="987" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F987" s="3" t="s">
-        <v>1829</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="988" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F988" s="3" t="s">
-        <v>1830</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="989" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D989" s="3" t="s">
-        <v>1831</v>
+        <v>1832</v>
       </c>
       <c r="F989" s="3" t="s">
-        <v>1832</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="990" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D990" s="3" t="s">
-        <v>1833</v>
+        <v>1834</v>
       </c>
       <c r="F990" s="3" t="s">
-        <v>1834</v>
+        <v>1835</v>
       </c>
     </row>
   </sheetData>
@@ -30771,1362 +30778,1362 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>1835</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>1836</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>1837</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>1838</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>1839</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>1841</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>1842</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>1843</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>1844</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>1845</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>1846</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>1847</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>1848</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>1849</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>1850</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>1839</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>1851</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>1852</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>1853</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="s">
-        <v>1854</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>1855</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="s">
-        <v>1856</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="s">
-        <v>1857</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="s">
-        <v>1858</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="s">
-        <v>1859</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="22" t="s">
-        <v>1860</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="22" t="s">
-        <v>1861</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="22" t="s">
-        <v>1862</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="22" t="s">
-        <v>1863</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="22" t="s">
-        <v>1864</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="22" t="s">
-        <v>1865</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="22" t="s">
-        <v>1866</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="22" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="22" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="22" t="s">
-        <v>1869</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="22" t="s">
-        <v>1870</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="22" t="s">
-        <v>1871</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="22" t="s">
-        <v>1872</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="22" t="s">
-        <v>1873</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="22" t="s">
-        <v>1874</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="22" t="s">
-        <v>1875</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="22" t="s">
-        <v>1876</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="22" t="s">
-        <v>1877</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="22" t="s">
-        <v>1878</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="22" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="22" t="s">
-        <v>1880</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="22" t="s">
-        <v>1881</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="22" t="s">
-        <v>1882</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="22" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="22" t="s">
-        <v>1884</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="22" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="22" t="s">
-        <v>1886</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="22" t="s">
-        <v>1887</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="22" t="s">
-        <v>1888</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="22" t="s">
-        <v>1889</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="22" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="22" t="s">
-        <v>1891</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="22" t="s">
-        <v>1892</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="22" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="22" t="s">
-        <v>1894</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="22" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="22" t="s">
-        <v>1896</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="22" t="s">
-        <v>1897</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="22" t="s">
-        <v>1898</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="22" t="s">
-        <v>1899</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="22" t="s">
-        <v>1900</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="22" t="s">
-        <v>1901</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="22" t="s">
-        <v>1902</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="22" t="s">
-        <v>1903</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="22" t="s">
-        <v>1904</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="22" t="s">
-        <v>1905</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="22" t="s">
-        <v>1906</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="22" t="s">
-        <v>1907</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="22" t="s">
-        <v>1908</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="22" t="s">
-        <v>1909</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="22" t="s">
-        <v>1910</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="22" t="s">
-        <v>1911</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="22" t="s">
-        <v>1912</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="22" t="s">
-        <v>1913</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="22" t="s">
-        <v>1914</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="22" t="s">
-        <v>1915</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="22" t="s">
-        <v>1916</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="22" t="s">
-        <v>1917</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="22" t="s">
-        <v>1918</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="22" t="s">
-        <v>1919</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="22" t="s">
-        <v>1920</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="22" t="s">
-        <v>1921</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="22" t="s">
-        <v>1922</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="22" t="s">
-        <v>1841</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="22" t="s">
-        <v>1923</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="22" t="s">
-        <v>1924</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="22" t="s">
-        <v>1925</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="22" t="s">
-        <v>1848</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="22" t="s">
-        <v>1926</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="22" t="s">
-        <v>1927</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="22" t="s">
-        <v>1928</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="22" t="s">
-        <v>1929</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="22" t="s">
-        <v>1930</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="22" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="22" t="s">
-        <v>1932</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="22" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="22" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="22" t="s">
-        <v>1935</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="22" t="s">
-        <v>1936</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="22" t="s">
-        <v>1937</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="22" t="s">
-        <v>1938</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="22" t="s">
-        <v>1939</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="22" t="s">
-        <v>1940</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="22" t="s">
-        <v>1941</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="22" t="s">
-        <v>1942</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="22" t="s">
-        <v>1943</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="22" t="s">
-        <v>1944</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="22" t="s">
-        <v>1945</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="22" t="s">
-        <v>1946</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="22" t="s">
-        <v>1947</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="22" t="s">
-        <v>1948</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="22" t="s">
-        <v>1949</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="22" t="s">
-        <v>1950</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="22" t="s">
-        <v>1951</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="22" t="s">
-        <v>1952</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="22" t="s">
-        <v>1953</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="22" t="s">
-        <v>1954</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="22" t="s">
-        <v>1955</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="22" t="s">
-        <v>1956</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="22" t="s">
-        <v>1957</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="22" t="s">
-        <v>1958</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="22" t="s">
-        <v>1959</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="22" t="s">
-        <v>1960</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="22" t="s">
-        <v>1961</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="22" t="s">
-        <v>1962</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="22" t="s">
-        <v>1963</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="22" t="s">
-        <v>1964</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="22" t="s">
-        <v>1965</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="22" t="s">
-        <v>1966</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="22" t="s">
-        <v>1967</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="22" t="s">
-        <v>1968</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="22" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="22" t="s">
-        <v>1970</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="22" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="22" t="s">
-        <v>1972</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="22" t="s">
-        <v>1973</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="22" t="s">
-        <v>1974</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="22" t="s">
-        <v>1975</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="22" t="s">
-        <v>1976</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="22" t="s">
-        <v>1977</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="22" t="s">
-        <v>1978</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="22" t="s">
-        <v>1979</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="22" t="s">
-        <v>1980</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="22" t="s">
-        <v>1981</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="22" t="s">
-        <v>1982</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="22" t="s">
-        <v>1983</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="22" t="s">
-        <v>1984</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="22" t="s">
-        <v>1985</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="22" t="s">
-        <v>1986</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="22" t="s">
-        <v>1987</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="22" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="22" t="s">
-        <v>1989</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="22" t="s">
-        <v>1990</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="22" t="s">
-        <v>1991</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="22" t="s">
-        <v>1992</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="22" t="s">
-        <v>1993</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="22" t="s">
-        <v>1994</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="22" t="s">
-        <v>1995</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="22" t="s">
-        <v>1996</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="22" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="22" t="s">
-        <v>1998</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="22" t="s">
-        <v>1999</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="22" t="s">
-        <v>2000</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="22" t="s">
-        <v>2001</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="22" t="s">
-        <v>2002</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="22" t="s">
-        <v>2003</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="22" t="s">
-        <v>2004</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="22" t="s">
-        <v>2005</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="22" t="s">
-        <v>2006</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="22" t="s">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="22" t="s">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="22" t="s">
-        <v>2009</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="22" t="s">
-        <v>2010</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="22" t="s">
-        <v>2011</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="22" t="s">
-        <v>2012</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="22" t="s">
-        <v>2013</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="22" t="s">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="22" t="s">
-        <v>2015</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="22" t="s">
-        <v>2016</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="22" t="s">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="22" t="s">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="22" t="s">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="22" t="s">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="22" t="s">
-        <v>2021</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="22" t="s">
-        <v>2022</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="22" t="s">
-        <v>2023</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="22" t="s">
-        <v>2024</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="22" t="s">
-        <v>2025</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="22" t="s">
-        <v>2026</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="22" t="s">
-        <v>2027</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="22" t="s">
-        <v>2028</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="22" t="s">
-        <v>1836</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="22" t="s">
-        <v>2029</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="22" t="s">
-        <v>2030</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="22" t="s">
-        <v>2031</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="22" t="s">
-        <v>2032</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="22" t="s">
-        <v>2033</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="22" t="s">
-        <v>2034</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="22" t="s">
-        <v>2035</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="22" t="s">
-        <v>2036</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="22" t="s">
-        <v>2037</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="22" t="s">
-        <v>2038</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="22" t="s">
-        <v>2039</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="22" t="s">
-        <v>2040</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="22" t="s">
-        <v>2041</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="22" t="s">
-        <v>2042</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="22" t="s">
-        <v>2043</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="22" t="s">
-        <v>2044</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="22" t="s">
-        <v>2045</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="22" t="s">
-        <v>2046</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="22" t="s">
-        <v>2047</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="22" t="s">
-        <v>2048</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="22" t="s">
-        <v>2049</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="22" t="s">
-        <v>2050</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="22" t="s">
-        <v>2051</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="22" t="s">
-        <v>2052</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="22" t="s">
-        <v>2053</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="22" t="s">
-        <v>2054</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="22" t="s">
-        <v>2055</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="22" t="s">
-        <v>2056</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="22" t="s">
-        <v>2057</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="22" t="s">
-        <v>2058</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="22" t="s">
-        <v>2059</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="22" t="s">
-        <v>2060</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="22" t="s">
-        <v>2061</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="22" t="s">
-        <v>2062</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="22" t="s">
-        <v>2063</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="22" t="s">
-        <v>2064</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="22" t="s">
-        <v>2065</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="22" t="s">
-        <v>2066</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="22" t="s">
-        <v>2067</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="22" t="s">
-        <v>2068</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="22" t="s">
-        <v>2069</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="22" t="s">
-        <v>2070</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="22" t="s">
-        <v>2071</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="22" t="s">
-        <v>2072</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="22" t="s">
-        <v>2073</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="22" t="s">
-        <v>1846</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="22" t="s">
-        <v>2074</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="22" t="s">
-        <v>2075</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="22" t="s">
-        <v>2076</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="22" t="s">
-        <v>2077</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="22" t="s">
-        <v>2078</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="22" t="s">
-        <v>2079</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="22" t="s">
-        <v>2080</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="22" t="s">
-        <v>2081</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="22" t="s">
-        <v>2082</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="22" t="s">
-        <v>2083</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="22" t="s">
-        <v>2084</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="22" t="s">
-        <v>2085</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="22" t="s">
-        <v>2086</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="22" t="s">
-        <v>2087</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="22" t="s">
-        <v>2088</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="22" t="s">
-        <v>2089</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="22" t="s">
-        <v>2090</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="22" t="s">
-        <v>2091</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="22" t="s">
-        <v>2092</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="22" t="s">
-        <v>2093</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="22" t="s">
-        <v>2094</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="22" t="s">
-        <v>2095</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="22" t="s">
-        <v>2096</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="22" t="s">
-        <v>2097</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="22" t="s">
-        <v>1853</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="22" t="s">
-        <v>2098</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="22" t="s">
-        <v>2099</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="22" t="s">
-        <v>2100</v>
+        <v>2101</v>
       </c>
     </row>
   </sheetData>
@@ -32161,48 +32168,48 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="36" t="s">
-        <v>2101</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="37" t="s">
-        <v>2102</v>
+        <v>2103</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>2103</v>
+        <v>2104</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>2104</v>
+        <v>2105</v>
       </c>
       <c r="I2" s="40"/>
       <c r="K2" s="22" t="s">
-        <v>2105</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="37" t="s">
-        <v>2106</v>
+        <v>2107</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>2103</v>
+        <v>2104</v>
       </c>
       <c r="H3" s="38"/>
       <c r="I3" s="41"/>
       <c r="J3" s="38"/>
       <c r="K3" s="12" t="s">
-        <v>2107</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="22" t="s">
-        <v>2108</v>
+        <v>2109</v>
       </c>
       <c r="C4" s="42"/>
       <c r="H4" s="38"/>
       <c r="I4" s="41"/>
       <c r="J4" s="38"/>
       <c r="K4" s="12" t="s">
-        <v>2109</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32211,7 +32218,7 @@
       <c r="I5" s="41"/>
       <c r="J5" s="38"/>
       <c r="K5" s="8" t="s">
-        <v>2110</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32230,90 +32237,90 @@
       <c r="I7" s="41"/>
       <c r="J7" s="38"/>
       <c r="K7" s="29" t="s">
-        <v>2111</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="12" t="s">
-        <v>2112</v>
+        <v>2113</v>
       </c>
       <c r="C8" s="42"/>
       <c r="H8" s="38"/>
       <c r="I8" s="41"/>
       <c r="J8" s="38"/>
       <c r="K8" s="22" t="s">
-        <v>2113</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="29" t="s">
-        <v>2114</v>
+        <v>2115</v>
       </c>
       <c r="C9" s="42"/>
       <c r="H9" s="38"/>
       <c r="I9" s="41"/>
       <c r="J9" s="38"/>
       <c r="K9" s="8" t="s">
-        <v>2115</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="8" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
       <c r="C10" s="42"/>
       <c r="H10" s="38"/>
       <c r="I10" s="41"/>
       <c r="J10" s="38"/>
       <c r="K10" s="12" t="s">
-        <v>2117</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="12" t="s">
-        <v>2118</v>
+        <v>2119</v>
       </c>
       <c r="C11" s="42"/>
       <c r="H11" s="38"/>
       <c r="I11" s="41"/>
       <c r="J11" s="38"/>
       <c r="K11" s="8" t="s">
-        <v>2119</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="8" t="s">
-        <v>2120</v>
+        <v>2121</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>2121</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0"/>
       <c r="K13" s="8" t="s">
-        <v>2122</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="22" t="s">
-        <v>2123</v>
+        <v>2124</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>2124</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
-        <v>2125</v>
+        <v>2126</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>2126</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K16" s="12" t="s">
-        <v>2127</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32321,10 +32328,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="22" t="s">
-        <v>2128</v>
+        <v>2129</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>2129</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32332,109 +32339,109 @@
         <v>119</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>2130</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>2131</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>2132</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="22" t="s">
-        <v>2133</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>2134</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>2135</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>2136</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="22" t="s">
-        <v>2137</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="22" t="s">
-        <v>2138</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="22" t="s">
-        <v>2139</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>2140</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="22" t="s">
-        <v>2141</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>2142</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="22" t="s">
-        <v>2143</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>2144</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="22" t="s">
-        <v>2145</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="22" t="s">
-        <v>2146</v>
+        <v>2147</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="22" t="s">
-        <v>2147</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="22" t="s">
-        <v>2148</v>
+        <v>2149</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="22" t="s">
-        <v>2149</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="22" t="s">
-        <v>2150</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32444,47 +32451,47 @@
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="22" t="s">
-        <v>2151</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="22" t="s">
-        <v>2152</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="22" t="s">
-        <v>2153</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="22" t="s">
-        <v>2154</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="22" t="s">
-        <v>2155</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="22" t="s">
-        <v>2156</v>
+        <v>2157</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="22" t="s">
-        <v>2157</v>
+        <v>2158</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="22" t="s">
-        <v>2158</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="22" t="s">
-        <v>2159</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32492,17 +32499,17 @@
         <v>193</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>1765</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="22" t="s">
-        <v>2160</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="22" t="s">
-        <v>2161</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32512,32 +32519,32 @@
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="22" t="s">
-        <v>2162</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="22" t="s">
-        <v>2163</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="22" t="s">
-        <v>2164</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="22" t="s">
-        <v>2165</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="22" t="s">
-        <v>2166</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="8" t="s">
-        <v>2167</v>
+        <v>2168</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>212</v>
@@ -32548,7 +32555,7 @@
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="8" t="s">
-        <v>2168</v>
+        <v>2169</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>212</v>
@@ -32559,13 +32566,13 @@
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="8" t="s">
-        <v>2169</v>
+        <v>2170</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>212</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>2170</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32584,12 +32591,12 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>2171</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="3" t="s">
-        <v>2172</v>
+        <v>2173</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="n">
@@ -32598,7 +32605,7 @@
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="8" t="s">
-        <v>2173</v>
+        <v>2174</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>212</v>
@@ -32609,7 +32616,7 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="3" t="s">
-        <v>2174</v>
+        <v>2175</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="n">
@@ -32618,7 +32625,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="3" t="s">
-        <v>2175</v>
+        <v>2176</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
@@ -32632,7 +32639,7 @@
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="8" t="s">
-        <v>2176</v>
+        <v>2177</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>212</v>
@@ -32641,7 +32648,7 @@
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="12" t="s">
-        <v>2177</v>
+        <v>2178</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>212</v>
@@ -32652,7 +32659,7 @@
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>2178</v>
+        <v>2179</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>212</v>
@@ -32670,7 +32677,7 @@
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="8" t="s">
-        <v>2179</v>
+        <v>2180</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>212</v>
@@ -32681,7 +32688,7 @@
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>2180</v>
+        <v>2181</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>212</v>
@@ -32692,7 +32699,7 @@
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="12" t="s">
-        <v>2181</v>
+        <v>2182</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>212</v>
@@ -32703,18 +32710,18 @@
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="12" t="s">
-        <v>2182</v>
+        <v>2183</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>212</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>2183</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
-        <v>2184</v>
+        <v>2185</v>
       </c>
       <c r="C91" s="12" t="s">
         <v>212</v>
@@ -32725,7 +32732,7 @@
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="8" t="s">
-        <v>2185</v>
+        <v>2186</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>212</v>
@@ -32736,18 +32743,18 @@
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="12" t="s">
-        <v>2186</v>
+        <v>2187</v>
       </c>
       <c r="C93" s="12" t="s">
         <v>212</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>2187</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="8" t="s">
-        <v>2188</v>
+        <v>2189</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>212</v>
@@ -32758,7 +32765,7 @@
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="12" t="s">
-        <v>2189</v>
+        <v>2190</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>212</v>
@@ -32769,7 +32776,7 @@
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="12" t="s">
-        <v>2190</v>
+        <v>2191</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>212</v>
@@ -32780,7 +32787,7 @@
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="8" t="s">
-        <v>2191</v>
+        <v>2192</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>212</v>
@@ -32791,7 +32798,7 @@
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="12" t="s">
-        <v>2110</v>
+        <v>2111</v>
       </c>
       <c r="C98" s="12" t="s">
         <v>212</v>
@@ -32802,7 +32809,7 @@
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="8" t="s">
-        <v>2192</v>
+        <v>2193</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>212</v>
@@ -32813,7 +32820,7 @@
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="12" t="s">
-        <v>2193</v>
+        <v>2194</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>212</v>
@@ -32824,7 +32831,7 @@
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>2194</v>
+        <v>2195</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>212</v>
@@ -32835,7 +32842,7 @@
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>2195</v>
+        <v>2196</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>212</v>
@@ -32846,16 +32853,16 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="3" t="s">
-        <v>2196</v>
+        <v>2197</v>
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3" t="s">
-        <v>2197</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
-        <v>2198</v>
+        <v>2199</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>212</v>
@@ -32866,18 +32873,18 @@
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="12" t="s">
-        <v>2199</v>
+        <v>2200</v>
       </c>
       <c r="C105" s="12" t="s">
         <v>212</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>2200</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="8" t="s">
-        <v>2201</v>
+        <v>2202</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>212</v>
@@ -32888,7 +32895,7 @@
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="12" t="s">
-        <v>2202</v>
+        <v>2203</v>
       </c>
       <c r="C107" s="12" t="s">
         <v>212</v>
@@ -32899,7 +32906,7 @@
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="8" t="s">
-        <v>2203</v>
+        <v>2204</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>212</v>
@@ -32910,7 +32917,7 @@
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="12" t="s">
-        <v>2204</v>
+        <v>2205</v>
       </c>
       <c r="C109" s="12" t="s">
         <v>212</v>
@@ -32931,7 +32938,7 @@
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="8" t="s">
-        <v>2205</v>
+        <v>2206</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>212</v>
@@ -32942,7 +32949,7 @@
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="12" t="s">
-        <v>2206</v>
+        <v>2207</v>
       </c>
       <c r="C113" s="12" t="s">
         <v>212</v>
@@ -32958,7 +32965,7 @@
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
-        <v>2207</v>
+        <v>2208</v>
       </c>
       <c r="C115" s="0"/>
       <c r="D115" s="0" t="s">
@@ -32967,16 +32974,16 @@
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="0" t="s">
-        <v>2208</v>
+        <v>2209</v>
       </c>
       <c r="C116" s="0"/>
       <c r="D116" s="0" t="s">
-        <v>2209</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="0" t="s">
-        <v>2210</v>
+        <v>2211</v>
       </c>
       <c r="C117" s="0"/>
       <c r="D117" s="0" t="s">
@@ -32990,7 +32997,7 @@
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="0" t="s">
-        <v>2211</v>
+        <v>2212</v>
       </c>
       <c r="C119" s="0"/>
       <c r="D119" s="0" t="n">
@@ -33013,7 +33020,7 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
-        <v>2212</v>
+        <v>2213</v>
       </c>
       <c r="C122" s="3"/>
       <c r="D122" s="3" t="s">
@@ -33022,27 +33029,27 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>2213</v>
+        <v>2214</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
-        <v>2209</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="8" t="s">
-        <v>2214</v>
+        <v>2215</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>212</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>2215</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="12" t="s">
-        <v>2216</v>
+        <v>2217</v>
       </c>
       <c r="C125" s="12" t="s">
         <v>212</v>
@@ -33053,7 +33060,7 @@
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="12" t="s">
-        <v>2217</v>
+        <v>2218</v>
       </c>
       <c r="C126" s="12" t="s">
         <v>212</v>
@@ -33064,7 +33071,7 @@
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="8" t="s">
-        <v>2218</v>
+        <v>2219</v>
       </c>
       <c r="C127" s="8" t="s">
         <v>212</v>
@@ -33075,7 +33082,7 @@
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="12" t="s">
-        <v>2219</v>
+        <v>2220</v>
       </c>
       <c r="C128" s="12" t="s">
         <v>212</v>
@@ -33086,7 +33093,7 @@
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="12" t="s">
-        <v>2220</v>
+        <v>2221</v>
       </c>
       <c r="C129" s="12" t="s">
         <v>212</v>
@@ -33104,7 +33111,7 @@
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="12" t="s">
-        <v>2221</v>
+        <v>2222</v>
       </c>
       <c r="C131" s="12" t="s">
         <v>212</v>
@@ -33446,472 +33453,472 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1" s="22" t="s">
-        <v>2222</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="22" t="s">
-        <v>2223</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="22" t="s">
-        <v>2224</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="22" t="s">
-        <v>2225</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="22" t="s">
-        <v>2226</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="22" t="s">
-        <v>2227</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="22" t="s">
-        <v>2228</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="22" t="s">
-        <v>2229</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="22" t="s">
-        <v>2230</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="22" t="s">
-        <v>2231</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="22" t="s">
-        <v>2232</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="22" t="s">
-        <v>2233</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="22" t="s">
-        <v>2234</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="22" t="s">
-        <v>2235</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="22" t="s">
-        <v>2236</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="22" t="s">
-        <v>2237</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="22" t="s">
-        <v>2238</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="22" t="s">
-        <v>2239</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="22" t="s">
-        <v>2240</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="22" t="s">
-        <v>2241</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="22" t="s">
-        <v>2242</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="22" t="s">
-        <v>2243</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="22" t="s">
-        <v>2244</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="22" t="s">
-        <v>2245</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="22" t="s">
-        <v>2246</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="22" t="s">
-        <v>2247</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="22" t="s">
-        <v>2248</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="22" t="s">
-        <v>2249</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="22" t="s">
-        <v>2250</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="22" t="s">
-        <v>2251</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="22" t="s">
-        <v>2252</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="22" t="s">
-        <v>2253</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="22" t="s">
-        <v>2254</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="22" t="s">
-        <v>2255</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="22" t="s">
-        <v>2256</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="22" t="s">
-        <v>2257</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="22" t="s">
-        <v>2258</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="22" t="s">
-        <v>2259</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="22" t="s">
-        <v>2260</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="22" t="s">
-        <v>2261</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="22" t="s">
-        <v>2262</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="22" t="s">
-        <v>2263</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="22" t="s">
-        <v>2264</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="22" t="s">
-        <v>2265</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="22" t="s">
-        <v>2266</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="22" t="s">
-        <v>2267</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="22" t="s">
-        <v>2268</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="22" t="s">
-        <v>2269</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="22" t="s">
-        <v>2270</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="22" t="s">
-        <v>2271</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="22" t="s">
-        <v>2272</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="22" t="s">
-        <v>2273</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="22" t="s">
-        <v>2274</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="22" t="s">
-        <v>2275</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="22" t="s">
-        <v>2276</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="22" t="s">
-        <v>2277</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="22" t="s">
-        <v>2278</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="22" t="s">
-        <v>2279</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="22" t="s">
-        <v>2280</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="22" t="s">
-        <v>2281</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="22" t="s">
-        <v>2282</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="22" t="s">
-        <v>2283</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="22" t="s">
-        <v>2284</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="22" t="s">
-        <v>2285</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="22" t="s">
-        <v>2286</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="22" t="s">
-        <v>2287</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="22" t="s">
-        <v>2288</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="22" t="s">
-        <v>2289</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="22" t="s">
-        <v>2290</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="22" t="s">
-        <v>2291</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="22" t="s">
-        <v>2292</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="22" t="s">
-        <v>2293</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="22" t="s">
-        <v>2294</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="22" t="s">
-        <v>2295</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="22" t="s">
-        <v>2296</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="22" t="s">
-        <v>2297</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="22" t="s">
-        <v>2298</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="22" t="s">
-        <v>2299</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="22" t="s">
-        <v>2300</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="22" t="s">
-        <v>2301</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="22" t="s">
-        <v>2302</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="22" t="s">
-        <v>2303</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="22" t="s">
-        <v>2304</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="22" t="s">
-        <v>2305</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="22" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="22" t="s">
-        <v>2307</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="22" t="s">
-        <v>2308</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="22" t="s">
-        <v>2309</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="22" t="s">
-        <v>2310</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="22" t="s">
-        <v>2311</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="22" t="s">
-        <v>2312</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="22" t="s">
-        <v>2313</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="22" t="s">
-        <v>2314</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="22" t="s">
-        <v>2315</v>
+        <v>2316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update snippet list for WP group
</commit_message>
<xml_diff>
--- a/pull-requests/filters.xlsx
+++ b/pull-requests/filters.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="filters" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6420" uniqueCount="2551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6427" uniqueCount="2556">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -6283,6 +6283,9 @@
     <t xml:space="preserve">https://baltic.info.pl</t>
   </si>
   <si>
+    <t xml:space="preserve">https://dom.wp.pl/niedrogie-kawiarki-dla-milosnikow-kawy-wyjdzie-lepsza-niz-w-kawiarni-6269021409613953a</t>
+  </si>
+  <si>
     <t xml:space="preserve">Domain</t>
   </si>
   <si>
@@ -7483,12 +7486,27 @@
     <t xml:space="preserve">prawo.money.pl</t>
   </si>
   <si>
+    <t xml:space="preserve">ADVERT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://prawo.money.pl/aktualnosci/okiem-eksperta/artykul/jak-rozwiazac-problem-kredytu-po-rozwodzie,28,0,2111260.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.money.pl/gospodarka/pandemia-redukuje-miejsca-pracy-polacy-traca-zatrudnienie-6547870512462528a.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">poczta.o2.pl</t>
   </si>
   <si>
     <t xml:space="preserve">abczdrowie.pl</t>
   </si>
   <si>
+    <t xml:space="preserve">https://zywienie.abczdrowie.pl/kolendra-wlasciwosci-odzywcze-zastosowanie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.contentstream-bar</t>
+  </si>
+  <si>
     <t xml:space="preserve">bloog.pl</t>
   </si>
   <si>
@@ -7516,19 +7534,10 @@
     <t xml:space="preserve">homebook.pl</t>
   </si>
   <si>
-    <t xml:space="preserve">check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.homebook.pl/produkty/krzesla-i-fotele?fpid=40606973&amp;utm_source=banner_wp&amp;utm_medium=koszyk&amp;utm_campaign=affiliate_redirect</t>
-  </si>
-  <si>
-    <t xml:space="preserve">floating cersanit right corner</t>
-  </si>
-  <si>
     <t xml:space="preserve">kafeteria.pl</t>
   </si>
   <si>
-    <t xml:space="preserve">in same place</t>
+    <t xml:space="preserve">forum.kafeteria.pl</t>
   </si>
   <si>
     <t xml:space="preserve">komorkomania.pl</t>
@@ -7546,15 +7555,15 @@
     <t xml:space="preserve">parenting.pl</t>
   </si>
   <si>
+    <t xml:space="preserve">https://parenting.pl/baby-blues-nie-boj-sie-prosic-o-wsparcie</t>
+  </si>
+  <si>
     <t xml:space="preserve">pinger.pl</t>
   </si>
   <si>
     <t xml:space="preserve">pogodnie.pl</t>
   </si>
   <si>
-    <t xml:space="preserve">ADVERT</t>
-  </si>
-  <si>
     <t xml:space="preserve">broken</t>
   </si>
   <si>
@@ -7600,12 +7609,15 @@
     <t xml:space="preserve">gryonline.wp.pl</t>
   </si>
   <si>
+    <t xml:space="preserve">https://gwiazdy.wp.pl/renata-kaczoruk-znowu-zaskakuje-pokazala-odwazne-zdjecia-6547894606838400a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">holding.wp.pl</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ok</t>
   </si>
   <si>
-    <t xml:space="preserve">holding.wp.pl</t>
-  </si>
-  <si>
     <t xml:space="preserve">magazyn.wp.pl</t>
   </si>
   <si>
@@ -7618,12 +7630,12 @@
     <t xml:space="preserve">nocowanie.wp.pl</t>
   </si>
   <si>
+    <t xml:space="preserve">https://opinie.wp.pl/makowski-rekonstrukcja-scentralizuje-zarzadzanie-ministerstwami-po-raz-pierwszy-w-takiej-skali-opinia-6546925882837121a</t>
+  </si>
+  <si>
     <t xml:space="preserve">poczta.wp.pl</t>
   </si>
   <si>
-    <t xml:space="preserve">to check</t>
-  </si>
-  <si>
     <t xml:space="preserve">profil.wp.pl</t>
   </si>
   <si>
@@ -7642,7 +7654,7 @@
     <t xml:space="preserve">telewizja.wp.pl</t>
   </si>
   <si>
-    <t xml:space="preserve">TO SUBMIT</t>
+    <t xml:space="preserve">https://turystyka.wp.pl/kruszyniany-zobacz-jak-wyglada-najbardziej-tatarska-wies-w-polsce-6547891877926529v</t>
   </si>
   <si>
     <t xml:space="preserve">twojeip.wp.pl</t>
@@ -7688,6 +7700,9 @@
   </si>
   <si>
     <t xml:space="preserve">sfora.pl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fotoblogia.pl</t>
   </si>
   <si>
     <t xml:space="preserve">COVER </t>
@@ -8831,10 +8846,10 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A950" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B950" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A950" activeCellId="0" sqref="A950"/>
-      <selection pane="topRight" activeCell="D846" activeCellId="0" sqref="D846"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1013" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1013" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1013" activeCellId="0" sqref="A1013"/>
+      <selection pane="topRight" activeCell="D1019" activeCellId="0" sqref="D1019"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34004,7 +34019,9 @@
       <c r="C1018" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D1018" s="37"/>
+      <c r="D1018" s="37" t="s">
+        <v>2080</v>
+      </c>
       <c r="E1018" s="11" t="s">
         <v>207</v>
       </c>
@@ -35772,1362 +35789,1362 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>2080</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>2081</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>2082</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>2083</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>2084</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>2085</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>2086</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>2087</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>2088</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>2089</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
-        <v>2090</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
-        <v>2091</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
-        <v>2092</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
-        <v>2093</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>2094</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>2095</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>2084</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>2096</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>2097</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="s">
-        <v>2098</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="20" t="s">
-        <v>2099</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="20" t="s">
-        <v>2100</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="20" t="s">
-        <v>2101</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="20" t="s">
-        <v>2102</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="20" t="s">
-        <v>2103</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="20" t="s">
-        <v>2104</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="20" t="s">
-        <v>2105</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="20" t="s">
-        <v>2106</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="20" t="s">
-        <v>2107</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="20" t="s">
-        <v>2108</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="20" t="s">
-        <v>2109</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20" t="s">
-        <v>2110</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="20" t="s">
-        <v>2111</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="20" t="s">
-        <v>2112</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="20" t="s">
-        <v>2113</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="20" t="s">
-        <v>2114</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="20" t="s">
-        <v>2115</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="20" t="s">
-        <v>2116</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="20" t="s">
-        <v>2117</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="20" t="s">
-        <v>2118</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="20" t="s">
-        <v>2119</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="20" t="s">
-        <v>2120</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="20" t="s">
-        <v>2121</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="20" t="s">
-        <v>2122</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="20" t="s">
-        <v>2123</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="20" t="s">
-        <v>2124</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="20" t="s">
-        <v>2125</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="20" t="s">
-        <v>2126</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="20" t="s">
-        <v>2127</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="20" t="s">
-        <v>2128</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="20" t="s">
-        <v>2129</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="20" t="s">
-        <v>2130</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="20" t="s">
-        <v>2131</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="20" t="s">
-        <v>2132</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="20" t="s">
-        <v>2133</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="20" t="s">
-        <v>2134</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="20" t="s">
-        <v>2135</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="20" t="s">
-        <v>2136</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="20" t="s">
-        <v>2137</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="20" t="s">
-        <v>2138</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="20" t="s">
-        <v>2139</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="20" t="s">
-        <v>2140</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="20" t="s">
-        <v>2141</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="20" t="s">
-        <v>2142</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="20" t="s">
-        <v>2143</v>
+        <v>2144</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="20" t="s">
-        <v>2144</v>
+        <v>2145</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="20" t="s">
-        <v>2145</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="20" t="s">
-        <v>2146</v>
+        <v>2147</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="20" t="s">
-        <v>2147</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="20" t="s">
-        <v>2148</v>
+        <v>2149</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="20" t="s">
-        <v>2149</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="20" t="s">
-        <v>2150</v>
+        <v>2151</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="20" t="s">
-        <v>2151</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="20" t="s">
-        <v>2152</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="20" t="s">
-        <v>2153</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="20" t="s">
-        <v>2154</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="20" t="s">
-        <v>2155</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="20" t="s">
-        <v>2156</v>
+        <v>2157</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="20" t="s">
-        <v>2157</v>
+        <v>2158</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="20" t="s">
-        <v>2158</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="20" t="s">
-        <v>2159</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="20" t="s">
-        <v>2160</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="20" t="s">
-        <v>2161</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="20" t="s">
-        <v>2162</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="20" t="s">
-        <v>2163</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="20" t="s">
-        <v>2164</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="20" t="s">
-        <v>2165</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="20" t="s">
-        <v>2166</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="20" t="s">
-        <v>2167</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="20" t="s">
-        <v>2086</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="20" t="s">
-        <v>2168</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="20" t="s">
-        <v>2169</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="20" t="s">
-        <v>2170</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="20" t="s">
-        <v>2093</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="20" t="s">
-        <v>2171</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="20" t="s">
-        <v>2172</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="20" t="s">
-        <v>2173</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="20" t="s">
-        <v>2174</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="20" t="s">
-        <v>2175</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="20" t="s">
-        <v>2176</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="20" t="s">
-        <v>2177</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="20" t="s">
-        <v>2178</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="20" t="s">
-        <v>2179</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="20" t="s">
-        <v>2180</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="20" t="s">
-        <v>2181</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="20" t="s">
-        <v>2182</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="20" t="s">
-        <v>2183</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="20" t="s">
-        <v>2184</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="20" t="s">
-        <v>2185</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="20" t="s">
-        <v>2186</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="20" t="s">
-        <v>2187</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="20" t="s">
-        <v>2188</v>
+        <v>2189</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="20" t="s">
-        <v>2189</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="20" t="s">
-        <v>2190</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="20" t="s">
-        <v>2191</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="20" t="s">
-        <v>2192</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="20" t="s">
-        <v>2193</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="20" t="s">
-        <v>2194</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="20" t="s">
-        <v>2195</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="20" t="s">
-        <v>2196</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="20" t="s">
-        <v>2197</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="20" t="s">
-        <v>2198</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="20" t="s">
-        <v>2199</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="20" t="s">
-        <v>2200</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="20" t="s">
-        <v>2201</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="20" t="s">
-        <v>2202</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="20" t="s">
-        <v>2203</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="20" t="s">
-        <v>2204</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="20" t="s">
-        <v>2205</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="20" t="s">
-        <v>2206</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="20" t="s">
-        <v>2207</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="20" t="s">
-        <v>2208</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="20" t="s">
-        <v>2209</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="20" t="s">
-        <v>2210</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="20" t="s">
-        <v>2211</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="20" t="s">
-        <v>2212</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="20" t="s">
-        <v>2213</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="20" t="s">
-        <v>2214</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="20" t="s">
-        <v>2215</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="20" t="s">
-        <v>2216</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="20" t="s">
-        <v>2217</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="20" t="s">
-        <v>2218</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="20" t="s">
-        <v>2219</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="20" t="s">
-        <v>2220</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="20" t="s">
-        <v>2221</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="20" t="s">
-        <v>2222</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="20" t="s">
-        <v>2223</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="20" t="s">
-        <v>2224</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="20" t="s">
-        <v>2225</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="20" t="s">
-        <v>2226</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="20" t="s">
-        <v>2227</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="20" t="s">
-        <v>2228</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="20" t="s">
-        <v>2229</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="20" t="s">
-        <v>2230</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="20" t="s">
-        <v>2231</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="20" t="s">
-        <v>2232</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="20" t="s">
-        <v>2233</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="20" t="s">
-        <v>2234</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="20" t="s">
-        <v>2235</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="20" t="s">
-        <v>2236</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="20" t="s">
-        <v>2237</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="20" t="s">
-        <v>2238</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="20" t="s">
-        <v>2239</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="20" t="s">
-        <v>2240</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="20" t="s">
-        <v>2241</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="20" t="s">
-        <v>2242</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="20" t="s">
-        <v>2243</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="20" t="s">
-        <v>2244</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="20" t="s">
-        <v>2245</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="20" t="s">
-        <v>2246</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="20" t="s">
-        <v>2247</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="20" t="s">
-        <v>2248</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="20" t="s">
-        <v>2249</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="20" t="s">
-        <v>2250</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="20" t="s">
-        <v>2251</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="20" t="s">
-        <v>2252</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="20" t="s">
-        <v>2253</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="20" t="s">
-        <v>2254</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="20" t="s">
-        <v>2255</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="20" t="s">
-        <v>2256</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="20" t="s">
-        <v>2257</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="20" t="s">
-        <v>2258</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="20" t="s">
-        <v>2259</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="20" t="s">
-        <v>2260</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="20" t="s">
-        <v>2261</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="20" t="s">
-        <v>2262</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="20" t="s">
-        <v>2263</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="20" t="s">
-        <v>2264</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="20" t="s">
-        <v>2265</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="20" t="s">
-        <v>2266</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="20" t="s">
-        <v>2267</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="20" t="s">
-        <v>2268</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="20" t="s">
-        <v>2269</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="20" t="s">
-        <v>2270</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="20" t="s">
-        <v>2271</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="20" t="s">
-        <v>2272</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="20" t="s">
-        <v>2273</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="20" t="s">
-        <v>2081</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="20" t="s">
-        <v>2274</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="20" t="s">
-        <v>2275</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="20" t="s">
-        <v>2276</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="20" t="s">
-        <v>2277</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="20" t="s">
-        <v>2278</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="20" t="s">
-        <v>2279</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="20" t="s">
-        <v>2280</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="20" t="s">
-        <v>2281</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="20" t="s">
-        <v>2282</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="20" t="s">
-        <v>2283</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="20" t="s">
-        <v>2284</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="20" t="s">
-        <v>2285</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="20" t="s">
-        <v>2286</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="20" t="s">
-        <v>2287</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="20" t="s">
-        <v>2288</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="20" t="s">
-        <v>2289</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="20" t="s">
-        <v>2290</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="20" t="s">
-        <v>2291</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="20" t="s">
-        <v>2292</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="20" t="s">
-        <v>2293</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="20" t="s">
-        <v>2294</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="20" t="s">
-        <v>2295</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="20" t="s">
-        <v>2296</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="20" t="s">
-        <v>2297</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="20" t="s">
-        <v>2298</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="20" t="s">
-        <v>2299</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="20" t="s">
-        <v>2300</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="20" t="s">
-        <v>2301</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="20" t="s">
-        <v>2302</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="20" t="s">
-        <v>2303</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="20" t="s">
-        <v>2304</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="20" t="s">
-        <v>2305</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="20" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="20" t="s">
-        <v>2307</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="20" t="s">
-        <v>2308</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="20" t="s">
-        <v>2309</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="20" t="s">
-        <v>2310</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="20" t="s">
-        <v>2311</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="20" t="s">
-        <v>2312</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="20" t="s">
-        <v>2313</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="20" t="s">
-        <v>2314</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="20" t="s">
-        <v>2315</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="20" t="s">
-        <v>2316</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="20" t="s">
-        <v>2317</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="20" t="s">
-        <v>2318</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="20" t="s">
-        <v>2091</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="20" t="s">
-        <v>2319</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="20" t="s">
-        <v>2320</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="20" t="s">
-        <v>2321</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="20" t="s">
-        <v>2322</v>
+        <v>2323</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="20" t="s">
-        <v>2323</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="20" t="s">
-        <v>2324</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="20" t="s">
-        <v>2325</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="20" t="s">
-        <v>2326</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="20" t="s">
-        <v>2327</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="20" t="s">
-        <v>2328</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="20" t="s">
-        <v>2329</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="20" t="s">
-        <v>2330</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="20" t="s">
-        <v>2331</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="20" t="s">
-        <v>2332</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="20" t="s">
-        <v>2333</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="20" t="s">
-        <v>2334</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="20" t="s">
-        <v>2335</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="20" t="s">
-        <v>2336</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="20" t="s">
-        <v>2337</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="20" t="s">
-        <v>2338</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="20" t="s">
-        <v>2339</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="20" t="s">
-        <v>2340</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="20" t="s">
-        <v>2341</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="20" t="s">
-        <v>2342</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="20" t="s">
-        <v>2098</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="20" t="s">
-        <v>2343</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="20" t="s">
-        <v>2344</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="20" t="s">
-        <v>2345</v>
+        <v>2346</v>
       </c>
     </row>
   </sheetData>
@@ -37169,10 +37186,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>2346</v>
+        <v>2347</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>2347</v>
+        <v>2348</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>4</v>
@@ -37181,82 +37198,82 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>2348</v>
+        <v>2349</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>2349</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>2350</v>
+        <v>2351</v>
       </c>
       <c r="C2" s="41" t="n">
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>2351</v>
+        <v>2352</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>207</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="H2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10"/>
       <c r="B3" s="11" t="s">
-        <v>2353</v>
+        <v>2354</v>
       </c>
       <c r="C3" s="41" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>2351</v>
+        <v>2352</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>207</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
-        <v>2354</v>
+        <v>2355</v>
       </c>
       <c r="C4" s="41" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>2351</v>
+        <v>2352</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>207</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="H4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10"/>
       <c r="B5" s="27" t="s">
-        <v>2355</v>
+        <v>2356</v>
       </c>
       <c r="C5" s="41" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>2356</v>
+        <v>2357</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>207</v>
@@ -37268,13 +37285,13 @@
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="43" t="s">
-        <v>2357</v>
+        <v>2358</v>
       </c>
       <c r="C6" s="41" t="n">
         <v>0</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>2356</v>
+        <v>2357</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>207</v>
@@ -37286,7 +37303,7 @@
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
-        <v>2358</v>
+        <v>2359</v>
       </c>
       <c r="C7" s="41" t="n">
         <v>2</v>
@@ -37302,7 +37319,7 @@
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="8" t="s">
-        <v>2359</v>
+        <v>2360</v>
       </c>
       <c r="C8" s="41" t="n">
         <v>2</v>
@@ -37318,7 +37335,7 @@
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
-        <v>2360</v>
+        <v>2361</v>
       </c>
       <c r="C9" s="41" t="n">
         <v>2</v>
@@ -37334,7 +37351,7 @@
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="8" t="s">
-        <v>2361</v>
+        <v>2362</v>
       </c>
       <c r="C10" s="41" t="n">
         <v>2</v>
@@ -37350,7 +37367,7 @@
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
-        <v>2362</v>
+        <v>2363</v>
       </c>
       <c r="C11" s="41" t="n">
         <v>2</v>
@@ -37366,7 +37383,7 @@
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
       <c r="B12" s="8" t="s">
-        <v>2363</v>
+        <v>2364</v>
       </c>
       <c r="C12" s="41" t="n">
         <v>2</v>
@@ -37382,7 +37399,7 @@
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>2364</v>
+        <v>2365</v>
       </c>
       <c r="C13" s="41" t="n">
         <v>2</v>
@@ -37398,7 +37415,7 @@
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
       <c r="B14" s="8" t="s">
-        <v>2365</v>
+        <v>2366</v>
       </c>
       <c r="C14" s="41" t="n">
         <v>2</v>
@@ -37414,7 +37431,7 @@
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>2366</v>
+        <v>2367</v>
       </c>
       <c r="C15" s="41" t="n">
         <v>2</v>
@@ -37430,7 +37447,7 @@
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
       <c r="B16" s="8" t="s">
-        <v>2367</v>
+        <v>2368</v>
       </c>
       <c r="C16" s="41" t="n">
         <v>1</v>
@@ -37446,7 +37463,7 @@
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>2368</v>
+        <v>2369</v>
       </c>
       <c r="C17" s="41" t="n">
         <v>1.5</v>
@@ -37462,7 +37479,7 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
       <c r="B18" s="8" t="s">
-        <v>2369</v>
+        <v>2370</v>
       </c>
       <c r="C18" s="41" t="n">
         <v>2</v>
@@ -37478,7 +37495,7 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
-        <v>2370</v>
+        <v>2371</v>
       </c>
       <c r="C19" s="41" t="n">
         <v>2</v>
@@ -37494,13 +37511,13 @@
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7"/>
       <c r="B20" s="8" t="s">
-        <v>2371</v>
+        <v>2372</v>
       </c>
       <c r="C20" s="41" t="n">
         <v>2</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>2372</v>
+        <v>2373</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>207</v>
@@ -37512,7 +37529,7 @@
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>2373</v>
+        <v>2374</v>
       </c>
       <c r="C21" s="41" t="n">
         <v>2</v>
@@ -37528,7 +37545,7 @@
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7"/>
       <c r="B22" s="8" t="s">
-        <v>2374</v>
+        <v>2375</v>
       </c>
       <c r="C22" s="41" t="n">
         <v>2</v>
@@ -37544,7 +37561,7 @@
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
-        <v>2375</v>
+        <v>2376</v>
       </c>
       <c r="C23" s="41" t="n">
         <v>2</v>
@@ -37560,7 +37577,7 @@
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7"/>
       <c r="B24" s="8" t="s">
-        <v>2376</v>
+        <v>2377</v>
       </c>
       <c r="C24" s="41" t="n">
         <v>2</v>
@@ -37575,16 +37592,16 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>2377</v>
+        <v>2378</v>
       </c>
       <c r="C25" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>2378</v>
+        <v>2379</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>207</v>
@@ -37596,7 +37613,7 @@
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7"/>
       <c r="B26" s="8" t="s">
-        <v>2379</v>
+        <v>2380</v>
       </c>
       <c r="C26" s="41" t="n">
         <v>2</v>
@@ -37612,7 +37629,7 @@
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
-        <v>2380</v>
+        <v>2381</v>
       </c>
       <c r="C27" s="41" t="n">
         <v>2</v>
@@ -37628,7 +37645,7 @@
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
       <c r="B28" s="8" t="s">
-        <v>2381</v>
+        <v>2382</v>
       </c>
       <c r="C28" s="41" t="n">
         <v>1.5</v>
@@ -37644,7 +37661,7 @@
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
       <c r="B29" s="11" t="s">
-        <v>2382</v>
+        <v>2383</v>
       </c>
       <c r="C29" s="41" t="n">
         <v>2</v>
@@ -37660,7 +37677,7 @@
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
       <c r="B30" s="8" t="s">
-        <v>2383</v>
+        <v>2384</v>
       </c>
       <c r="C30" s="41" t="n">
         <v>2</v>
@@ -37676,7 +37693,7 @@
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
-        <v>2384</v>
+        <v>2385</v>
       </c>
       <c r="C31" s="41" t="n">
         <v>2</v>
@@ -37692,7 +37709,7 @@
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7"/>
       <c r="B32" s="8" t="s">
-        <v>2385</v>
+        <v>2386</v>
       </c>
       <c r="C32" s="41" t="n">
         <v>1.5</v>
@@ -37708,7 +37725,7 @@
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
-        <v>2386</v>
+        <v>2387</v>
       </c>
       <c r="C33" s="41" t="n">
         <v>2</v>
@@ -37724,7 +37741,7 @@
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7"/>
       <c r="B34" s="8" t="s">
-        <v>2387</v>
+        <v>2388</v>
       </c>
       <c r="C34" s="41" t="n">
         <v>1.5</v>
@@ -37740,7 +37757,7 @@
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
       <c r="B35" s="11" t="s">
-        <v>2388</v>
+        <v>2389</v>
       </c>
       <c r="C35" s="41" t="n">
         <v>2</v>
@@ -37756,7 +37773,7 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7"/>
       <c r="B36" s="8" t="s">
-        <v>2389</v>
+        <v>2390</v>
       </c>
       <c r="C36" s="41" t="n">
         <v>2</v>
@@ -37772,7 +37789,7 @@
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
       <c r="B37" s="11" t="s">
-        <v>2390</v>
+        <v>2391</v>
       </c>
       <c r="C37" s="41" t="n">
         <v>2</v>
@@ -37788,7 +37805,7 @@
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
-        <v>2391</v>
+        <v>2392</v>
       </c>
       <c r="C38" s="41" t="n">
         <v>2</v>
@@ -37803,16 +37820,16 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>2392</v>
+        <v>2393</v>
       </c>
       <c r="C39" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>2378</v>
+        <v>2379</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>207</v>
@@ -37823,7 +37840,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>1052</v>
@@ -37832,7 +37849,7 @@
         <v>3</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>2378</v>
+        <v>2379</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>207</v>
@@ -37843,16 +37860,16 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>2393</v>
+        <v>2394</v>
       </c>
       <c r="C41" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>2378</v>
+        <v>2379</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>207</v>
@@ -37863,16 +37880,16 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>2394</v>
+        <v>2395</v>
       </c>
       <c r="C42" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>2378</v>
+        <v>2379</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>207</v>
@@ -37883,16 +37900,16 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>2395</v>
+        <v>2396</v>
       </c>
       <c r="C43" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>2378</v>
+        <v>2379</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>207</v>
@@ -37903,16 +37920,16 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>2396</v>
+        <v>2397</v>
       </c>
       <c r="C44" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>2378</v>
+        <v>2379</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>207</v>
@@ -37923,16 +37940,16 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>2397</v>
+        <v>2398</v>
       </c>
       <c r="C45" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>2378</v>
+        <v>2379</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>207</v>
@@ -37943,16 +37960,16 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>2398</v>
+        <v>2399</v>
       </c>
       <c r="C46" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>2378</v>
+        <v>2379</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>207</v>
@@ -41071,19 +41088,19 @@
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="45"/>
       <c r="B1" s="46" t="s">
-        <v>2399</v>
+        <v>2400</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>2400</v>
+        <v>2401</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>2401</v>
+        <v>2402</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>2402</v>
+        <v>2403</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>2403</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41091,13 +41108,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>2404</v>
+        <v>2405</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>2405</v>
+        <v>2406</v>
       </c>
       <c r="E2" s="35"/>
       <c r="F2" s="49"/>
@@ -41107,13 +41124,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>2406</v>
+        <v>2407</v>
       </c>
       <c r="C3" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>2407</v>
+        <v>2408</v>
       </c>
       <c r="E3" s="51"/>
       <c r="F3" s="52"/>
@@ -41123,16 +41140,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>2408</v>
+        <v>2409</v>
       </c>
       <c r="C4" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>2409</v>
+        <v>2410</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>2410</v>
+        <v>2411</v>
       </c>
       <c r="F4" s="49"/>
     </row>
@@ -41141,19 +41158,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>2408</v>
+        <v>2409</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>2411</v>
+        <v>2412</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>2412</v>
+        <v>2413</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>2413</v>
+        <v>2414</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>2414</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41161,13 +41178,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>2415</v>
+        <v>2416</v>
       </c>
       <c r="C6" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>2416</v>
+        <v>2417</v>
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="49"/>
@@ -41177,17 +41194,17 @@
         <v>6</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>2417</v>
+        <v>2418</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>2418</v>
+        <v>2419</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>2419</v>
+        <v>2420</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="52" t="s">
-        <v>2420</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41195,13 +41212,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>2421</v>
+        <v>2422</v>
       </c>
       <c r="C8" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>2422</v>
+        <v>2423</v>
       </c>
       <c r="E8" s="35"/>
       <c r="F8" s="49"/>
@@ -41211,16 +41228,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>2404</v>
+        <v>2405</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>2411</v>
+        <v>2412</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>2423</v>
+        <v>2424</v>
       </c>
       <c r="E9" s="51" t="s">
-        <v>2424</v>
+        <v>2425</v>
       </c>
       <c r="F9" s="52"/>
     </row>
@@ -41229,18 +41246,18 @@
         <v>9</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>2425</v>
+        <v>2426</v>
       </c>
       <c r="C10" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>2426</v>
+        <v>2427</v>
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="49"/>
       <c r="G10" s="35" t="s">
-        <v>2427</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41248,13 +41265,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>2428</v>
+        <v>2429</v>
       </c>
       <c r="C11" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>2429</v>
+        <v>2430</v>
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="52"/>
@@ -41264,13 +41281,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="53" t="s">
-        <v>2430</v>
+        <v>2431</v>
       </c>
       <c r="C12" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>2431</v>
+        <v>2432</v>
       </c>
       <c r="E12" s="35"/>
       <c r="F12" s="49"/>
@@ -41280,13 +41297,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>2432</v>
+        <v>2433</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>2433</v>
+        <v>2434</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>2434</v>
+        <v>2435</v>
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="52"/>
@@ -41296,16 +41313,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>2432</v>
+        <v>2433</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>2435</v>
+        <v>2436</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>2436</v>
+        <v>2437</v>
       </c>
       <c r="F14" s="49"/>
     </row>
@@ -41314,16 +41331,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>2437</v>
+        <v>2438</v>
       </c>
       <c r="C15" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>2438</v>
+        <v>2439</v>
       </c>
       <c r="E15" s="51" t="s">
-        <v>2439</v>
+        <v>2440</v>
       </c>
       <c r="F15" s="52"/>
     </row>
@@ -41332,7 +41349,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>2437</v>
+        <v>2438</v>
       </c>
       <c r="C16" s="35" t="s">
         <v>1736</v>
@@ -41344,7 +41361,7 @@
         <v>1748</v>
       </c>
       <c r="F16" s="49" t="s">
-        <v>2440</v>
+        <v>2441</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41352,13 +41369,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>2441</v>
+        <v>2442</v>
       </c>
       <c r="C17" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>2442</v>
+        <v>2443</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="52"/>
@@ -41368,13 +41385,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>2443</v>
+        <v>2444</v>
       </c>
       <c r="C18" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>2444</v>
+        <v>2445</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="49"/>
@@ -41384,13 +41401,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>2443</v>
+        <v>2444</v>
       </c>
       <c r="C19" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>2445</v>
+        <v>2446</v>
       </c>
       <c r="E19" s="51"/>
       <c r="F19" s="52"/>
@@ -41400,13 +41417,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>2446</v>
+        <v>2447</v>
       </c>
       <c r="C20" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>2447</v>
+        <v>2448</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="49"/>
@@ -41416,16 +41433,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>2448</v>
+        <v>2449</v>
       </c>
       <c r="C21" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>2449</v>
+        <v>2450</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>2450</v>
+        <v>2451</v>
       </c>
       <c r="F21" s="52"/>
     </row>
@@ -41434,13 +41451,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>2448</v>
+        <v>2449</v>
       </c>
       <c r="C22" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>2451</v>
+        <v>2452</v>
       </c>
       <c r="E22" s="35"/>
       <c r="F22" s="49"/>
@@ -41450,13 +41467,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>2452</v>
+        <v>2453</v>
       </c>
       <c r="C23" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>2453</v>
+        <v>2454</v>
       </c>
       <c r="E23" s="51"/>
       <c r="F23" s="52"/>
@@ -41466,16 +41483,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>2454</v>
+        <v>2455</v>
       </c>
       <c r="C24" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>2455</v>
+        <v>2456</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>2456</v>
+        <v>2457</v>
       </c>
       <c r="F24" s="49"/>
     </row>
@@ -41484,13 +41501,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>2457</v>
+        <v>2458</v>
       </c>
       <c r="C25" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>2458</v>
+        <v>2459</v>
       </c>
       <c r="E25" s="51"/>
       <c r="F25" s="52"/>
@@ -41500,13 +41517,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>2459</v>
+        <v>2460</v>
       </c>
       <c r="C26" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>2460</v>
+        <v>2461</v>
       </c>
       <c r="E26" s="35"/>
       <c r="F26" s="49"/>
@@ -41516,13 +41533,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>2461</v>
+        <v>2462</v>
       </c>
       <c r="C27" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D27" s="51" t="s">
-        <v>2462</v>
+        <v>2463</v>
       </c>
       <c r="E27" s="51"/>
       <c r="F27" s="52"/>
@@ -41532,16 +41549,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>2463</v>
+        <v>2464</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>2433</v>
+        <v>2434</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>2464</v>
+        <v>2465</v>
       </c>
       <c r="E28" s="35" t="s">
-        <v>2465</v>
+        <v>2466</v>
       </c>
       <c r="F28" s="49"/>
     </row>
@@ -41550,13 +41567,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>2466</v>
+        <v>2467</v>
       </c>
       <c r="C29" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D29" s="51" t="s">
-        <v>2467</v>
+        <v>2468</v>
       </c>
       <c r="E29" s="51"/>
       <c r="F29" s="52"/>
@@ -41566,7 +41583,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>2468</v>
+        <v>2469</v>
       </c>
       <c r="C30" s="35"/>
       <c r="D30" s="35"/>
@@ -41578,7 +41595,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>2469</v>
+        <v>2470</v>
       </c>
       <c r="C31" s="51"/>
       <c r="D31" s="51"/>
@@ -41590,7 +41607,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>2470</v>
+        <v>2471</v>
       </c>
       <c r="C32" s="35"/>
       <c r="D32" s="35"/>
@@ -41602,7 +41619,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="51" t="s">
-        <v>2471</v>
+        <v>2472</v>
       </c>
       <c r="C33" s="51"/>
       <c r="D33" s="51"/>
@@ -41614,7 +41631,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>2472</v>
+        <v>2473</v>
       </c>
       <c r="C34" s="35"/>
       <c r="D34" s="35"/>
@@ -41626,7 +41643,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>2473</v>
+        <v>2474</v>
       </c>
       <c r="C35" s="51"/>
       <c r="D35" s="51"/>
@@ -41854,8 +41871,8 @@
   </sheetPr>
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E70" activeCellId="0" sqref="E70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -41874,19 +41891,19 @@
       <c r="A1" s="45"/>
       <c r="B1" s="46"/>
       <c r="C1" s="46" t="s">
-        <v>2399</v>
+        <v>2400</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>2400</v>
+        <v>2401</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>2401</v>
+        <v>2402</v>
       </c>
       <c r="F1" s="62" t="s">
-        <v>2402</v>
+        <v>2403</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>2403</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41898,10 +41915,10 @@
         <v>com</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>2474</v>
+        <v>2475</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E2" s="40"/>
       <c r="F2" s="64"/>
@@ -41916,10 +41933,10 @@
         <v>fm</v>
       </c>
       <c r="C3" s="53" t="s">
+        <v>2477</v>
+      </c>
+      <c r="D3" s="53" t="s">
         <v>2476</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>2475</v>
       </c>
       <c r="E3" s="53"/>
       <c r="F3" s="66"/>
@@ -41934,10 +41951,10 @@
         <v>money.pl</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>2477</v>
+        <v>2478</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E4" s="40"/>
       <c r="F4" s="64"/>
@@ -41952,10 +41969,10 @@
         <v>money.pl</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>2478</v>
+        <v>2479</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E5" s="53"/>
       <c r="F5" s="66"/>
@@ -41970,14 +41987,18 @@
         <v>money.pl</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>2479</v>
+        <v>2480</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>2475</v>
-      </c>
-      <c r="E6" s="40"/>
+        <v>2481</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>2482</v>
+      </c>
       <c r="F6" s="64"/>
-      <c r="G6" s="65"/>
+      <c r="G6" s="65" t="s">
+        <v>2483</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="50" t="n">
@@ -41988,10 +42009,10 @@
         <v>o2.pl</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>2480</v>
+        <v>2484</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E7" s="53"/>
       <c r="F7" s="66"/>
@@ -42006,15 +42027,17 @@
         <v>pl</v>
       </c>
       <c r="C8" s="40" t="s">
+        <v>2485</v>
+      </c>
+      <c r="D8" s="40" t="s">
         <v>2481</v>
       </c>
-      <c r="D8" s="40" t="s">
-        <v>2475</v>
-      </c>
       <c r="E8" s="40" t="s">
-        <v>1763</v>
-      </c>
-      <c r="F8" s="64"/>
+        <v>2486</v>
+      </c>
+      <c r="F8" s="64" t="s">
+        <v>2487</v>
+      </c>
       <c r="G8" s="65"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42026,10 +42049,10 @@
         <v>pl</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>2421</v>
+        <v>2422</v>
       </c>
       <c r="D9" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E9" s="53"/>
       <c r="F9" s="66"/>
@@ -42044,10 +42067,10 @@
         <v>pl</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>2482</v>
+        <v>2488</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="64"/>
@@ -42062,10 +42085,10 @@
         <v>pl</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>2483</v>
+        <v>2489</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E11" s="53"/>
       <c r="F11" s="66"/>
@@ -42080,10 +42103,10 @@
         <v>pl</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>2484</v>
+        <v>2490</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E12" s="40"/>
       <c r="F12" s="64"/>
@@ -42098,10 +42121,10 @@
         <v>pl</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>2485</v>
+        <v>2491</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E13" s="53"/>
       <c r="F13" s="66"/>
@@ -42116,13 +42139,13 @@
         <v>pl</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>2487</v>
+        <v>2493</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>2488</v>
+        <v>2494</v>
       </c>
       <c r="F14" s="64"/>
       <c r="G14" s="65"/>
@@ -42136,10 +42159,10 @@
         <v>pl</v>
       </c>
       <c r="C15" s="53" t="s">
-        <v>2489</v>
+        <v>2495</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E15" s="53"/>
       <c r="F15" s="66"/>
@@ -42154,17 +42177,13 @@
         <v>pl</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>2490</v>
+        <v>2496</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>2491</v>
-      </c>
-      <c r="E16" s="40" t="s">
-        <v>2492</v>
-      </c>
-      <c r="F16" s="64" t="s">
-        <v>2493</v>
-      </c>
+        <v>2476</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="64"/>
       <c r="G16" s="65"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42176,10 +42195,10 @@
         <v>pl</v>
       </c>
       <c r="C17" s="53" t="s">
-        <v>2494</v>
+        <v>2497</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E17" s="53"/>
       <c r="F17" s="66"/>
@@ -42191,13 +42210,13 @@
       </c>
       <c r="B18" s="40" t="str">
         <f aca="false">RIGHT(C18,LEN(C18)-FIND(".",C18))</f>
-        <v>pl</v>
+        <v>kafeteria.pl</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>2494</v>
+        <v>2498</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E18" s="40"/>
       <c r="F18" s="64"/>
@@ -42212,14 +42231,12 @@
         <v>pl</v>
       </c>
       <c r="C19" s="53" t="s">
-        <v>2428</v>
+        <v>2429</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>2475</v>
-      </c>
-      <c r="E19" s="53" t="s">
-        <v>2495</v>
-      </c>
+        <v>2476</v>
+      </c>
+      <c r="E19" s="53"/>
       <c r="F19" s="66"/>
       <c r="G19" s="67"/>
     </row>
@@ -42232,10 +42249,10 @@
         <v>pl</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>2496</v>
+        <v>2499</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E20" s="40"/>
       <c r="F20" s="64"/>
@@ -42250,10 +42267,10 @@
         <v>pl</v>
       </c>
       <c r="C21" s="53" t="s">
-        <v>2497</v>
+        <v>2500</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E21" s="53"/>
       <c r="F21" s="66"/>
@@ -42268,10 +42285,10 @@
         <v>pl</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>2498</v>
+        <v>2501</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="64"/>
@@ -42286,10 +42303,10 @@
         <v>pl</v>
       </c>
       <c r="C23" s="53" t="s">
-        <v>2499</v>
+        <v>2502</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E23" s="53"/>
       <c r="F23" s="66"/>
@@ -42304,10 +42321,10 @@
         <v>pl</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>2408</v>
+        <v>2409</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E24" s="40"/>
       <c r="F24" s="64"/>
@@ -42322,12 +42339,14 @@
         <v>pl</v>
       </c>
       <c r="C25" s="53" t="s">
-        <v>2500</v>
+        <v>2503</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>2475</v>
-      </c>
-      <c r="E25" s="53"/>
+        <v>2481</v>
+      </c>
+      <c r="E25" s="53" t="s">
+        <v>2504</v>
+      </c>
       <c r="F25" s="66"/>
       <c r="G25" s="67"/>
     </row>
@@ -42340,10 +42359,10 @@
         <v>pl</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>2501</v>
+        <v>2505</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E26" s="40"/>
       <c r="F26" s="64"/>
@@ -42358,10 +42377,10 @@
         <v>pl</v>
       </c>
       <c r="C27" s="53" t="s">
-        <v>2502</v>
+        <v>2506</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E27" s="53"/>
       <c r="F27" s="66"/>
@@ -42376,14 +42395,14 @@
         <v>pl</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>2417</v>
+        <v>2418</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>2503</v>
+        <v>2481</v>
       </c>
       <c r="E28" s="40"/>
       <c r="F28" s="64" t="s">
-        <v>2504</v>
+        <v>2507</v>
       </c>
       <c r="G28" s="65"/>
     </row>
@@ -42396,10 +42415,10 @@
         <v>pl</v>
       </c>
       <c r="C29" s="53" t="s">
-        <v>2505</v>
+        <v>2508</v>
       </c>
       <c r="D29" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E29" s="53"/>
       <c r="F29" s="66"/>
@@ -42414,10 +42433,10 @@
         <v>pl</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>2506</v>
+        <v>2509</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E30" s="40"/>
       <c r="F30" s="64"/>
@@ -42432,10 +42451,10 @@
         <v>pl</v>
       </c>
       <c r="C31" s="53" t="s">
-        <v>2507</v>
+        <v>2510</v>
       </c>
       <c r="D31" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E31" s="53"/>
       <c r="F31" s="66"/>
@@ -42450,10 +42469,10 @@
         <v>pl</v>
       </c>
       <c r="C32" s="40" t="s">
-        <v>2508</v>
+        <v>2511</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E32" s="40"/>
       <c r="F32" s="64"/>
@@ -42468,10 +42487,10 @@
         <v>pl</v>
       </c>
       <c r="C33" s="53" t="s">
-        <v>2509</v>
+        <v>2512</v>
       </c>
       <c r="D33" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E33" s="53"/>
       <c r="F33" s="66"/>
@@ -42486,10 +42505,10 @@
         <v>pl</v>
       </c>
       <c r="C34" s="68" t="s">
-        <v>2510</v>
+        <v>2513</v>
       </c>
       <c r="D34" s="68" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E34" s="68"/>
       <c r="F34" s="69"/>
@@ -42504,10 +42523,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C35" s="53" t="s">
-        <v>2511</v>
+        <v>2514</v>
       </c>
       <c r="D35" s="53" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E35" s="53"/>
       <c r="F35" s="66"/>
@@ -42522,10 +42541,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>2512</v>
+        <v>2515</v>
       </c>
       <c r="D36" s="40" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E36" s="40"/>
       <c r="F36" s="64"/>
@@ -42540,10 +42559,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C37" s="53" t="s">
-        <v>2513</v>
+        <v>2516</v>
       </c>
       <c r="D37" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E37" s="53"/>
       <c r="F37" s="66"/>
@@ -42558,10 +42577,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>2514</v>
+        <v>2517</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E38" s="40"/>
       <c r="F38" s="64"/>
@@ -42576,10 +42595,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C39" s="53" t="s">
-        <v>2515</v>
+        <v>2518</v>
       </c>
       <c r="D39" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E39" s="53"/>
       <c r="F39" s="66"/>
@@ -42594,10 +42613,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>2443</v>
+        <v>2444</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E40" s="40"/>
       <c r="F40" s="64"/>
@@ -42612,10 +42631,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>2516</v>
+        <v>2519</v>
       </c>
       <c r="D41" s="53" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E41" s="53"/>
       <c r="F41" s="66"/>
@@ -42630,10 +42649,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>2448</v>
+        <v>2449</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E42" s="40"/>
       <c r="F42" s="64"/>
@@ -42648,10 +42667,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>2432</v>
+        <v>2433</v>
       </c>
       <c r="D43" s="53" t="s">
-        <v>2475</v>
+        <v>2481</v>
       </c>
       <c r="E43" s="53"/>
       <c r="F43" s="66"/>
@@ -42666,10 +42685,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>2406</v>
+        <v>2407</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>2475</v>
+        <v>2481</v>
       </c>
       <c r="E44" s="40"/>
       <c r="F44" s="64"/>
@@ -42684,10 +42703,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C45" s="53" t="s">
-        <v>2517</v>
+        <v>2520</v>
       </c>
       <c r="D45" s="53" t="s">
-        <v>2503</v>
+        <v>2481</v>
       </c>
       <c r="E45" s="53"/>
       <c r="F45" s="66"/>
@@ -42702,10 +42721,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>2518</v>
+        <v>2521</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E46" s="40"/>
       <c r="F46" s="64"/>
@@ -42720,12 +42739,14 @@
         <v>wp.pl</v>
       </c>
       <c r="C47" s="53" t="s">
-        <v>2415</v>
+        <v>2416</v>
       </c>
       <c r="D47" s="53" t="s">
-        <v>2519</v>
-      </c>
-      <c r="E47" s="53"/>
+        <v>2481</v>
+      </c>
+      <c r="E47" s="53" t="s">
+        <v>2522</v>
+      </c>
       <c r="F47" s="66"/>
       <c r="G47" s="67"/>
     </row>
@@ -42738,10 +42759,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>2520</v>
+        <v>2523</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E48" s="40"/>
       <c r="F48" s="64"/>
@@ -42756,10 +42777,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C49" s="53" t="s">
-        <v>2454</v>
+        <v>2455</v>
       </c>
       <c r="D49" s="53" t="s">
-        <v>2519</v>
+        <v>2524</v>
       </c>
       <c r="E49" s="53"/>
       <c r="F49" s="66"/>
@@ -42774,10 +42795,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>2469</v>
+        <v>2470</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>2503</v>
+        <v>2481</v>
       </c>
       <c r="E50" s="40"/>
       <c r="F50" s="64"/>
@@ -42792,10 +42813,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C51" s="53" t="s">
-        <v>2457</v>
+        <v>2458</v>
       </c>
       <c r="D51" s="53" t="s">
-        <v>2475</v>
+        <v>2481</v>
       </c>
       <c r="E51" s="53"/>
       <c r="F51" s="66"/>
@@ -42810,10 +42831,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>2459</v>
+        <v>2460</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E52" s="40"/>
       <c r="F52" s="64"/>
@@ -42828,10 +42849,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C53" s="53" t="s">
-        <v>2521</v>
+        <v>2525</v>
       </c>
       <c r="D53" s="71" t="s">
-        <v>2522</v>
+        <v>2526</v>
       </c>
       <c r="E53" s="53"/>
       <c r="F53" s="66"/>
@@ -42846,10 +42867,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C54" s="40" t="s">
-        <v>2523</v>
+        <v>2527</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E54" s="40"/>
       <c r="F54" s="64"/>
@@ -42864,10 +42885,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C55" s="53" t="s">
-        <v>2468</v>
+        <v>2469</v>
       </c>
       <c r="D55" s="53" t="s">
-        <v>2503</v>
+        <v>2481</v>
       </c>
       <c r="E55" s="53"/>
       <c r="F55" s="66"/>
@@ -42882,10 +42903,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C56" s="40" t="s">
-        <v>2524</v>
+        <v>2528</v>
       </c>
       <c r="D56" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E56" s="40"/>
       <c r="F56" s="64"/>
@@ -42900,12 +42921,14 @@
         <v>wp.pl</v>
       </c>
       <c r="C57" s="53" t="s">
-        <v>2446</v>
+        <v>2447</v>
       </c>
       <c r="D57" s="53" t="s">
-        <v>2475</v>
-      </c>
-      <c r="E57" s="53"/>
+        <v>2481</v>
+      </c>
+      <c r="E57" s="53" t="s">
+        <v>2529</v>
+      </c>
       <c r="F57" s="66"/>
       <c r="G57" s="67"/>
     </row>
@@ -42918,10 +42941,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C58" s="40" t="s">
-        <v>2471</v>
+        <v>2472</v>
       </c>
       <c r="D58" s="40" t="s">
-        <v>2503</v>
+        <v>2481</v>
       </c>
       <c r="E58" s="40"/>
       <c r="F58" s="64"/>
@@ -42936,10 +42959,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C59" s="53" t="s">
-        <v>2525</v>
+        <v>2530</v>
       </c>
       <c r="D59" s="53" t="s">
-        <v>2526</v>
+        <v>2476</v>
       </c>
       <c r="E59" s="53"/>
       <c r="F59" s="66"/>
@@ -42954,10 +42977,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C60" s="40" t="s">
-        <v>2441</v>
+        <v>2442</v>
       </c>
       <c r="D60" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E60" s="40"/>
       <c r="F60" s="64"/>
@@ -42972,10 +42995,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C61" s="53" t="s">
-        <v>2527</v>
+        <v>2531</v>
       </c>
       <c r="D61" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E61" s="53"/>
       <c r="F61" s="66"/>
@@ -42990,10 +43013,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C62" s="40" t="s">
-        <v>2528</v>
+        <v>2532</v>
       </c>
       <c r="D62" s="40" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E62" s="40"/>
       <c r="F62" s="64"/>
@@ -43008,10 +43031,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C63" s="72" t="s">
-        <v>2529</v>
+        <v>2533</v>
       </c>
       <c r="D63" s="53" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E63" s="53"/>
       <c r="F63" s="66"/>
@@ -43026,10 +43049,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C64" s="40" t="s">
-        <v>2530</v>
+        <v>2534</v>
       </c>
       <c r="D64" s="40" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E64" s="40"/>
       <c r="F64" s="64"/>
@@ -43044,10 +43067,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C65" s="53" t="s">
-        <v>2404</v>
+        <v>2405</v>
       </c>
       <c r="D65" s="53" t="s">
-        <v>2475</v>
+        <v>2481</v>
       </c>
       <c r="E65" s="53"/>
       <c r="F65" s="66"/>
@@ -43062,10 +43085,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C66" s="40" t="s">
-        <v>2531</v>
+        <v>2535</v>
       </c>
       <c r="D66" s="40" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E66" s="40"/>
       <c r="F66" s="64"/>
@@ -43080,10 +43103,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C67" s="53" t="s">
-        <v>2466</v>
+        <v>2467</v>
       </c>
       <c r="D67" s="53" t="s">
-        <v>2503</v>
+        <v>2481</v>
       </c>
       <c r="E67" s="53"/>
       <c r="F67" s="66"/>
@@ -43098,10 +43121,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C68" s="40" t="s">
-        <v>2437</v>
+        <v>2438</v>
       </c>
       <c r="D68" s="40" t="s">
-        <v>2475</v>
+        <v>2481</v>
       </c>
       <c r="E68" s="40"/>
       <c r="F68" s="64"/>
@@ -43116,10 +43139,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C69" s="53" t="s">
-        <v>2532</v>
+        <v>2536</v>
       </c>
       <c r="D69" s="53" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E69" s="53"/>
       <c r="F69" s="66"/>
@@ -43134,12 +43157,14 @@
         <v>wp.pl</v>
       </c>
       <c r="C70" s="40" t="s">
-        <v>2461</v>
+        <v>2462</v>
       </c>
       <c r="D70" s="40" t="s">
-        <v>2533</v>
-      </c>
-      <c r="E70" s="40"/>
+        <v>2481</v>
+      </c>
+      <c r="E70" s="40" t="s">
+        <v>2537</v>
+      </c>
       <c r="F70" s="64"/>
       <c r="G70" s="65"/>
     </row>
@@ -43152,10 +43177,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C71" s="53" t="s">
-        <v>2472</v>
+        <v>2473</v>
       </c>
       <c r="D71" s="53" t="s">
-        <v>2503</v>
+        <v>2481</v>
       </c>
       <c r="E71" s="53"/>
       <c r="F71" s="66"/>
@@ -43170,10 +43195,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C72" s="40" t="s">
-        <v>2534</v>
+        <v>2538</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>2475</v>
+        <v>2481</v>
       </c>
       <c r="E72" s="40"/>
       <c r="F72" s="64"/>
@@ -43188,10 +43213,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C73" s="53" t="s">
-        <v>2535</v>
+        <v>2539</v>
       </c>
       <c r="D73" s="53" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E73" s="53"/>
       <c r="F73" s="66"/>
@@ -43206,10 +43231,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C74" s="40" t="s">
-        <v>2473</v>
+        <v>2474</v>
       </c>
       <c r="D74" s="40" t="s">
-        <v>2504</v>
+        <v>2481</v>
       </c>
       <c r="E74" s="40"/>
       <c r="F74" s="64"/>
@@ -43224,10 +43249,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C75" s="53" t="s">
-        <v>2430</v>
+        <v>2431</v>
       </c>
       <c r="D75" s="53" t="s">
-        <v>2475</v>
+        <v>2481</v>
       </c>
       <c r="E75" s="53"/>
       <c r="F75" s="66"/>
@@ -43242,10 +43267,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C76" s="40" t="s">
-        <v>2470</v>
+        <v>2471</v>
       </c>
       <c r="D76" s="40" t="s">
-        <v>2503</v>
+        <v>2481</v>
       </c>
       <c r="E76" s="40"/>
       <c r="F76" s="64"/>
@@ -43260,10 +43285,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C77" s="73" t="s">
-        <v>2536</v>
+        <v>2540</v>
       </c>
       <c r="D77" s="73" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E77" s="73"/>
       <c r="F77" s="74"/>
@@ -43275,10 +43300,10 @@
       </c>
       <c r="B78" s="40"/>
       <c r="C78" s="40" t="s">
-        <v>2452</v>
+        <v>2453</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E78" s="40"/>
       <c r="F78" s="64"/>
@@ -43290,10 +43315,10 @@
       </c>
       <c r="B79" s="53"/>
       <c r="C79" s="53" t="s">
-        <v>2537</v>
+        <v>2541</v>
       </c>
       <c r="D79" s="53" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E79" s="53"/>
       <c r="F79" s="66"/>
@@ -43305,10 +43330,10 @@
       </c>
       <c r="B80" s="40"/>
       <c r="C80" s="40" t="s">
-        <v>2538</v>
+        <v>2542</v>
       </c>
       <c r="D80" s="40" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E80" s="40"/>
       <c r="F80" s="64"/>
@@ -43320,10 +43345,10 @@
       </c>
       <c r="B81" s="53"/>
       <c r="C81" s="53" t="s">
-        <v>2539</v>
+        <v>2543</v>
       </c>
       <c r="D81" s="53" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E81" s="53"/>
       <c r="F81" s="66"/>
@@ -43335,10 +43360,10 @@
       </c>
       <c r="B82" s="40"/>
       <c r="C82" s="40" t="s">
-        <v>2540</v>
+        <v>2544</v>
       </c>
       <c r="D82" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E82" s="40"/>
       <c r="F82" s="64"/>
@@ -43350,13 +43375,13 @@
       </c>
       <c r="B83" s="53"/>
       <c r="C83" s="53" t="s">
-        <v>2541</v>
+        <v>2545</v>
       </c>
       <c r="D83" s="53" t="s">
-        <v>2486</v>
+        <v>2492</v>
       </c>
       <c r="E83" s="53" t="s">
-        <v>2542</v>
+        <v>2546</v>
       </c>
       <c r="F83" s="66"/>
       <c r="G83" s="67"/>
@@ -43367,10 +43392,10 @@
       </c>
       <c r="B84" s="53"/>
       <c r="C84" s="40" t="s">
-        <v>2543</v>
+        <v>2547</v>
       </c>
       <c r="D84" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E84" s="40"/>
       <c r="F84" s="64"/>
@@ -43382,13 +43407,13 @@
       </c>
       <c r="B85" s="53"/>
       <c r="C85" s="53" t="s">
-        <v>2544</v>
+        <v>2548</v>
       </c>
       <c r="D85" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E85" s="53" t="s">
-        <v>2542</v>
+        <v>2546</v>
       </c>
       <c r="F85" s="66"/>
       <c r="G85" s="67"/>
@@ -43399,10 +43424,10 @@
       </c>
       <c r="B86" s="53"/>
       <c r="C86" s="40" t="s">
-        <v>2545</v>
+        <v>2549</v>
       </c>
       <c r="D86" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E86" s="40"/>
       <c r="F86" s="64"/>
@@ -43414,10 +43439,10 @@
       </c>
       <c r="B87" s="53"/>
       <c r="C87" s="53" t="s">
-        <v>2546</v>
+        <v>2550</v>
       </c>
       <c r="D87" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E87" s="53"/>
       <c r="F87" s="66"/>
@@ -43429,10 +43454,10 @@
       </c>
       <c r="B88" s="53"/>
       <c r="C88" s="53" t="s">
-        <v>2547</v>
+        <v>2551</v>
       </c>
       <c r="D88" s="53" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E88" s="53"/>
       <c r="F88" s="64"/>
@@ -43444,10 +43469,10 @@
       </c>
       <c r="B89" s="53"/>
       <c r="C89" s="40" t="s">
-        <v>2548</v>
+        <v>2552</v>
       </c>
       <c r="D89" s="40" t="s">
-        <v>2475</v>
+        <v>2476</v>
       </c>
       <c r="E89" s="40"/>
       <c r="F89" s="66"/>
@@ -43458,8 +43483,12 @@
         <v>89</v>
       </c>
       <c r="B90" s="53"/>
-      <c r="C90" s="40"/>
-      <c r="D90" s="40"/>
+      <c r="C90" s="40" t="s">
+        <v>2553</v>
+      </c>
+      <c r="D90" s="40" t="s">
+        <v>2476</v>
+      </c>
       <c r="E90" s="40"/>
       <c r="F90" s="64"/>
       <c r="G90" s="65"/>
@@ -43587,19 +43616,19 @@
       <c r="A102" s="76"/>
       <c r="B102" s="77"/>
       <c r="C102" s="78" t="s">
-        <v>2549</v>
+        <v>2554</v>
       </c>
       <c r="D102" s="79" t="n">
         <f aca="false">(COUNTIF(D2:D101,"OK")+COUNTIF(D2:D101,"NO ADS BY DEFAULT"))/COUNTIF(D2:D101,"*")</f>
-        <v>0.852272727272727</v>
+        <v>0.741573033707865</v>
       </c>
       <c r="E102" s="80"/>
       <c r="F102" s="78" t="s">
-        <v>2550</v>
+        <v>2555</v>
       </c>
       <c r="G102" s="79" t="n">
         <f aca="false">(COUNTIF(D2:D101,"ADVERT")+COUNTIF(D2:D101,"Anti-adblock"))/COUNTIF(D2:D101,"*")</f>
-        <v>0.0909090909090909</v>
+        <v>0.247191011235955</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 5 new filters
</commit_message>
<xml_diff>
--- a/pull-requests/filters.xlsx
+++ b/pull-requests/filters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6501" uniqueCount="2635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6516" uniqueCount="2649">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -6494,6 +6494,48 @@
   </si>
   <si>
     <t xml:space="preserve">633</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smart-test.pl##.banneritem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://smart-test.pl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">634</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slonskyradio.eu###ruchomeReklamy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://slonskyradio.eu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slonskyradio.eu###n2-ss-4-align</t>
+  </si>
+  <si>
+    <t xml:space="preserve">635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sochaczewianin.pl##.td-a-rec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sochaczewianin.pl/2020/09/zmiany-w-rokladzie-na-prosbe-pasazerow/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">636</t>
+  </si>
+  <si>
+    <t xml:space="preserve">||softonet.pl^*^mobik%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://softonet.pl/publikacje/poradniki/Pizza.Hut.z.opcja.zamawiania.jedzenia.przez.Messengera,1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637</t>
+  </si>
+  <si>
+    <t xml:space="preserve">||speedtest.pl^*^play7^$subdocument</t>
   </si>
   <si>
     <t xml:space="preserve">Domain</t>
@@ -9086,7 +9128,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1023" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1023" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1023" activeCellId="0" sqref="A1023"/>
-      <selection pane="topRight" activeCell="C1048" activeCellId="0" sqref="C1048"/>
+      <selection pane="topRight" activeCell="G1049" activeCellId="0" sqref="G1049"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34798,7 +34840,7 @@
       </c>
       <c r="F1044" s="27"/>
       <c r="G1044" s="11" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="H1044" s="8"/>
     </row>
@@ -34820,7 +34862,7 @@
       </c>
       <c r="F1045" s="11"/>
       <c r="G1045" s="11" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="H1045" s="11"/>
     </row>
@@ -34842,7 +34884,7 @@
       </c>
       <c r="F1046" s="27"/>
       <c r="G1046" s="11" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="H1046" s="8"/>
     </row>
@@ -34864,7 +34906,7 @@
       </c>
       <c r="F1047" s="11"/>
       <c r="G1047" s="11" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="H1047" s="11"/>
     </row>
@@ -34886,7 +34928,7 @@
       </c>
       <c r="F1048" s="27"/>
       <c r="G1048" s="11" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="H1048" s="8"/>
     </row>
@@ -34894,13 +34936,17 @@
       <c r="A1049" s="10" t="s">
         <v>2150</v>
       </c>
-      <c r="B1049" s="11"/>
+      <c r="B1049" s="11" t="s">
+        <v>2151</v>
+      </c>
       <c r="C1049" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D1049" s="11"/>
+      <c r="D1049" s="11" t="s">
+        <v>2152</v>
+      </c>
       <c r="E1049" s="11" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="F1049" s="11"/>
       <c r="G1049" s="11" t="s">
@@ -34909,13 +34955,20 @@
       <c r="H1049" s="11"/>
     </row>
     <row r="1050" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1050" s="40"/>
+      <c r="A1050" s="1" t="s">
+        <v>2153</v>
+      </c>
+      <c r="B1050" s="40" t="s">
+        <v>2154</v>
+      </c>
       <c r="C1050" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D1050" s="37"/>
+      <c r="D1050" s="39" t="s">
+        <v>2155</v>
+      </c>
       <c r="E1050" s="11" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="F1050" s="27"/>
       <c r="G1050" s="11" t="s">
@@ -34925,13 +34978,15 @@
     </row>
     <row r="1051" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1051" s="10"/>
-      <c r="B1051" s="11"/>
+      <c r="B1051" s="11" t="s">
+        <v>2156</v>
+      </c>
       <c r="C1051" s="11" t="s">
         <v>27</v>
       </c>
       <c r="D1051" s="11"/>
       <c r="E1051" s="11" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="F1051" s="11"/>
       <c r="G1051" s="11" t="s">
@@ -34940,13 +34995,20 @@
       <c r="H1051" s="11"/>
     </row>
     <row r="1052" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1052" s="40"/>
+      <c r="A1052" s="1" t="s">
+        <v>2157</v>
+      </c>
+      <c r="B1052" s="40" t="s">
+        <v>2158</v>
+      </c>
       <c r="C1052" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D1052" s="37"/>
+      <c r="D1052" s="39" t="s">
+        <v>2159</v>
+      </c>
       <c r="E1052" s="11" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="F1052" s="27"/>
       <c r="G1052" s="11" t="s">
@@ -34955,14 +35017,20 @@
       <c r="H1052" s="8"/>
     </row>
     <row r="1053" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1053" s="10"/>
-      <c r="B1053" s="11"/>
+      <c r="A1053" s="10" t="s">
+        <v>2160</v>
+      </c>
+      <c r="B1053" s="11" t="s">
+        <v>2161</v>
+      </c>
       <c r="C1053" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D1053" s="11"/>
+      <c r="D1053" s="11" t="s">
+        <v>2162</v>
+      </c>
       <c r="E1053" s="11" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="F1053" s="11"/>
       <c r="G1053" s="11" t="s">
@@ -34971,13 +35039,20 @@
       <c r="H1053" s="11"/>
     </row>
     <row r="1054" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1054" s="40"/>
+      <c r="A1054" s="1" t="s">
+        <v>2163</v>
+      </c>
+      <c r="B1054" s="40" t="s">
+        <v>2164</v>
+      </c>
       <c r="C1054" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D1054" s="37"/>
+      <c r="D1054" s="39" t="s">
+        <v>1277</v>
+      </c>
       <c r="E1054" s="11" t="s">
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="F1054" s="27"/>
       <c r="G1054" s="11" t="s">
@@ -36145,6 +36220,11 @@
     <hyperlink ref="D1046" r:id="rId283" display="https://f1.dziel-pasje.pl/F1_news-31280-Stella_Sainz_i_Norris_maja_pewne_cechy_wspolne_z_Schumacherem_czy_Alonso.html"/>
     <hyperlink ref="D1047" r:id="rId284" display="http://biegowki.pl/forum/index.php"/>
     <hyperlink ref="D1048" r:id="rId285" display="https://sklep-muzyczny.com.pl"/>
+    <hyperlink ref="D1049" r:id="rId286" display="http://smart-test.pl"/>
+    <hyperlink ref="D1050" r:id="rId287" display="https://slonskyradio.eu"/>
+    <hyperlink ref="D1052" r:id="rId288" display="https://sochaczewianin.pl/2020/09/zmiany-w-rokladzie-na-prosbe-pasazerow/"/>
+    <hyperlink ref="D1053" r:id="rId289" display="https://softonet.pl/publikacje/poradniki/Pizza.Hut.z.opcja.zamawiania.jedzenia.przez.Messengera,1992"/>
+    <hyperlink ref="D1054" r:id="rId290" display="https://www.speedtest.pl"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -36154,7 +36234,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId286"/>
+    <tablePart r:id="rId291"/>
   </tableParts>
 </worksheet>
 </file>
@@ -36177,1362 +36257,1362 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>2151</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>2152</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="20" t="s">
-        <v>2153</v>
+        <v>2167</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
-        <v>2154</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20" t="s">
-        <v>2155</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20" t="s">
-        <v>2156</v>
+        <v>2170</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="20" t="s">
-        <v>2157</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>2158</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>2159</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="20" t="s">
-        <v>2160</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
-        <v>2161</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20" t="s">
-        <v>2162</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
-        <v>2163</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
-        <v>2164</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="s">
-        <v>2165</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="s">
-        <v>2166</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>2155</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>2167</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>2168</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="s">
-        <v>2169</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="20" t="s">
-        <v>2170</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="20" t="s">
-        <v>2171</v>
+        <v>2185</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="20" t="s">
-        <v>2172</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="20" t="s">
-        <v>2173</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="20" t="s">
-        <v>2174</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="20" t="s">
-        <v>2175</v>
+        <v>2189</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="20" t="s">
-        <v>2176</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="20" t="s">
-        <v>2177</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="20" t="s">
-        <v>2178</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="20" t="s">
-        <v>2179</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="20" t="s">
-        <v>2180</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20" t="s">
-        <v>2181</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="20" t="s">
-        <v>2182</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="20" t="s">
-        <v>2183</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="20" t="s">
-        <v>2184</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="20" t="s">
-        <v>2185</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="20" t="s">
-        <v>2186</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="20" t="s">
-        <v>2187</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="20" t="s">
-        <v>2188</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="20" t="s">
-        <v>2189</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="20" t="s">
-        <v>2190</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="20" t="s">
-        <v>2191</v>
+        <v>2205</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="20" t="s">
-        <v>2192</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="20" t="s">
-        <v>2193</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="20" t="s">
-        <v>2194</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="20" t="s">
-        <v>2195</v>
+        <v>2209</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="20" t="s">
-        <v>2196</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="20" t="s">
-        <v>2197</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="20" t="s">
-        <v>2198</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="20" t="s">
-        <v>2199</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="20" t="s">
-        <v>2200</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="20" t="s">
-        <v>2201</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="20" t="s">
-        <v>2202</v>
+        <v>2216</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="20" t="s">
-        <v>2203</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="20" t="s">
-        <v>2204</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="20" t="s">
-        <v>2205</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="20" t="s">
-        <v>2206</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="20" t="s">
-        <v>2207</v>
+        <v>2221</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="20" t="s">
-        <v>2208</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="20" t="s">
-        <v>2209</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="20" t="s">
-        <v>2210</v>
+        <v>2224</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="20" t="s">
-        <v>2211</v>
+        <v>2225</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="20" t="s">
-        <v>2212</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="20" t="s">
-        <v>2213</v>
+        <v>2227</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="20" t="s">
-        <v>2214</v>
+        <v>2228</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="20" t="s">
-        <v>2215</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="20" t="s">
-        <v>2216</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="20" t="s">
-        <v>2217</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="20" t="s">
-        <v>2218</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="20" t="s">
-        <v>2219</v>
+        <v>2233</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="20" t="s">
-        <v>2220</v>
+        <v>2234</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="20" t="s">
-        <v>2221</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="20" t="s">
-        <v>2222</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="20" t="s">
-        <v>2223</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="20" t="s">
-        <v>2224</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="20" t="s">
-        <v>2225</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="20" t="s">
-        <v>2226</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="20" t="s">
-        <v>2227</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="20" t="s">
-        <v>2228</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="20" t="s">
-        <v>2229</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="20" t="s">
-        <v>2230</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="20" t="s">
-        <v>2231</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="20" t="s">
-        <v>2232</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="20" t="s">
-        <v>2233</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="20" t="s">
-        <v>2234</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="20" t="s">
-        <v>2235</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="20" t="s">
-        <v>2236</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="20" t="s">
-        <v>2237</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="20" t="s">
-        <v>2238</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="20" t="s">
-        <v>2157</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="20" t="s">
-        <v>2239</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="20" t="s">
-        <v>2240</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="20" t="s">
-        <v>2241</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="20" t="s">
-        <v>2164</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="20" t="s">
-        <v>2242</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="20" t="s">
-        <v>2243</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="20" t="s">
-        <v>2244</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="20" t="s">
-        <v>2245</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="20" t="s">
-        <v>2246</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="20" t="s">
-        <v>2247</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="20" t="s">
-        <v>2248</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="20" t="s">
-        <v>2249</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="20" t="s">
-        <v>2250</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="20" t="s">
-        <v>2251</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="20" t="s">
-        <v>2252</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="20" t="s">
-        <v>2253</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="20" t="s">
-        <v>2254</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="20" t="s">
-        <v>2255</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="20" t="s">
-        <v>2256</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="20" t="s">
-        <v>2257</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="20" t="s">
-        <v>2258</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="20" t="s">
-        <v>2259</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="20" t="s">
-        <v>2260</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="20" t="s">
-        <v>2261</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="20" t="s">
-        <v>2262</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="20" t="s">
-        <v>2263</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="20" t="s">
-        <v>2264</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="20" t="s">
-        <v>2265</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="20" t="s">
-        <v>2266</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="20" t="s">
-        <v>2267</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="20" t="s">
-        <v>2268</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="20" t="s">
-        <v>2269</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="20" t="s">
-        <v>2270</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="20" t="s">
-        <v>2271</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="20" t="s">
-        <v>2272</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="20" t="s">
-        <v>2273</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="20" t="s">
-        <v>2274</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="20" t="s">
-        <v>2275</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="20" t="s">
-        <v>2276</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="20" t="s">
-        <v>2277</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="20" t="s">
-        <v>2278</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="20" t="s">
-        <v>2279</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="20" t="s">
-        <v>2280</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="20" t="s">
-        <v>2281</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="20" t="s">
-        <v>2282</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="20" t="s">
-        <v>2283</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="20" t="s">
-        <v>2284</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="20" t="s">
-        <v>2285</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="20" t="s">
-        <v>2286</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="20" t="s">
-        <v>2287</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="20" t="s">
-        <v>2288</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="20" t="s">
-        <v>2289</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="20" t="s">
-        <v>2290</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="20" t="s">
-        <v>2291</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="20" t="s">
-        <v>2292</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="20" t="s">
-        <v>2293</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="20" t="s">
-        <v>2294</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="20" t="s">
-        <v>2295</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="20" t="s">
-        <v>2296</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="20" t="s">
-        <v>2297</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="20" t="s">
-        <v>2298</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="20" t="s">
-        <v>2299</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="20" t="s">
-        <v>2300</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="20" t="s">
-        <v>2301</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="20" t="s">
-        <v>2302</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="20" t="s">
-        <v>2303</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="20" t="s">
-        <v>2304</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="20" t="s">
-        <v>2305</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="20" t="s">
-        <v>2306</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="20" t="s">
-        <v>2307</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="20" t="s">
-        <v>2308</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="20" t="s">
-        <v>2309</v>
+        <v>2323</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="20" t="s">
-        <v>2310</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="20" t="s">
-        <v>2311</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="20" t="s">
-        <v>2312</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="20" t="s">
-        <v>2313</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="20" t="s">
-        <v>2314</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="20" t="s">
-        <v>2315</v>
+        <v>2329</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="20" t="s">
-        <v>2316</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="20" t="s">
-        <v>2317</v>
+        <v>2331</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="20" t="s">
-        <v>2318</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="20" t="s">
-        <v>2319</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="20" t="s">
-        <v>2320</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="20" t="s">
-        <v>2321</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="20" t="s">
-        <v>2322</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="20" t="s">
-        <v>2323</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="20" t="s">
-        <v>2324</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="20" t="s">
-        <v>2325</v>
+        <v>2339</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="20" t="s">
-        <v>2326</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="20" t="s">
-        <v>2327</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="20" t="s">
-        <v>2328</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="20" t="s">
-        <v>2329</v>
+        <v>2343</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="20" t="s">
-        <v>2330</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="20" t="s">
-        <v>2331</v>
+        <v>2345</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="20" t="s">
-        <v>2332</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="20" t="s">
-        <v>2333</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="20" t="s">
-        <v>2334</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="20" t="s">
-        <v>2335</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="20" t="s">
-        <v>2336</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="20" t="s">
-        <v>2337</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="20" t="s">
-        <v>2338</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="20" t="s">
-        <v>2339</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="20" t="s">
-        <v>2340</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="20" t="s">
-        <v>2341</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="20" t="s">
-        <v>2342</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="20" t="s">
-        <v>2343</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="20" t="s">
-        <v>2344</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="20" t="s">
-        <v>2152</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="20" t="s">
-        <v>2345</v>
+        <v>2359</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="20" t="s">
-        <v>2346</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="20" t="s">
-        <v>2347</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="20" t="s">
-        <v>2348</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="20" t="s">
-        <v>2349</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="20" t="s">
-        <v>2350</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="20" t="s">
-        <v>2351</v>
+        <v>2365</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="20" t="s">
-        <v>2352</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="20" t="s">
-        <v>2353</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="20" t="s">
-        <v>2354</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="20" t="s">
-        <v>2355</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="20" t="s">
-        <v>2356</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="20" t="s">
-        <v>2357</v>
+        <v>2371</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="20" t="s">
-        <v>2358</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="20" t="s">
-        <v>2359</v>
+        <v>2373</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="20" t="s">
-        <v>2360</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="20" t="s">
-        <v>2361</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="20" t="s">
-        <v>2362</v>
+        <v>2376</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="20" t="s">
-        <v>2363</v>
+        <v>2377</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="20" t="s">
-        <v>2364</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="20" t="s">
-        <v>2365</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="20" t="s">
-        <v>2366</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="20" t="s">
-        <v>2367</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="20" t="s">
-        <v>2368</v>
+        <v>2382</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="20" t="s">
-        <v>2369</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="20" t="s">
-        <v>2370</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="20" t="s">
-        <v>2371</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="20" t="s">
-        <v>2372</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="20" t="s">
-        <v>2373</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="20" t="s">
-        <v>2374</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="20" t="s">
-        <v>2375</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="20" t="s">
-        <v>2376</v>
+        <v>2390</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="20" t="s">
-        <v>2377</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="20" t="s">
-        <v>2378</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="20" t="s">
-        <v>2379</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="20" t="s">
-        <v>2380</v>
+        <v>2394</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="20" t="s">
-        <v>2381</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="20" t="s">
-        <v>2382</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="20" t="s">
-        <v>2383</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="20" t="s">
-        <v>2384</v>
+        <v>2398</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="20" t="s">
-        <v>2385</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="20" t="s">
-        <v>2386</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="20" t="s">
-        <v>2387</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="20" t="s">
-        <v>2388</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="20" t="s">
-        <v>2389</v>
+        <v>2403</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="20" t="s">
-        <v>2162</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="20" t="s">
-        <v>2390</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="20" t="s">
-        <v>2391</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="20" t="s">
-        <v>2392</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="20" t="s">
-        <v>2393</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="20" t="s">
-        <v>2394</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="20" t="s">
-        <v>2395</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="20" t="s">
-        <v>2396</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="20" t="s">
-        <v>2397</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="20" t="s">
-        <v>2398</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="20" t="s">
-        <v>2399</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="20" t="s">
-        <v>2400</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="20" t="s">
-        <v>2401</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="20" t="s">
-        <v>2402</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="20" t="s">
-        <v>2403</v>
+        <v>2417</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="20" t="s">
-        <v>2404</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="20" t="s">
-        <v>2405</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="20" t="s">
-        <v>2406</v>
+        <v>2420</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="20" t="s">
-        <v>2407</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="20" t="s">
-        <v>2408</v>
+        <v>2422</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="20" t="s">
-        <v>2409</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="20" t="s">
-        <v>2410</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="20" t="s">
-        <v>2411</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="20" t="s">
-        <v>2412</v>
+        <v>2426</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="20" t="s">
-        <v>2413</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="20" t="s">
-        <v>2169</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="20" t="s">
-        <v>2414</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="20" t="s">
-        <v>2415</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="20" t="s">
-        <v>2416</v>
+        <v>2430</v>
       </c>
     </row>
   </sheetData>
@@ -37574,10 +37654,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>2417</v>
+        <v>2431</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>2418</v>
+        <v>2432</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>4</v>
@@ -37586,82 +37666,82 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>2419</v>
+        <v>2433</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>2420</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>2421</v>
+        <v>2435</v>
       </c>
       <c r="C2" s="41" t="n">
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>2422</v>
+        <v>2436</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>207</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
-        <v>2423</v>
+        <v>2437</v>
       </c>
       <c r="H2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10"/>
       <c r="B3" s="11" t="s">
-        <v>2424</v>
+        <v>2438</v>
       </c>
       <c r="C3" s="41" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>2422</v>
+        <v>2436</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>207</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="11" t="s">
-        <v>2423</v>
+        <v>2437</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
-        <v>2425</v>
+        <v>2439</v>
       </c>
       <c r="C4" s="41" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>2422</v>
+        <v>2436</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>207</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8" t="s">
-        <v>2423</v>
+        <v>2437</v>
       </c>
       <c r="H4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10"/>
       <c r="B5" s="27" t="s">
-        <v>2426</v>
+        <v>2440</v>
       </c>
       <c r="C5" s="41" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>2427</v>
+        <v>2441</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>207</v>
@@ -37673,13 +37753,13 @@
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="43" t="s">
-        <v>2428</v>
+        <v>2442</v>
       </c>
       <c r="C6" s="41" t="n">
         <v>0</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>2427</v>
+        <v>2441</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>207</v>
@@ -37691,7 +37771,7 @@
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
-        <v>2429</v>
+        <v>2443</v>
       </c>
       <c r="C7" s="41" t="n">
         <v>2</v>
@@ -37707,7 +37787,7 @@
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
       <c r="B8" s="8" t="s">
-        <v>2430</v>
+        <v>2444</v>
       </c>
       <c r="C8" s="41" t="n">
         <v>2</v>
@@ -37723,7 +37803,7 @@
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
-        <v>2431</v>
+        <v>2445</v>
       </c>
       <c r="C9" s="41" t="n">
         <v>2</v>
@@ -37739,7 +37819,7 @@
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
       <c r="B10" s="8" t="s">
-        <v>2432</v>
+        <v>2446</v>
       </c>
       <c r="C10" s="41" t="n">
         <v>2</v>
@@ -37755,7 +37835,7 @@
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
-        <v>2433</v>
+        <v>2447</v>
       </c>
       <c r="C11" s="41" t="n">
         <v>2</v>
@@ -37771,7 +37851,7 @@
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
       <c r="B12" s="8" t="s">
-        <v>2434</v>
+        <v>2448</v>
       </c>
       <c r="C12" s="41" t="n">
         <v>2</v>
@@ -37787,7 +37867,7 @@
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>2435</v>
+        <v>2449</v>
       </c>
       <c r="C13" s="41" t="n">
         <v>2</v>
@@ -37803,7 +37883,7 @@
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
       <c r="B14" s="8" t="s">
-        <v>2436</v>
+        <v>2450</v>
       </c>
       <c r="C14" s="41" t="n">
         <v>2</v>
@@ -37819,7 +37899,7 @@
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
-        <v>2437</v>
+        <v>2451</v>
       </c>
       <c r="C15" s="41" t="n">
         <v>2</v>
@@ -37835,7 +37915,7 @@
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
       <c r="B16" s="8" t="s">
-        <v>2438</v>
+        <v>2452</v>
       </c>
       <c r="C16" s="41" t="n">
         <v>1</v>
@@ -37851,7 +37931,7 @@
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>2439</v>
+        <v>2453</v>
       </c>
       <c r="C17" s="41" t="n">
         <v>1.5</v>
@@ -37867,7 +37947,7 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
       <c r="B18" s="8" t="s">
-        <v>2440</v>
+        <v>2454</v>
       </c>
       <c r="C18" s="41" t="n">
         <v>2</v>
@@ -37883,7 +37963,7 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
-        <v>2441</v>
+        <v>2455</v>
       </c>
       <c r="C19" s="41" t="n">
         <v>2</v>
@@ -37899,7 +37979,7 @@
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7"/>
       <c r="B20" s="8" t="s">
-        <v>2442</v>
+        <v>2456</v>
       </c>
       <c r="C20" s="41" t="n">
         <v>2</v>
@@ -37917,7 +37997,7 @@
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>2443</v>
+        <v>2457</v>
       </c>
       <c r="C21" s="41" t="n">
         <v>2</v>
@@ -37933,7 +38013,7 @@
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7"/>
       <c r="B22" s="8" t="s">
-        <v>2444</v>
+        <v>2458</v>
       </c>
       <c r="C22" s="41" t="n">
         <v>2</v>
@@ -37949,7 +38029,7 @@
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
-        <v>2445</v>
+        <v>2459</v>
       </c>
       <c r="C23" s="41" t="n">
         <v>2</v>
@@ -37965,7 +38045,7 @@
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7"/>
       <c r="B24" s="8" t="s">
-        <v>2446</v>
+        <v>2460</v>
       </c>
       <c r="C24" s="41" t="n">
         <v>2</v>
@@ -37980,16 +38060,16 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>2423</v>
+        <v>2437</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>2447</v>
+        <v>2461</v>
       </c>
       <c r="C25" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>2448</v>
+        <v>2462</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>207</v>
@@ -38001,7 +38081,7 @@
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7"/>
       <c r="B26" s="8" t="s">
-        <v>2449</v>
+        <v>2463</v>
       </c>
       <c r="C26" s="41" t="n">
         <v>2</v>
@@ -38017,7 +38097,7 @@
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
-        <v>2450</v>
+        <v>2464</v>
       </c>
       <c r="C27" s="41" t="n">
         <v>2</v>
@@ -38033,7 +38113,7 @@
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
       <c r="B28" s="8" t="s">
-        <v>2451</v>
+        <v>2465</v>
       </c>
       <c r="C28" s="41" t="n">
         <v>1.5</v>
@@ -38049,7 +38129,7 @@
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
       <c r="B29" s="11" t="s">
-        <v>2452</v>
+        <v>2466</v>
       </c>
       <c r="C29" s="41" t="n">
         <v>2</v>
@@ -38065,7 +38145,7 @@
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7"/>
       <c r="B30" s="8" t="s">
-        <v>2453</v>
+        <v>2467</v>
       </c>
       <c r="C30" s="41" t="n">
         <v>2</v>
@@ -38081,7 +38161,7 @@
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
-        <v>2454</v>
+        <v>2468</v>
       </c>
       <c r="C31" s="41" t="n">
         <v>2</v>
@@ -38097,7 +38177,7 @@
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7"/>
       <c r="B32" s="8" t="s">
-        <v>2455</v>
+        <v>2469</v>
       </c>
       <c r="C32" s="41" t="n">
         <v>1.5</v>
@@ -38113,7 +38193,7 @@
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
-        <v>2456</v>
+        <v>2470</v>
       </c>
       <c r="C33" s="41" t="n">
         <v>2</v>
@@ -38129,7 +38209,7 @@
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7"/>
       <c r="B34" s="8" t="s">
-        <v>2457</v>
+        <v>2471</v>
       </c>
       <c r="C34" s="41" t="n">
         <v>1.5</v>
@@ -38145,7 +38225,7 @@
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
       <c r="B35" s="11" t="s">
-        <v>2458</v>
+        <v>2472</v>
       </c>
       <c r="C35" s="41" t="n">
         <v>2</v>
@@ -38161,7 +38241,7 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7"/>
       <c r="B36" s="8" t="s">
-        <v>2459</v>
+        <v>2473</v>
       </c>
       <c r="C36" s="41" t="n">
         <v>2</v>
@@ -38177,7 +38257,7 @@
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
       <c r="B37" s="11" t="s">
-        <v>2460</v>
+        <v>2474</v>
       </c>
       <c r="C37" s="41" t="n">
         <v>2</v>
@@ -38193,7 +38273,7 @@
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
-        <v>2461</v>
+        <v>2475</v>
       </c>
       <c r="C38" s="41" t="n">
         <v>2</v>
@@ -38208,16 +38288,16 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>2423</v>
+        <v>2437</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>2462</v>
+        <v>2476</v>
       </c>
       <c r="C39" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>2448</v>
+        <v>2462</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>207</v>
@@ -38228,7 +38308,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>2423</v>
+        <v>2437</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>1052</v>
@@ -38237,7 +38317,7 @@
         <v>3</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>2448</v>
+        <v>2462</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>207</v>
@@ -38248,16 +38328,16 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>2423</v>
+        <v>2437</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>2463</v>
+        <v>2477</v>
       </c>
       <c r="C41" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>2448</v>
+        <v>2462</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>207</v>
@@ -38268,16 +38348,16 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>2423</v>
+        <v>2437</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>2464</v>
+        <v>2478</v>
       </c>
       <c r="C42" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>2448</v>
+        <v>2462</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>207</v>
@@ -38288,16 +38368,16 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>2423</v>
+        <v>2437</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>2465</v>
+        <v>2479</v>
       </c>
       <c r="C43" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>2448</v>
+        <v>2462</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>207</v>
@@ -38308,16 +38388,16 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>2423</v>
+        <v>2437</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>2466</v>
+        <v>2480</v>
       </c>
       <c r="C44" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>2448</v>
+        <v>2462</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>207</v>
@@ -38328,16 +38408,16 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>2423</v>
+        <v>2437</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>2467</v>
+        <v>2481</v>
       </c>
       <c r="C45" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>2448</v>
+        <v>2462</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>207</v>
@@ -38348,16 +38428,16 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
-        <v>2423</v>
+        <v>2437</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>2468</v>
+        <v>2482</v>
       </c>
       <c r="C46" s="41" t="n">
         <v>3</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>2448</v>
+        <v>2462</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>207</v>
@@ -38433,7 +38513,7 @@
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10"/>
       <c r="B51" s="11" t="s">
-        <v>2469</v>
+        <v>2483</v>
       </c>
       <c r="C51" s="41" t="n">
         <v>2</v>
@@ -41422,19 +41502,19 @@
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="45"/>
       <c r="B1" s="46" t="s">
-        <v>2470</v>
+        <v>2484</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>2471</v>
+        <v>2485</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>2472</v>
+        <v>2486</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>2473</v>
+        <v>2487</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>2474</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41442,13 +41522,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>2475</v>
+        <v>2489</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>2476</v>
+        <v>2490</v>
       </c>
       <c r="E2" s="35"/>
       <c r="F2" s="49"/>
@@ -41458,13 +41538,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>2477</v>
+        <v>2491</v>
       </c>
       <c r="C3" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>2478</v>
+        <v>2492</v>
       </c>
       <c r="E3" s="51"/>
       <c r="F3" s="52"/>
@@ -41474,16 +41554,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>2479</v>
+        <v>2493</v>
       </c>
       <c r="C4" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>2480</v>
+        <v>2494</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>2481</v>
+        <v>2495</v>
       </c>
       <c r="F4" s="49"/>
     </row>
@@ -41492,19 +41572,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>2479</v>
+        <v>2493</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>2482</v>
+        <v>2496</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>2483</v>
+        <v>2497</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>2484</v>
+        <v>2498</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>2485</v>
+        <v>2499</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41512,13 +41592,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>2486</v>
+        <v>2500</v>
       </c>
       <c r="C6" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>2487</v>
+        <v>2501</v>
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="49"/>
@@ -41528,17 +41608,17 @@
         <v>6</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>2488</v>
+        <v>2502</v>
       </c>
       <c r="C7" s="51" t="s">
-        <v>2489</v>
+        <v>2503</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>2490</v>
+        <v>2504</v>
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="52" t="s">
-        <v>2491</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41546,13 +41626,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>2492</v>
+        <v>2506</v>
       </c>
       <c r="C8" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>2493</v>
+        <v>2507</v>
       </c>
       <c r="E8" s="35"/>
       <c r="F8" s="49"/>
@@ -41562,16 +41642,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>2475</v>
+        <v>2489</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>2482</v>
+        <v>2496</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>2494</v>
+        <v>2508</v>
       </c>
       <c r="E9" s="51" t="s">
-        <v>2495</v>
+        <v>2509</v>
       </c>
       <c r="F9" s="52"/>
     </row>
@@ -41580,18 +41660,18 @@
         <v>9</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>2496</v>
+        <v>2510</v>
       </c>
       <c r="C10" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>2497</v>
+        <v>2511</v>
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="49"/>
       <c r="G10" s="35" t="s">
-        <v>2498</v>
+        <v>2512</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41599,13 +41679,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>2499</v>
+        <v>2513</v>
       </c>
       <c r="C11" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>2500</v>
+        <v>2514</v>
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="52"/>
@@ -41615,13 +41695,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="53" t="s">
-        <v>2501</v>
+        <v>2515</v>
       </c>
       <c r="C12" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>2502</v>
+        <v>2516</v>
       </c>
       <c r="E12" s="35"/>
       <c r="F12" s="49"/>
@@ -41631,13 +41711,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>2503</v>
+        <v>2517</v>
       </c>
       <c r="C13" s="51" t="s">
-        <v>2504</v>
+        <v>2518</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>2505</v>
+        <v>2519</v>
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="52"/>
@@ -41647,16 +41727,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>2503</v>
+        <v>2517</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>2506</v>
+        <v>2520</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>2507</v>
+        <v>2521</v>
       </c>
       <c r="F14" s="49"/>
     </row>
@@ -41665,16 +41745,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>2508</v>
+        <v>2522</v>
       </c>
       <c r="C15" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>2509</v>
+        <v>2523</v>
       </c>
       <c r="E15" s="51" t="s">
-        <v>2510</v>
+        <v>2524</v>
       </c>
       <c r="F15" s="52"/>
     </row>
@@ -41683,7 +41763,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>2508</v>
+        <v>2522</v>
       </c>
       <c r="C16" s="35" t="s">
         <v>1736</v>
@@ -41695,7 +41775,7 @@
         <v>1748</v>
       </c>
       <c r="F16" s="49" t="s">
-        <v>2511</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -41703,13 +41783,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>2512</v>
+        <v>2526</v>
       </c>
       <c r="C17" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>2513</v>
+        <v>2527</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="52"/>
@@ -41719,13 +41799,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>2514</v>
+        <v>2528</v>
       </c>
       <c r="C18" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>2515</v>
+        <v>2529</v>
       </c>
       <c r="E18" s="35"/>
       <c r="F18" s="49"/>
@@ -41735,13 +41815,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>2514</v>
+        <v>2528</v>
       </c>
       <c r="C19" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>2516</v>
+        <v>2530</v>
       </c>
       <c r="E19" s="51"/>
       <c r="F19" s="52"/>
@@ -41751,13 +41831,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>2517</v>
+        <v>2531</v>
       </c>
       <c r="C20" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>2518</v>
+        <v>2532</v>
       </c>
       <c r="E20" s="35"/>
       <c r="F20" s="49"/>
@@ -41767,16 +41847,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>2519</v>
+        <v>2533</v>
       </c>
       <c r="C21" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>2520</v>
+        <v>2534</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>2521</v>
+        <v>2535</v>
       </c>
       <c r="F21" s="52"/>
     </row>
@@ -41785,13 +41865,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>2519</v>
+        <v>2533</v>
       </c>
       <c r="C22" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>2522</v>
+        <v>2536</v>
       </c>
       <c r="E22" s="35"/>
       <c r="F22" s="49"/>
@@ -41801,13 +41881,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>2523</v>
+        <v>2537</v>
       </c>
       <c r="C23" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>2524</v>
+        <v>2538</v>
       </c>
       <c r="E23" s="51"/>
       <c r="F23" s="52"/>
@@ -41817,16 +41897,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>2525</v>
+        <v>2539</v>
       </c>
       <c r="C24" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>2526</v>
+        <v>2540</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>2527</v>
+        <v>2541</v>
       </c>
       <c r="F24" s="49"/>
     </row>
@@ -41835,13 +41915,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>2528</v>
+        <v>2542</v>
       </c>
       <c r="C25" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D25" s="51" t="s">
-        <v>2529</v>
+        <v>2543</v>
       </c>
       <c r="E25" s="51"/>
       <c r="F25" s="52"/>
@@ -41851,13 +41931,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>2530</v>
+        <v>2544</v>
       </c>
       <c r="C26" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>2531</v>
+        <v>2545</v>
       </c>
       <c r="E26" s="35"/>
       <c r="F26" s="49"/>
@@ -41867,13 +41947,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>2532</v>
+        <v>2546</v>
       </c>
       <c r="C27" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D27" s="51" t="s">
-        <v>2533</v>
+        <v>2547</v>
       </c>
       <c r="E27" s="51"/>
       <c r="F27" s="52"/>
@@ -41883,16 +41963,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>2534</v>
+        <v>2548</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>2504</v>
+        <v>2518</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>2535</v>
+        <v>2549</v>
       </c>
       <c r="E28" s="35" t="s">
-        <v>2536</v>
+        <v>2550</v>
       </c>
       <c r="F28" s="49"/>
     </row>
@@ -41901,13 +41981,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>2537</v>
+        <v>2551</v>
       </c>
       <c r="C29" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D29" s="51" t="s">
-        <v>2538</v>
+        <v>2552</v>
       </c>
       <c r="E29" s="51"/>
       <c r="F29" s="52"/>
@@ -41917,7 +41997,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>2539</v>
+        <v>2553</v>
       </c>
       <c r="C30" s="35" t="s">
         <v>1736</v>
@@ -41931,7 +42011,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>2540</v>
+        <v>2554</v>
       </c>
       <c r="C31" s="51" t="s">
         <v>1736</v>
@@ -41945,7 +42025,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>2541</v>
+        <v>2555</v>
       </c>
       <c r="C32" s="35"/>
       <c r="D32" s="35"/>
@@ -41957,7 +42037,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="51" t="s">
-        <v>2542</v>
+        <v>2556</v>
       </c>
       <c r="C33" s="51"/>
       <c r="D33" s="51"/>
@@ -41969,7 +42049,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>2543</v>
+        <v>2557</v>
       </c>
       <c r="C34" s="35"/>
       <c r="D34" s="35"/>
@@ -41981,7 +42061,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>2544</v>
+        <v>2558</v>
       </c>
       <c r="C35" s="51"/>
       <c r="D35" s="51"/>
@@ -41993,13 +42073,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>2545</v>
+        <v>2559</v>
       </c>
       <c r="C36" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>2546</v>
+        <v>2560</v>
       </c>
       <c r="E36" s="35"/>
       <c r="F36" s="49"/>
@@ -42009,7 +42089,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="51" t="s">
-        <v>2547</v>
+        <v>2561</v>
       </c>
       <c r="C37" s="51" t="s">
         <v>1736</v>
@@ -42023,13 +42103,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>2477</v>
+        <v>2491</v>
       </c>
       <c r="C38" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>2548</v>
+        <v>2562</v>
       </c>
       <c r="E38" s="35"/>
       <c r="F38" s="49"/>
@@ -42039,7 +42119,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="51" t="s">
-        <v>2539</v>
+        <v>2553</v>
       </c>
       <c r="C39" s="51" t="s">
         <v>1736</v>
@@ -42053,13 +42133,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="35" t="s">
-        <v>2540</v>
+        <v>2554</v>
       </c>
       <c r="C40" s="35" t="s">
-        <v>2504</v>
+        <v>2518</v>
       </c>
       <c r="D40" s="35" t="s">
-        <v>2549</v>
+        <v>2563</v>
       </c>
       <c r="E40" s="35"/>
       <c r="F40" s="49"/>
@@ -42069,10 +42149,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="51" t="s">
-        <v>2550</v>
+        <v>2564</v>
       </c>
       <c r="C41" s="51" t="s">
-        <v>2504</v>
+        <v>2518</v>
       </c>
       <c r="D41" s="51"/>
       <c r="E41" s="51"/>
@@ -42083,13 +42163,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>2551</v>
+        <v>2565</v>
       </c>
       <c r="C42" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>2552</v>
+        <v>2566</v>
       </c>
       <c r="E42" s="35"/>
       <c r="F42" s="49"/>
@@ -42099,13 +42179,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="51" t="s">
-        <v>2553</v>
+        <v>2567</v>
       </c>
       <c r="C43" s="51" t="s">
         <v>1736</v>
       </c>
       <c r="D43" s="51" t="s">
-        <v>2554</v>
+        <v>2568</v>
       </c>
       <c r="E43" s="51"/>
       <c r="F43" s="52"/>
@@ -42115,13 +42195,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>2541</v>
+        <v>2555</v>
       </c>
       <c r="C44" s="35" t="s">
-        <v>2504</v>
+        <v>2518</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>2555</v>
+        <v>2569</v>
       </c>
       <c r="E44" s="35"/>
       <c r="F44" s="49"/>
@@ -42277,19 +42357,19 @@
       <c r="A1" s="45"/>
       <c r="B1" s="46"/>
       <c r="C1" s="46" t="s">
-        <v>2470</v>
+        <v>2484</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>2471</v>
+        <v>2485</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>2472</v>
+        <v>2486</v>
       </c>
       <c r="F1" s="62" t="s">
-        <v>2473</v>
+        <v>2487</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>2474</v>
+        <v>2488</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42301,10 +42381,10 @@
         <v>com</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>2556</v>
+        <v>2570</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E2" s="40"/>
       <c r="F2" s="64"/>
@@ -42319,10 +42399,10 @@
         <v>fm</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>2558</v>
+        <v>2572</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E3" s="53"/>
       <c r="F3" s="66"/>
@@ -42337,10 +42417,10 @@
         <v>money.pl</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>2559</v>
+        <v>2573</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E4" s="40"/>
       <c r="F4" s="64"/>
@@ -42355,10 +42435,10 @@
         <v>money.pl</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>2560</v>
+        <v>2574</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E5" s="53"/>
       <c r="F5" s="66"/>
@@ -42373,17 +42453,17 @@
         <v>money.pl</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>2561</v>
+        <v>2575</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>2562</v>
+        <v>2576</v>
       </c>
       <c r="F6" s="64"/>
       <c r="G6" s="65" t="s">
-        <v>2563</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42395,10 +42475,10 @@
         <v>o2.pl</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>2564</v>
+        <v>2578</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E7" s="53"/>
       <c r="F7" s="66"/>
@@ -42413,16 +42493,16 @@
         <v>pl</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>2565</v>
+        <v>2579</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>2567</v>
+        <v>2581</v>
       </c>
       <c r="F8" s="64" t="s">
-        <v>2568</v>
+        <v>2582</v>
       </c>
       <c r="G8" s="65"/>
     </row>
@@ -42435,10 +42515,10 @@
         <v>pl</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>2492</v>
+        <v>2506</v>
       </c>
       <c r="D9" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E9" s="53"/>
       <c r="F9" s="66"/>
@@ -42453,10 +42533,10 @@
         <v>pl</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>2569</v>
+        <v>2583</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E10" s="40"/>
       <c r="F10" s="64"/>
@@ -42471,10 +42551,10 @@
         <v>com</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>2570</v>
+        <v>2584</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E11" s="53"/>
       <c r="F11" s="66"/>
@@ -42489,10 +42569,10 @@
         <v>pl</v>
       </c>
       <c r="C12" s="40" t="s">
+        <v>2585</v>
+      </c>
+      <c r="D12" s="40" t="s">
         <v>2571</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>2557</v>
       </c>
       <c r="E12" s="40"/>
       <c r="F12" s="64"/>
@@ -42507,10 +42587,10 @@
         <v>pl</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>2572</v>
+        <v>2586</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E13" s="53"/>
       <c r="F13" s="66"/>
@@ -42525,13 +42605,13 @@
         <v>pl</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>2574</v>
+        <v>2588</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>2575</v>
+        <v>2589</v>
       </c>
       <c r="F14" s="64"/>
       <c r="G14" s="65"/>
@@ -42545,10 +42625,10 @@
         <v>pl</v>
       </c>
       <c r="C15" s="53" t="s">
-        <v>2576</v>
+        <v>2590</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E15" s="53"/>
       <c r="F15" s="66"/>
@@ -42563,10 +42643,10 @@
         <v>pl</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>2577</v>
+        <v>2591</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E16" s="40"/>
       <c r="F16" s="64"/>
@@ -42581,10 +42661,10 @@
         <v>pl</v>
       </c>
       <c r="C17" s="53" t="s">
-        <v>2578</v>
+        <v>2592</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E17" s="53"/>
       <c r="F17" s="66"/>
@@ -42599,10 +42679,10 @@
         <v>kafeteria.pl</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>2579</v>
+        <v>2593</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E18" s="40"/>
       <c r="F18" s="64"/>
@@ -42617,10 +42697,10 @@
         <v>pl</v>
       </c>
       <c r="C19" s="53" t="s">
-        <v>2499</v>
+        <v>2513</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E19" s="53"/>
       <c r="F19" s="66"/>
@@ -42635,10 +42715,10 @@
         <v>pl</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>2580</v>
+        <v>2594</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E20" s="40"/>
       <c r="F20" s="64"/>
@@ -42653,10 +42733,10 @@
         <v>pl</v>
       </c>
       <c r="C21" s="53" t="s">
-        <v>2581</v>
+        <v>2595</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E21" s="53"/>
       <c r="F21" s="66"/>
@@ -42671,10 +42751,10 @@
         <v>pl</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>2582</v>
+        <v>2596</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E22" s="40"/>
       <c r="F22" s="64"/>
@@ -42689,10 +42769,10 @@
         <v>pl</v>
       </c>
       <c r="C23" s="53" t="s">
-        <v>2583</v>
+        <v>2597</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E23" s="53"/>
       <c r="F23" s="66"/>
@@ -42707,10 +42787,10 @@
         <v>pl</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>2479</v>
+        <v>2493</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E24" s="40"/>
       <c r="F24" s="64"/>
@@ -42725,13 +42805,13 @@
         <v>pl</v>
       </c>
       <c r="C25" s="53" t="s">
-        <v>2553</v>
+        <v>2567</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>2584</v>
+        <v>2598</v>
       </c>
       <c r="E25" s="53" t="s">
-        <v>2585</v>
+        <v>2599</v>
       </c>
       <c r="F25" s="66"/>
       <c r="G25" s="67"/>
@@ -42745,10 +42825,10 @@
         <v>pl</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>2586</v>
+        <v>2600</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E26" s="40"/>
       <c r="F26" s="64"/>
@@ -42763,10 +42843,10 @@
         <v>pl</v>
       </c>
       <c r="C27" s="53" t="s">
-        <v>2587</v>
+        <v>2601</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E27" s="53"/>
       <c r="F27" s="66"/>
@@ -42781,14 +42861,14 @@
         <v>pl</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>2488</v>
+        <v>2502</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E28" s="40"/>
       <c r="F28" s="64" t="s">
-        <v>2588</v>
+        <v>2602</v>
       </c>
       <c r="G28" s="65"/>
     </row>
@@ -42801,10 +42881,10 @@
         <v>pl</v>
       </c>
       <c r="C29" s="53" t="s">
-        <v>2589</v>
+        <v>2603</v>
       </c>
       <c r="D29" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E29" s="53"/>
       <c r="F29" s="66"/>
@@ -42819,10 +42899,10 @@
         <v>pl</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>2590</v>
+        <v>2604</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E30" s="40"/>
       <c r="F30" s="64"/>
@@ -42837,10 +42917,10 @@
         <v>pl</v>
       </c>
       <c r="C31" s="53" t="s">
-        <v>2591</v>
+        <v>2605</v>
       </c>
       <c r="D31" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E31" s="53"/>
       <c r="F31" s="66"/>
@@ -42855,10 +42935,10 @@
         <v>pl</v>
       </c>
       <c r="C32" s="40" t="s">
-        <v>2592</v>
+        <v>2606</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E32" s="40"/>
       <c r="F32" s="64"/>
@@ -42873,10 +42953,10 @@
         <v>pl</v>
       </c>
       <c r="C33" s="53" t="s">
-        <v>2593</v>
+        <v>2607</v>
       </c>
       <c r="D33" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E33" s="53"/>
       <c r="F33" s="66"/>
@@ -42891,10 +42971,10 @@
         <v>pl</v>
       </c>
       <c r="C34" s="68" t="s">
-        <v>2594</v>
+        <v>2608</v>
       </c>
       <c r="D34" s="68" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E34" s="68"/>
       <c r="F34" s="69"/>
@@ -42909,10 +42989,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C35" s="53" t="s">
-        <v>2595</v>
+        <v>2609</v>
       </c>
       <c r="D35" s="53" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E35" s="53"/>
       <c r="F35" s="66"/>
@@ -42927,10 +43007,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>2596</v>
+        <v>2610</v>
       </c>
       <c r="D36" s="40" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E36" s="40"/>
       <c r="F36" s="64"/>
@@ -42945,10 +43025,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C37" s="53" t="s">
-        <v>2597</v>
+        <v>2611</v>
       </c>
       <c r="D37" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E37" s="53"/>
       <c r="F37" s="66"/>
@@ -42963,10 +43043,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>2598</v>
+        <v>2612</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E38" s="40"/>
       <c r="F38" s="64"/>
@@ -42981,10 +43061,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C39" s="53" t="s">
-        <v>2599</v>
+        <v>2613</v>
       </c>
       <c r="D39" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E39" s="53"/>
       <c r="F39" s="66"/>
@@ -42999,10 +43079,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>2514</v>
+        <v>2528</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E40" s="40"/>
       <c r="F40" s="64"/>
@@ -43017,10 +43097,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>2600</v>
+        <v>2614</v>
       </c>
       <c r="D41" s="53" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E41" s="53"/>
       <c r="F41" s="66"/>
@@ -43035,10 +43115,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>2519</v>
+        <v>2533</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E42" s="40"/>
       <c r="F42" s="64"/>
@@ -43053,10 +43133,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>2503</v>
+        <v>2517</v>
       </c>
       <c r="D43" s="53" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E43" s="53"/>
       <c r="F43" s="66"/>
@@ -43071,13 +43151,13 @@
         <v>wp.pl</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>2477</v>
+        <v>2491</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>2584</v>
+        <v>2598</v>
       </c>
       <c r="E44" s="40" t="s">
-        <v>2601</v>
+        <v>2615</v>
       </c>
       <c r="F44" s="64"/>
       <c r="G44" s="65"/>
@@ -43091,10 +43171,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C45" s="53" t="s">
-        <v>2550</v>
+        <v>2564</v>
       </c>
       <c r="D45" s="53" t="s">
-        <v>2584</v>
+        <v>2598</v>
       </c>
       <c r="E45" s="53"/>
       <c r="F45" s="66"/>
@@ -43109,10 +43189,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>2602</v>
+        <v>2616</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E46" s="40"/>
       <c r="F46" s="64"/>
@@ -43127,13 +43207,13 @@
         <v>wp.pl</v>
       </c>
       <c r="C47" s="53" t="s">
-        <v>2486</v>
+        <v>2500</v>
       </c>
       <c r="D47" s="53" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E47" s="53" t="s">
-        <v>2603</v>
+        <v>2617</v>
       </c>
       <c r="F47" s="66"/>
       <c r="G47" s="67"/>
@@ -43147,10 +43227,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>2604</v>
+        <v>2618</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E48" s="40"/>
       <c r="F48" s="64"/>
@@ -43165,10 +43245,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C49" s="53" t="s">
-        <v>2525</v>
+        <v>2539</v>
       </c>
       <c r="D49" s="53" t="s">
-        <v>2605</v>
+        <v>2619</v>
       </c>
       <c r="E49" s="53"/>
       <c r="F49" s="66"/>
@@ -43183,10 +43263,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>2540</v>
+        <v>2554</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>2584</v>
+        <v>2598</v>
       </c>
       <c r="E50" s="40"/>
       <c r="F50" s="64"/>
@@ -43201,10 +43281,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C51" s="53" t="s">
-        <v>2528</v>
+        <v>2542</v>
       </c>
       <c r="D51" s="53" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E51" s="53"/>
       <c r="F51" s="66"/>
@@ -43219,10 +43299,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>2530</v>
+        <v>2544</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E52" s="40"/>
       <c r="F52" s="64"/>
@@ -43237,10 +43317,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C53" s="53" t="s">
-        <v>2606</v>
+        <v>2620</v>
       </c>
       <c r="D53" s="71" t="s">
-        <v>2607</v>
+        <v>2621</v>
       </c>
       <c r="E53" s="53"/>
       <c r="F53" s="66"/>
@@ -43255,10 +43335,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C54" s="40" t="s">
-        <v>2608</v>
+        <v>2622</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E54" s="40"/>
       <c r="F54" s="64"/>
@@ -43273,13 +43353,13 @@
         <v>wp.pl</v>
       </c>
       <c r="C55" s="53" t="s">
-        <v>2539</v>
+        <v>2553</v>
       </c>
       <c r="D55" s="53" t="s">
-        <v>2584</v>
+        <v>2598</v>
       </c>
       <c r="E55" s="53" t="s">
-        <v>2601</v>
+        <v>2615</v>
       </c>
       <c r="F55" s="66"/>
       <c r="G55" s="67"/>
@@ -43293,10 +43373,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C56" s="40" t="s">
-        <v>2609</v>
+        <v>2623</v>
       </c>
       <c r="D56" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E56" s="40"/>
       <c r="F56" s="64"/>
@@ -43311,13 +43391,13 @@
         <v>wp.pl</v>
       </c>
       <c r="C57" s="53" t="s">
-        <v>2517</v>
+        <v>2531</v>
       </c>
       <c r="D57" s="53" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E57" s="53" t="s">
-        <v>2610</v>
+        <v>2624</v>
       </c>
       <c r="F57" s="66"/>
       <c r="G57" s="67"/>
@@ -43331,10 +43411,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C58" s="40" t="s">
-        <v>2542</v>
+        <v>2556</v>
       </c>
       <c r="D58" s="40" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E58" s="40"/>
       <c r="F58" s="64"/>
@@ -43349,10 +43429,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C59" s="53" t="s">
-        <v>2611</v>
+        <v>2625</v>
       </c>
       <c r="D59" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E59" s="53"/>
       <c r="F59" s="66"/>
@@ -43367,10 +43447,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C60" s="40" t="s">
-        <v>2512</v>
+        <v>2526</v>
       </c>
       <c r="D60" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E60" s="40"/>
       <c r="F60" s="64"/>
@@ -43385,10 +43465,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C61" s="53" t="s">
-        <v>2612</v>
+        <v>2626</v>
       </c>
       <c r="D61" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E61" s="53"/>
       <c r="F61" s="66"/>
@@ -43403,10 +43483,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C62" s="40" t="s">
-        <v>2613</v>
+        <v>2627</v>
       </c>
       <c r="D62" s="40" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E62" s="40"/>
       <c r="F62" s="64"/>
@@ -43421,10 +43501,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C63" s="72" t="s">
-        <v>2614</v>
+        <v>2628</v>
       </c>
       <c r="D63" s="53" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E63" s="53"/>
       <c r="F63" s="66"/>
@@ -43439,10 +43519,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C64" s="40" t="s">
-        <v>2615</v>
+        <v>2629</v>
       </c>
       <c r="D64" s="40" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E64" s="40"/>
       <c r="F64" s="64"/>
@@ -43457,10 +43537,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C65" s="53" t="s">
-        <v>2475</v>
+        <v>2489</v>
       </c>
       <c r="D65" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E65" s="53"/>
       <c r="F65" s="66"/>
@@ -43475,10 +43555,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C66" s="40" t="s">
-        <v>2616</v>
+        <v>2630</v>
       </c>
       <c r="D66" s="40" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E66" s="40"/>
       <c r="F66" s="64"/>
@@ -43493,10 +43573,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C67" s="53" t="s">
-        <v>2537</v>
+        <v>2551</v>
       </c>
       <c r="D67" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E67" s="53"/>
       <c r="F67" s="66"/>
@@ -43511,10 +43591,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C68" s="40" t="s">
-        <v>2508</v>
+        <v>2522</v>
       </c>
       <c r="D68" s="40" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E68" s="40"/>
       <c r="F68" s="64"/>
@@ -43529,10 +43609,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C69" s="53" t="s">
-        <v>2617</v>
+        <v>2631</v>
       </c>
       <c r="D69" s="53" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E69" s="53"/>
       <c r="F69" s="66"/>
@@ -43547,13 +43627,13 @@
         <v>wp.pl</v>
       </c>
       <c r="C70" s="40" t="s">
-        <v>2532</v>
+        <v>2546</v>
       </c>
       <c r="D70" s="40" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E70" s="40" t="s">
-        <v>2618</v>
+        <v>2632</v>
       </c>
       <c r="F70" s="64"/>
       <c r="G70" s="65"/>
@@ -43567,10 +43647,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C71" s="53" t="s">
-        <v>2543</v>
+        <v>2557</v>
       </c>
       <c r="D71" s="53" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E71" s="53"/>
       <c r="F71" s="66"/>
@@ -43585,10 +43665,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C72" s="40" t="s">
-        <v>2551</v>
+        <v>2565</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E72" s="40"/>
       <c r="F72" s="64"/>
@@ -43603,10 +43683,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C73" s="53" t="s">
-        <v>2619</v>
+        <v>2633</v>
       </c>
       <c r="D73" s="53" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E73" s="53"/>
       <c r="F73" s="66"/>
@@ -43621,10 +43701,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C74" s="40" t="s">
-        <v>2544</v>
+        <v>2558</v>
       </c>
       <c r="D74" s="40" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E74" s="40"/>
       <c r="F74" s="64"/>
@@ -43639,10 +43719,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C75" s="53" t="s">
-        <v>2501</v>
+        <v>2515</v>
       </c>
       <c r="D75" s="53" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E75" s="53"/>
       <c r="F75" s="66"/>
@@ -43657,10 +43737,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C76" s="40" t="s">
-        <v>2541</v>
+        <v>2555</v>
       </c>
       <c r="D76" s="40" t="s">
-        <v>2566</v>
+        <v>2580</v>
       </c>
       <c r="E76" s="40"/>
       <c r="F76" s="64"/>
@@ -43675,10 +43755,10 @@
         <v>wp.pl</v>
       </c>
       <c r="C77" s="73" t="s">
-        <v>2620</v>
+        <v>2634</v>
       </c>
       <c r="D77" s="73" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E77" s="73"/>
       <c r="F77" s="74"/>
@@ -43690,10 +43770,10 @@
       </c>
       <c r="B78" s="40"/>
       <c r="C78" s="40" t="s">
-        <v>2523</v>
+        <v>2537</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E78" s="40"/>
       <c r="F78" s="64"/>
@@ -43705,10 +43785,10 @@
       </c>
       <c r="B79" s="53"/>
       <c r="C79" s="53" t="s">
-        <v>2621</v>
+        <v>2635</v>
       </c>
       <c r="D79" s="53" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E79" s="53"/>
       <c r="F79" s="66"/>
@@ -43720,10 +43800,10 @@
       </c>
       <c r="B80" s="40"/>
       <c r="C80" s="40" t="s">
-        <v>2622</v>
+        <v>2636</v>
       </c>
       <c r="D80" s="40" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E80" s="40"/>
       <c r="F80" s="64"/>
@@ -43735,10 +43815,10 @@
       </c>
       <c r="B81" s="53"/>
       <c r="C81" s="53" t="s">
-        <v>2570</v>
+        <v>2584</v>
       </c>
       <c r="D81" s="53" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E81" s="53"/>
       <c r="F81" s="66"/>
@@ -43750,10 +43830,10 @@
       </c>
       <c r="B82" s="40"/>
       <c r="C82" s="40" t="s">
-        <v>2623</v>
+        <v>2637</v>
       </c>
       <c r="D82" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E82" s="40"/>
       <c r="F82" s="64"/>
@@ -43765,13 +43845,13 @@
       </c>
       <c r="B83" s="53"/>
       <c r="C83" s="53" t="s">
-        <v>2624</v>
+        <v>2638</v>
       </c>
       <c r="D83" s="53" t="s">
-        <v>2573</v>
+        <v>2587</v>
       </c>
       <c r="E83" s="53" t="s">
-        <v>2625</v>
+        <v>2639</v>
       </c>
       <c r="F83" s="66"/>
       <c r="G83" s="67"/>
@@ -43782,10 +43862,10 @@
       </c>
       <c r="B84" s="53"/>
       <c r="C84" s="40" t="s">
-        <v>2626</v>
+        <v>2640</v>
       </c>
       <c r="D84" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E84" s="40"/>
       <c r="F84" s="64"/>
@@ -43797,13 +43877,13 @@
       </c>
       <c r="B85" s="53"/>
       <c r="C85" s="53" t="s">
-        <v>2627</v>
+        <v>2641</v>
       </c>
       <c r="D85" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E85" s="53" t="s">
-        <v>2625</v>
+        <v>2639</v>
       </c>
       <c r="F85" s="66"/>
       <c r="G85" s="67"/>
@@ -43814,10 +43894,10 @@
       </c>
       <c r="B86" s="53"/>
       <c r="C86" s="40" t="s">
-        <v>2628</v>
+        <v>2642</v>
       </c>
       <c r="D86" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E86" s="40"/>
       <c r="F86" s="64"/>
@@ -43829,10 +43909,10 @@
       </c>
       <c r="B87" s="53"/>
       <c r="C87" s="53" t="s">
-        <v>2629</v>
+        <v>2643</v>
       </c>
       <c r="D87" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E87" s="53"/>
       <c r="F87" s="66"/>
@@ -43844,10 +43924,10 @@
       </c>
       <c r="B88" s="53"/>
       <c r="C88" s="53" t="s">
-        <v>2630</v>
+        <v>2644</v>
       </c>
       <c r="D88" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E88" s="53"/>
       <c r="F88" s="64"/>
@@ -43859,10 +43939,10 @@
       </c>
       <c r="B89" s="53"/>
       <c r="C89" s="40" t="s">
-        <v>2631</v>
+        <v>2645</v>
       </c>
       <c r="D89" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E89" s="40"/>
       <c r="F89" s="66"/>
@@ -43874,10 +43954,10 @@
       </c>
       <c r="B90" s="53"/>
       <c r="C90" s="40" t="s">
-        <v>2632</v>
+        <v>2646</v>
       </c>
       <c r="D90" s="40" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E90" s="40"/>
       <c r="F90" s="64"/>
@@ -43889,10 +43969,10 @@
       </c>
       <c r="B91" s="53"/>
       <c r="C91" s="53" t="s">
-        <v>2547</v>
+        <v>2561</v>
       </c>
       <c r="D91" s="53" t="s">
-        <v>2557</v>
+        <v>2571</v>
       </c>
       <c r="E91" s="53"/>
       <c r="F91" s="66"/>
@@ -44010,7 +44090,7 @@
       <c r="A102" s="76"/>
       <c r="B102" s="77"/>
       <c r="C102" s="78" t="s">
-        <v>2633</v>
+        <v>2647</v>
       </c>
       <c r="D102" s="79" t="n">
         <f aca="false">(COUNTIF(D2:D101,"OK")+COUNTIF(D2:D101,"NO ADS BY DEFAULT"))/COUNTIF(D2:D101,"*")</f>
@@ -44018,7 +44098,7 @@
       </c>
       <c r="E102" s="80"/>
       <c r="F102" s="78" t="s">
-        <v>2634</v>
+        <v>2648</v>
       </c>
       <c r="G102" s="79" t="n">
         <f aca="false">(COUNTIF(D2:D101,"ADVERT")+COUNTIF(D2:D101,"Anti-adblock"))/COUNTIF(D2:D101,"*")</f>

</xml_diff>